<commit_message>
Economy rework - Europe finished
</commit_message>
<xml_diff>
--- a/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
+++ b/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\economy spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CE2B77-99CD-4978-9984-61E788091760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1904943-E2F7-4FBE-BB51-247328DE03E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C93B8E2A-6318-41E2-B454-20DC41C43396}"/>
   </bookViews>
@@ -22,10 +22,6 @@
     <sheet name="Support Data" sheetId="9" r:id="rId7"/>
     <sheet name="Building slots" sheetId="10" r:id="rId8"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Building slots'!$C$3:$C$21</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Building slots'!$D$3:$D$21</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2380,20 +2376,12 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2410,11 +2398,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2434,7 +2431,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -8444,246 +8440,246 @@
   <sheetData>
     <row r="1" spans="2:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:70" x14ac:dyDescent="0.25">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="63" t="s">
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="63" t="s">
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="63" t="s">
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="63" t="s">
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="64"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="63" t="s">
+      <c r="T2" s="72"/>
+      <c r="U2" s="72"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="63" t="s">
+      <c r="X2" s="72"/>
+      <c r="Y2" s="72"/>
+      <c r="Z2" s="73"/>
+      <c r="AA2" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="64"/>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="63" t="s">
+      <c r="AB2" s="72"/>
+      <c r="AC2" s="72"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="64"/>
-      <c r="AG2" s="64"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="63" t="s">
+      <c r="AF2" s="72"/>
+      <c r="AG2" s="72"/>
+      <c r="AH2" s="73"/>
+      <c r="AI2" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="AJ2" s="64"/>
-      <c r="AK2" s="64"/>
-      <c r="AL2" s="65"/>
-      <c r="AM2" s="63" t="s">
+      <c r="AJ2" s="72"/>
+      <c r="AK2" s="72"/>
+      <c r="AL2" s="73"/>
+      <c r="AM2" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="AN2" s="64"/>
-      <c r="AO2" s="64"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="63" t="s">
+      <c r="AN2" s="72"/>
+      <c r="AO2" s="72"/>
+      <c r="AP2" s="73"/>
+      <c r="AQ2" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="AR2" s="64"/>
-      <c r="AS2" s="64"/>
-      <c r="AT2" s="65"/>
-      <c r="AU2" s="63" t="s">
+      <c r="AR2" s="72"/>
+      <c r="AS2" s="72"/>
+      <c r="AT2" s="73"/>
+      <c r="AU2" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="AV2" s="64"/>
-      <c r="AW2" s="64"/>
-      <c r="AX2" s="65"/>
-      <c r="AY2" s="63" t="s">
+      <c r="AV2" s="72"/>
+      <c r="AW2" s="72"/>
+      <c r="AX2" s="73"/>
+      <c r="AY2" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="AZ2" s="64"/>
-      <c r="BA2" s="64"/>
-      <c r="BB2" s="65"/>
-      <c r="BC2" s="63" t="s">
+      <c r="AZ2" s="72"/>
+      <c r="BA2" s="72"/>
+      <c r="BB2" s="73"/>
+      <c r="BC2" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="BD2" s="64"/>
-      <c r="BE2" s="64"/>
-      <c r="BF2" s="65"/>
-      <c r="BG2" s="63" t="s">
+      <c r="BD2" s="72"/>
+      <c r="BE2" s="72"/>
+      <c r="BF2" s="73"/>
+      <c r="BG2" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="BH2" s="64"/>
-      <c r="BI2" s="64"/>
-      <c r="BJ2" s="65"/>
-      <c r="BK2" s="63" t="s">
+      <c r="BH2" s="72"/>
+      <c r="BI2" s="72"/>
+      <c r="BJ2" s="73"/>
+      <c r="BK2" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="BL2" s="64"/>
-      <c r="BM2" s="64"/>
-      <c r="BN2" s="65"/>
-      <c r="BO2" s="63" t="s">
+      <c r="BL2" s="72"/>
+      <c r="BM2" s="72"/>
+      <c r="BN2" s="73"/>
+      <c r="BO2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="BP2" s="64"/>
-      <c r="BQ2" s="64"/>
-      <c r="BR2" s="65"/>
+      <c r="BP2" s="72"/>
+      <c r="BQ2" s="72"/>
+      <c r="BR2" s="73"/>
     </row>
     <row r="3" spans="2:70" x14ac:dyDescent="0.25">
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67" t="s">
+      <c r="D3" s="65"/>
+      <c r="E3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="68"/>
-      <c r="G3" s="66" t="s">
+      <c r="F3" s="66"/>
+      <c r="G3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67" t="s">
+      <c r="H3" s="65"/>
+      <c r="I3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="68"/>
-      <c r="K3" s="66" t="s">
+      <c r="J3" s="66"/>
+      <c r="K3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67" t="s">
+      <c r="L3" s="65"/>
+      <c r="M3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="68"/>
-      <c r="O3" s="66" t="s">
+      <c r="N3" s="66"/>
+      <c r="O3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67" t="s">
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="68"/>
-      <c r="S3" s="66" t="s">
+      <c r="R3" s="66"/>
+      <c r="S3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67" t="s">
+      <c r="T3" s="65"/>
+      <c r="U3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="68"/>
-      <c r="W3" s="66" t="s">
+      <c r="V3" s="66"/>
+      <c r="W3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="67"/>
-      <c r="Y3" s="67" t="s">
+      <c r="X3" s="65"/>
+      <c r="Y3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="68"/>
-      <c r="AA3" s="66" t="s">
+      <c r="Z3" s="66"/>
+      <c r="AA3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="67"/>
-      <c r="AC3" s="67" t="s">
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="66" t="s">
+      <c r="AD3" s="66"/>
+      <c r="AE3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="67" t="s">
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AH3" s="68"/>
-      <c r="AI3" s="66" t="s">
+      <c r="AH3" s="66"/>
+      <c r="AI3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AJ3" s="67"/>
-      <c r="AK3" s="67" t="s">
+      <c r="AJ3" s="65"/>
+      <c r="AK3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AL3" s="68"/>
-      <c r="AM3" s="66" t="s">
+      <c r="AL3" s="66"/>
+      <c r="AM3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AN3" s="67"/>
-      <c r="AO3" s="67" t="s">
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AP3" s="68"/>
-      <c r="AQ3" s="66" t="s">
+      <c r="AP3" s="66"/>
+      <c r="AQ3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AR3" s="67"/>
-      <c r="AS3" s="67" t="s">
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AT3" s="68"/>
-      <c r="AU3" s="66" t="s">
+      <c r="AT3" s="66"/>
+      <c r="AU3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AV3" s="67"/>
-      <c r="AW3" s="67" t="s">
+      <c r="AV3" s="65"/>
+      <c r="AW3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AX3" s="68"/>
-      <c r="AY3" s="66" t="s">
+      <c r="AX3" s="66"/>
+      <c r="AY3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AZ3" s="67"/>
-      <c r="BA3" s="67" t="s">
+      <c r="AZ3" s="65"/>
+      <c r="BA3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="BB3" s="68"/>
-      <c r="BC3" s="66" t="s">
+      <c r="BB3" s="66"/>
+      <c r="BC3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="BD3" s="67"/>
-      <c r="BE3" s="67" t="s">
+      <c r="BD3" s="65"/>
+      <c r="BE3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="BF3" s="68"/>
-      <c r="BG3" s="66" t="s">
+      <c r="BF3" s="66"/>
+      <c r="BG3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="BH3" s="67"/>
-      <c r="BI3" s="67" t="s">
+      <c r="BH3" s="65"/>
+      <c r="BI3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="BJ3" s="68"/>
-      <c r="BK3" s="66" t="s">
+      <c r="BJ3" s="66"/>
+      <c r="BK3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="BL3" s="67"/>
-      <c r="BM3" s="67" t="s">
+      <c r="BL3" s="65"/>
+      <c r="BM3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="BN3" s="68"/>
-      <c r="BO3" s="66" t="s">
+      <c r="BN3" s="66"/>
+      <c r="BO3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="BP3" s="67"/>
-      <c r="BQ3" s="67" t="s">
+      <c r="BP3" s="65"/>
+      <c r="BQ3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="BR3" s="68"/>
+      <c r="BR3" s="66"/>
     </row>
     <row r="4" spans="2:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
@@ -8895,10 +8891,10 @@
       <c r="B5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="69">
+      <c r="C5" s="67">
         <v>1</v>
       </c>
-      <c r="D5" s="70"/>
+      <c r="D5" s="68"/>
       <c r="E5" s="22">
         <v>2.9780000000000002</v>
       </c>
@@ -8906,10 +8902,10 @@
         <f>E5/C5-1</f>
         <v>1.9780000000000002</v>
       </c>
-      <c r="G5" s="69">
+      <c r="G5" s="67">
         <v>1</v>
       </c>
-      <c r="H5" s="70"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="22">
         <v>1.84</v>
       </c>
@@ -8917,10 +8913,10 @@
         <f>I5/G5-1</f>
         <v>0.84000000000000008</v>
       </c>
-      <c r="K5" s="69">
+      <c r="K5" s="67">
         <v>1</v>
       </c>
-      <c r="L5" s="70"/>
+      <c r="L5" s="68"/>
       <c r="M5" s="22">
         <v>2.2770000000000001</v>
       </c>
@@ -8928,10 +8924,10 @@
         <f>M5/K5-1</f>
         <v>1.2770000000000001</v>
       </c>
-      <c r="O5" s="69">
+      <c r="O5" s="67">
         <v>1</v>
       </c>
-      <c r="P5" s="70"/>
+      <c r="P5" s="68"/>
       <c r="Q5" s="22">
         <v>2.8029999999999999</v>
       </c>
@@ -8939,10 +8935,10 @@
         <f>Q5/O5-1</f>
         <v>1.8029999999999999</v>
       </c>
-      <c r="S5" s="73">
+      <c r="S5" s="74">
         <v>2</v>
       </c>
-      <c r="T5" s="70"/>
+      <c r="T5" s="68"/>
       <c r="U5" s="22">
         <v>12.585000000000001</v>
       </c>
@@ -8950,10 +8946,10 @@
         <f>U5/S5-1</f>
         <v>5.2925000000000004</v>
       </c>
-      <c r="W5" s="69">
+      <c r="W5" s="67">
         <v>2</v>
       </c>
-      <c r="X5" s="70"/>
+      <c r="X5" s="68"/>
       <c r="Y5" s="22">
         <v>10.067</v>
       </c>
@@ -8961,10 +8957,10 @@
         <f>Y5/W5-1</f>
         <v>4.0335000000000001</v>
       </c>
-      <c r="AA5" s="69">
+      <c r="AA5" s="67">
         <v>2</v>
       </c>
-      <c r="AB5" s="70"/>
+      <c r="AB5" s="68"/>
       <c r="AC5" s="22">
         <v>9.9779999999999998</v>
       </c>
@@ -8972,10 +8968,10 @@
         <f>AC5/AA5-1</f>
         <v>3.9889999999999999</v>
       </c>
-      <c r="AE5" s="69">
+      <c r="AE5" s="67">
         <v>7</v>
       </c>
-      <c r="AF5" s="70"/>
+      <c r="AF5" s="68"/>
       <c r="AG5" s="22">
         <v>15.536</v>
       </c>
@@ -8983,10 +8979,10 @@
         <f>AG5/AE5-1</f>
         <v>1.2194285714285713</v>
       </c>
-      <c r="AI5" s="69">
+      <c r="AI5" s="67">
         <v>7</v>
       </c>
-      <c r="AJ5" s="70"/>
+      <c r="AJ5" s="68"/>
       <c r="AK5" s="22">
         <v>24.87</v>
       </c>
@@ -8994,10 +8990,10 @@
         <f>AK5/AI5-1</f>
         <v>2.5528571428571429</v>
       </c>
-      <c r="AM5" s="69">
+      <c r="AM5" s="67">
         <v>7</v>
       </c>
-      <c r="AN5" s="70"/>
+      <c r="AN5" s="68"/>
       <c r="AO5" s="22">
         <v>14.685</v>
       </c>
@@ -9005,10 +9001,10 @@
         <f>AO5/AM5-1</f>
         <v>1.0978571428571429</v>
       </c>
-      <c r="AQ5" s="69">
+      <c r="AQ5" s="67">
         <v>10</v>
       </c>
-      <c r="AR5" s="70"/>
+      <c r="AR5" s="68"/>
       <c r="AS5" s="22">
         <v>13.314</v>
       </c>
@@ -9016,10 +9012,10 @@
         <f>AS5/AQ5-1</f>
         <v>0.33139999999999992</v>
       </c>
-      <c r="AU5" s="69">
+      <c r="AU5" s="67">
         <v>15</v>
       </c>
-      <c r="AV5" s="70"/>
+      <c r="AV5" s="68"/>
       <c r="AW5" s="22">
         <v>35.488</v>
       </c>
@@ -9027,10 +9023,10 @@
         <f>AW5/AU5-1</f>
         <v>1.3658666666666668</v>
       </c>
-      <c r="AY5" s="69">
+      <c r="AY5" s="67">
         <v>20</v>
       </c>
-      <c r="AZ5" s="70"/>
+      <c r="AZ5" s="68"/>
       <c r="BA5" s="22">
         <v>46.418999999999997</v>
       </c>
@@ -9038,10 +9034,10 @@
         <f>BA5/AY5-1</f>
         <v>1.3209499999999998</v>
       </c>
-      <c r="BC5" s="69">
+      <c r="BC5" s="67">
         <v>20</v>
       </c>
-      <c r="BD5" s="70"/>
+      <c r="BD5" s="68"/>
       <c r="BE5" s="22">
         <v>77.132000000000005</v>
       </c>
@@ -9049,10 +9045,10 @@
         <f>BE5/BC5-1</f>
         <v>2.8566000000000003</v>
       </c>
-      <c r="BG5" s="69">
+      <c r="BG5" s="67">
         <v>20</v>
       </c>
-      <c r="BH5" s="70"/>
+      <c r="BH5" s="68"/>
       <c r="BI5" s="22">
         <v>50.906999999999996</v>
       </c>
@@ -9060,10 +9056,10 @@
         <f>BI5/BG5-1</f>
         <v>1.54535</v>
       </c>
-      <c r="BK5" s="69">
+      <c r="BK5" s="67">
         <v>30</v>
       </c>
-      <c r="BL5" s="70"/>
+      <c r="BL5" s="68"/>
       <c r="BM5" s="22">
         <v>39.054000000000002</v>
       </c>
@@ -9071,10 +9067,10 @@
         <f>BM5/BK5-1</f>
         <v>0.30180000000000007</v>
       </c>
-      <c r="BO5" s="69">
+      <c r="BO5" s="67">
         <v>30</v>
       </c>
-      <c r="BP5" s="70"/>
+      <c r="BP5" s="68"/>
       <c r="BQ5" s="22">
         <v>40.4</v>
       </c>
@@ -9087,138 +9083,138 @@
       <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="71">
+      <c r="C6" s="62">
         <v>11</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="63"/>
       <c r="E6" s="23">
         <v>10</v>
       </c>
       <c r="F6" s="26"/>
-      <c r="G6" s="71">
+      <c r="G6" s="62">
         <v>17</v>
       </c>
-      <c r="H6" s="72"/>
+      <c r="H6" s="63"/>
       <c r="I6" s="23">
         <v>30</v>
       </c>
       <c r="J6" s="26"/>
-      <c r="K6" s="71">
+      <c r="K6" s="62">
         <v>10</v>
       </c>
-      <c r="L6" s="72"/>
+      <c r="L6" s="63"/>
       <c r="M6" s="23">
         <v>18</v>
       </c>
       <c r="N6" s="26"/>
-      <c r="O6" s="71">
+      <c r="O6" s="62">
         <v>18</v>
       </c>
-      <c r="P6" s="72"/>
+      <c r="P6" s="63"/>
       <c r="Q6" s="23">
         <v>22</v>
       </c>
       <c r="R6" s="26"/>
-      <c r="S6" s="74">
+      <c r="S6" s="75">
         <v>40</v>
       </c>
-      <c r="T6" s="72"/>
+      <c r="T6" s="63"/>
       <c r="U6" s="23">
         <v>37</v>
       </c>
       <c r="V6" s="26"/>
-      <c r="W6" s="71">
+      <c r="W6" s="62">
         <v>18</v>
       </c>
-      <c r="X6" s="72"/>
+      <c r="X6" s="63"/>
       <c r="Y6" s="23">
         <v>18</v>
       </c>
       <c r="Z6" s="26"/>
-      <c r="AA6" s="71">
+      <c r="AA6" s="62">
         <v>18</v>
       </c>
-      <c r="AB6" s="72"/>
+      <c r="AB6" s="63"/>
       <c r="AC6" s="23">
         <v>20</v>
       </c>
       <c r="AD6" s="26"/>
-      <c r="AE6" s="71">
+      <c r="AE6" s="62">
         <v>14</v>
       </c>
-      <c r="AF6" s="72"/>
+      <c r="AF6" s="63"/>
       <c r="AG6" s="23">
         <v>19</v>
       </c>
       <c r="AH6" s="26"/>
-      <c r="AI6" s="71">
+      <c r="AI6" s="62">
         <v>23</v>
       </c>
-      <c r="AJ6" s="72"/>
+      <c r="AJ6" s="63"/>
       <c r="AK6" s="23">
         <v>21</v>
       </c>
       <c r="AL6" s="26"/>
-      <c r="AM6" s="71">
+      <c r="AM6" s="62">
         <v>7</v>
       </c>
-      <c r="AN6" s="72"/>
+      <c r="AN6" s="63"/>
       <c r="AO6" s="23">
         <v>9</v>
       </c>
       <c r="AP6" s="26"/>
-      <c r="AQ6" s="71">
+      <c r="AQ6" s="62">
         <v>14</v>
       </c>
-      <c r="AR6" s="72"/>
+      <c r="AR6" s="63"/>
       <c r="AS6" s="23">
         <v>22</v>
       </c>
       <c r="AT6" s="26"/>
-      <c r="AU6" s="71">
+      <c r="AU6" s="62">
         <v>12</v>
       </c>
-      <c r="AV6" s="72"/>
+      <c r="AV6" s="63"/>
       <c r="AW6" s="23">
         <v>40</v>
       </c>
       <c r="AX6" s="26"/>
-      <c r="AY6" s="71">
+      <c r="AY6" s="62">
         <v>37</v>
       </c>
-      <c r="AZ6" s="72"/>
+      <c r="AZ6" s="63"/>
       <c r="BA6" s="23">
         <v>44</v>
       </c>
       <c r="BB6" s="26"/>
-      <c r="BC6" s="71">
+      <c r="BC6" s="62">
         <v>30</v>
       </c>
-      <c r="BD6" s="72"/>
+      <c r="BD6" s="63"/>
       <c r="BE6" s="23">
         <v>58</v>
       </c>
       <c r="BF6" s="26"/>
-      <c r="BG6" s="71">
+      <c r="BG6" s="62">
         <v>23</v>
       </c>
-      <c r="BH6" s="72"/>
+      <c r="BH6" s="63"/>
       <c r="BI6" s="23">
         <v>47</v>
       </c>
       <c r="BJ6" s="26"/>
-      <c r="BK6" s="71">
+      <c r="BK6" s="62">
         <v>37</v>
       </c>
-      <c r="BL6" s="72"/>
+      <c r="BL6" s="63"/>
       <c r="BM6" s="23">
         <v>40</v>
       </c>
       <c r="BN6" s="26"/>
-      <c r="BO6" s="71">
+      <c r="BO6" s="62">
         <v>36</v>
       </c>
-      <c r="BP6" s="72"/>
+      <c r="BP6" s="63"/>
       <c r="BQ6" s="23">
         <v>23</v>
       </c>
@@ -9228,104 +9224,104 @@
       <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="72"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="63"/>
       <c r="E7" s="23">
         <v>18</v>
       </c>
       <c r="F7" s="26"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="72"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="63"/>
       <c r="I7" s="23">
         <v>30</v>
       </c>
       <c r="J7" s="26"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="72"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="63"/>
       <c r="M7" s="23">
         <v>32</v>
       </c>
       <c r="N7" s="26"/>
-      <c r="O7" s="71"/>
-      <c r="P7" s="72"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="63"/>
       <c r="Q7" s="23">
         <v>18</v>
       </c>
       <c r="R7" s="26"/>
-      <c r="S7" s="74"/>
-      <c r="T7" s="72"/>
+      <c r="S7" s="75"/>
+      <c r="T7" s="63"/>
       <c r="U7" s="23">
         <v>22</v>
       </c>
       <c r="V7" s="26"/>
-      <c r="W7" s="71"/>
-      <c r="X7" s="72"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="63"/>
       <c r="Y7" s="23">
         <v>22</v>
       </c>
       <c r="Z7" s="26"/>
-      <c r="AA7" s="71"/>
-      <c r="AB7" s="72"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="63"/>
       <c r="AC7" s="23">
         <v>10</v>
       </c>
       <c r="AD7" s="26"/>
-      <c r="AE7" s="71"/>
-      <c r="AF7" s="72"/>
+      <c r="AE7" s="62"/>
+      <c r="AF7" s="63"/>
       <c r="AG7" s="23">
         <v>43</v>
       </c>
       <c r="AH7" s="26"/>
-      <c r="AI7" s="71"/>
-      <c r="AJ7" s="72"/>
+      <c r="AI7" s="62"/>
+      <c r="AJ7" s="63"/>
       <c r="AK7" s="23">
         <v>27</v>
       </c>
       <c r="AL7" s="26"/>
-      <c r="AM7" s="71"/>
-      <c r="AN7" s="72"/>
+      <c r="AM7" s="62"/>
+      <c r="AN7" s="63"/>
       <c r="AO7" s="23">
         <v>6</v>
       </c>
       <c r="AP7" s="26"/>
-      <c r="AQ7" s="71"/>
-      <c r="AR7" s="72"/>
+      <c r="AQ7" s="62"/>
+      <c r="AR7" s="63"/>
       <c r="AS7" s="23">
         <v>15</v>
       </c>
       <c r="AT7" s="26"/>
-      <c r="AU7" s="71"/>
-      <c r="AV7" s="72"/>
+      <c r="AU7" s="62"/>
+      <c r="AV7" s="63"/>
       <c r="AW7" s="23">
         <v>25</v>
       </c>
       <c r="AX7" s="26"/>
-      <c r="AY7" s="71"/>
-      <c r="AZ7" s="72"/>
+      <c r="AY7" s="62"/>
+      <c r="AZ7" s="63"/>
       <c r="BA7" s="23">
         <v>18</v>
       </c>
       <c r="BB7" s="26"/>
-      <c r="BC7" s="71"/>
-      <c r="BD7" s="72"/>
+      <c r="BC7" s="62"/>
+      <c r="BD7" s="63"/>
       <c r="BE7" s="23">
         <v>26</v>
       </c>
       <c r="BF7" s="26"/>
-      <c r="BG7" s="71"/>
-      <c r="BH7" s="72"/>
+      <c r="BG7" s="62"/>
+      <c r="BH7" s="63"/>
       <c r="BI7" s="23">
         <v>36</v>
       </c>
       <c r="BJ7" s="26"/>
-      <c r="BK7" s="71"/>
-      <c r="BL7" s="72"/>
+      <c r="BK7" s="62"/>
+      <c r="BL7" s="63"/>
       <c r="BM7" s="23">
         <v>23</v>
       </c>
       <c r="BN7" s="26"/>
-      <c r="BO7" s="71"/>
-      <c r="BP7" s="72"/>
+      <c r="BO7" s="62"/>
+      <c r="BP7" s="63"/>
       <c r="BQ7" s="23">
         <v>33</v>
       </c>
@@ -9335,11 +9331,11 @@
       <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="61">
+      <c r="C8" s="69">
         <f>C6</f>
         <v>11</v>
       </c>
-      <c r="D8" s="62"/>
+      <c r="D8" s="70"/>
       <c r="E8" s="24">
         <f>(E6+E7)/2</f>
         <v>14</v>
@@ -9348,11 +9344,11 @@
         <f>E8/C8-1</f>
         <v>0.27272727272727271</v>
       </c>
-      <c r="G8" s="61">
+      <c r="G8" s="69">
         <f>G6</f>
         <v>17</v>
       </c>
-      <c r="H8" s="62"/>
+      <c r="H8" s="70"/>
       <c r="I8" s="24">
         <f>(I6+I7)/2</f>
         <v>30</v>
@@ -9361,11 +9357,11 @@
         <f>I8/G8-1</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="K8" s="61">
+      <c r="K8" s="69">
         <f>K6</f>
         <v>10</v>
       </c>
-      <c r="L8" s="62"/>
+      <c r="L8" s="70"/>
       <c r="M8" s="24">
         <f>(M6+M7)/2</f>
         <v>25</v>
@@ -9374,11 +9370,11 @@
         <f>M8/K8-1</f>
         <v>1.5</v>
       </c>
-      <c r="O8" s="61">
+      <c r="O8" s="69">
         <f>O6</f>
         <v>18</v>
       </c>
-      <c r="P8" s="62"/>
+      <c r="P8" s="70"/>
       <c r="Q8" s="24">
         <f>(Q6+Q7)/2</f>
         <v>20</v>
@@ -9387,11 +9383,11 @@
         <f>Q8/O8-1</f>
         <v>0.11111111111111116</v>
       </c>
-      <c r="S8" s="75">
+      <c r="S8" s="76">
         <f>S6</f>
         <v>40</v>
       </c>
-      <c r="T8" s="62"/>
+      <c r="T8" s="70"/>
       <c r="U8" s="24">
         <f>(U6+U7)/2</f>
         <v>29.5</v>
@@ -9400,11 +9396,11 @@
         <f>U8/S8-1</f>
         <v>-0.26249999999999996</v>
       </c>
-      <c r="W8" s="61">
+      <c r="W8" s="69">
         <f>W6</f>
         <v>18</v>
       </c>
-      <c r="X8" s="62"/>
+      <c r="X8" s="70"/>
       <c r="Y8" s="24">
         <f>(Y6+Y7)/2</f>
         <v>20</v>
@@ -9413,11 +9409,11 @@
         <f>Y8/W8-1</f>
         <v>0.11111111111111116</v>
       </c>
-      <c r="AA8" s="61">
+      <c r="AA8" s="69">
         <f>AA6</f>
         <v>18</v>
       </c>
-      <c r="AB8" s="62"/>
+      <c r="AB8" s="70"/>
       <c r="AC8" s="24">
         <f>(AC6+AC7)/2</f>
         <v>15</v>
@@ -9426,11 +9422,11 @@
         <f>AC8/AA8-1</f>
         <v>-0.16666666666666663</v>
       </c>
-      <c r="AE8" s="61">
+      <c r="AE8" s="69">
         <f>AE6</f>
         <v>14</v>
       </c>
-      <c r="AF8" s="62"/>
+      <c r="AF8" s="70"/>
       <c r="AG8" s="24">
         <f>(AG6+AG7)/2</f>
         <v>31</v>
@@ -9439,11 +9435,11 @@
         <f>AG8/AE8-1</f>
         <v>1.2142857142857144</v>
       </c>
-      <c r="AI8" s="61">
+      <c r="AI8" s="69">
         <f>AI6</f>
         <v>23</v>
       </c>
-      <c r="AJ8" s="62"/>
+      <c r="AJ8" s="70"/>
       <c r="AK8" s="24">
         <f>(AK6+AK7)/2</f>
         <v>24</v>
@@ -9452,11 +9448,11 @@
         <f>AK8/AI8-1</f>
         <v>4.3478260869565188E-2</v>
       </c>
-      <c r="AM8" s="61">
+      <c r="AM8" s="69">
         <f>AM6</f>
         <v>7</v>
       </c>
-      <c r="AN8" s="62"/>
+      <c r="AN8" s="70"/>
       <c r="AO8" s="24">
         <f>(AO6+AO7)/2</f>
         <v>7.5</v>
@@ -9465,11 +9461,11 @@
         <f>AO8/AM8-1</f>
         <v>7.1428571428571397E-2</v>
       </c>
-      <c r="AQ8" s="61">
+      <c r="AQ8" s="69">
         <f>AQ6</f>
         <v>14</v>
       </c>
-      <c r="AR8" s="62"/>
+      <c r="AR8" s="70"/>
       <c r="AS8" s="24">
         <f>(AS6+AS7)/2</f>
         <v>18.5</v>
@@ -9478,11 +9474,11 @@
         <f>AS8/AQ8-1</f>
         <v>0.3214285714285714</v>
       </c>
-      <c r="AU8" s="61">
+      <c r="AU8" s="69">
         <f>AU6</f>
         <v>12</v>
       </c>
-      <c r="AV8" s="62"/>
+      <c r="AV8" s="70"/>
       <c r="AW8" s="24">
         <f>(AW6+AW7)/2</f>
         <v>32.5</v>
@@ -9491,11 +9487,11 @@
         <f>AW8/AU8-1</f>
         <v>1.7083333333333335</v>
       </c>
-      <c r="AY8" s="61">
+      <c r="AY8" s="69">
         <f>AY6</f>
         <v>37</v>
       </c>
-      <c r="AZ8" s="62"/>
+      <c r="AZ8" s="70"/>
       <c r="BA8" s="24">
         <f>(BA6+BA7)/2</f>
         <v>31</v>
@@ -9504,11 +9500,11 @@
         <f>BA8/AY8-1</f>
         <v>-0.16216216216216217</v>
       </c>
-      <c r="BC8" s="61">
+      <c r="BC8" s="69">
         <f>BC6</f>
         <v>30</v>
       </c>
-      <c r="BD8" s="62"/>
+      <c r="BD8" s="70"/>
       <c r="BE8" s="24">
         <f>(BE6+BE7)/2</f>
         <v>42</v>
@@ -9517,11 +9513,11 @@
         <f>BE8/BC8-1</f>
         <v>0.39999999999999991</v>
       </c>
-      <c r="BG8" s="61">
+      <c r="BG8" s="69">
         <f>BG6</f>
         <v>23</v>
       </c>
-      <c r="BH8" s="62"/>
+      <c r="BH8" s="70"/>
       <c r="BI8" s="24">
         <f>(BI6+BI7)/2</f>
         <v>41.5</v>
@@ -9530,11 +9526,11 @@
         <f>BI8/BG8-1</f>
         <v>0.80434782608695654</v>
       </c>
-      <c r="BK8" s="61">
+      <c r="BK8" s="69">
         <f>BK6</f>
         <v>37</v>
       </c>
-      <c r="BL8" s="62"/>
+      <c r="BL8" s="70"/>
       <c r="BM8" s="24">
         <f>(BM6+BM7)/2</f>
         <v>31.5</v>
@@ -9543,11 +9539,11 @@
         <f>BM8/BK8-1</f>
         <v>-0.14864864864864868</v>
       </c>
-      <c r="BO8" s="61">
+      <c r="BO8" s="69">
         <f>BO6</f>
         <v>36</v>
       </c>
-      <c r="BP8" s="62"/>
+      <c r="BP8" s="70"/>
       <c r="BQ8" s="24">
         <f>(BQ6+BQ7)/2</f>
         <v>28</v>
@@ -12531,20 +12527,87 @@
     </row>
   </sheetData>
   <mergeCells count="119">
-    <mergeCell ref="BO7:BP7"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AW3:AX3"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AU7:AV7"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="BE3:BF3"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BC7:BD7"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="AY7:AZ7"/>
+    <mergeCell ref="BC8:BD8"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="AM8:AN8"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="AO3:AP3"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AM6:AN6"/>
+    <mergeCell ref="AM7:AN7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="BO8:BP8"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="BO2:BR2"/>
+    <mergeCell ref="BO3:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="AY2:BB2"/>
+    <mergeCell ref="AY3:AZ3"/>
+    <mergeCell ref="BA3:BB3"/>
+    <mergeCell ref="BK2:BN2"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="BM3:BN3"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BK7:BL7"/>
     <mergeCell ref="BK8:BL8"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="AQ3:AR3"/>
@@ -12569,87 +12632,20 @@
     <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="AQ6:AR6"/>
     <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="BO8:BP8"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="BO2:BR2"/>
-    <mergeCell ref="BO3:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BO5:BP5"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="AY2:BB2"/>
-    <mergeCell ref="AY3:AZ3"/>
-    <mergeCell ref="BA3:BB3"/>
-    <mergeCell ref="BK2:BN2"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="BM3:BN3"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BK7:BL7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="AM8:AN8"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AM3:AN3"/>
-    <mergeCell ref="AO3:AP3"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="AM7:AN7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="BC8:BD8"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="BO7:BP7"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AU7:AV7"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="BE3:BF3"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BC7:BD7"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="AY7:AZ7"/>
   </mergeCells>
   <conditionalFormatting sqref="BP21">
     <cfRule type="cellIs" dxfId="63" priority="103" operator="lessThan">
@@ -13099,10 +13095,10 @@
   <dimension ref="B1:AN187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="15" topLeftCell="C112" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="15" topLeftCell="C166" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="B124" sqref="B124"/>
+      <selection pane="bottomRight" activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13487,12 +13483,12 @@
       <c r="AH14" s="39"/>
       <c r="AI14" s="39"/>
       <c r="AJ14" s="39"/>
-      <c r="AK14" s="76" t="s">
+      <c r="AK14" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="AL14" s="77"/>
-      <c r="AM14" s="77"/>
-      <c r="AN14" s="78"/>
+      <c r="AL14" s="78"/>
+      <c r="AM14" s="78"/>
+      <c r="AN14" s="79"/>
     </row>
     <row r="15" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B15" s="35" t="s">
@@ -13756,7 +13752,7 @@
       </c>
     </row>
     <row r="17" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="60" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="35">
@@ -14888,7 +14884,7 @@
       </c>
     </row>
     <row r="25" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="60" t="s">
         <v>73</v>
       </c>
       <c r="C25" s="35">
@@ -15758,7 +15754,7 @@
       </c>
     </row>
     <row r="31" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="60" t="s">
         <v>85</v>
       </c>
       <c r="C31" s="35">
@@ -15903,7 +15899,7 @@
       </c>
     </row>
     <row r="32" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="60" t="s">
         <v>87</v>
       </c>
       <c r="C32" s="35">
@@ -16628,7 +16624,7 @@
       </c>
     </row>
     <row r="37" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="60" t="s">
         <v>99</v>
       </c>
       <c r="C37" s="35">
@@ -17208,7 +17204,7 @@
       </c>
     </row>
     <row r="41" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="60" t="s">
         <v>108</v>
       </c>
       <c r="C41" s="35">
@@ -19673,7 +19669,7 @@
       </c>
     </row>
     <row r="58" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B58" s="35" t="s">
+      <c r="B58" s="60" t="s">
         <v>145</v>
       </c>
       <c r="C58" s="35">
@@ -19818,7 +19814,7 @@
       </c>
     </row>
     <row r="59" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B59" s="35" t="s">
+      <c r="B59" s="60" t="s">
         <v>150</v>
       </c>
       <c r="C59" s="35">
@@ -19963,7 +19959,7 @@
       </c>
     </row>
     <row r="60" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B60" s="35" t="s">
+      <c r="B60" s="60" t="s">
         <v>152</v>
       </c>
       <c r="C60" s="35">
@@ -22573,7 +22569,7 @@
       </c>
     </row>
     <row r="78" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B78" s="35" t="s">
+      <c r="B78" s="60" t="s">
         <v>19</v>
       </c>
       <c r="C78" s="35">
@@ -22863,7 +22859,7 @@
       </c>
     </row>
     <row r="80" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B80" s="35" t="s">
+      <c r="B80" s="60" t="s">
         <v>199</v>
       </c>
       <c r="C80" s="35">
@@ -24023,7 +24019,7 @@
       </c>
     </row>
     <row r="88" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B88" s="35" t="s">
+      <c r="B88" s="60" t="s">
         <v>221</v>
       </c>
       <c r="C88" s="35">
@@ -25183,7 +25179,7 @@
       </c>
     </row>
     <row r="96" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B96" s="35" t="s">
+      <c r="B96" s="60" t="s">
         <v>238</v>
       </c>
       <c r="C96" s="35">
@@ -26343,7 +26339,7 @@
       </c>
     </row>
     <row r="104" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B104" s="35" t="s">
+      <c r="B104" s="60" t="s">
         <v>255</v>
       </c>
       <c r="C104" s="35">
@@ -27648,7 +27644,7 @@
       </c>
     </row>
     <row r="113" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B113" s="35" t="s">
+      <c r="B113" s="60" t="s">
         <v>277</v>
       </c>
       <c r="C113" s="35">
@@ -28518,7 +28514,7 @@
       </c>
     </row>
     <row r="119" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B119" s="35" t="s">
+      <c r="B119" s="60" t="s">
         <v>291</v>
       </c>
       <c r="C119" s="35">
@@ -29388,7 +29384,7 @@
       </c>
     </row>
     <row r="125" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B125" s="35" t="s">
+      <c r="B125" s="60" t="s">
         <v>303</v>
       </c>
       <c r="C125" s="35">
@@ -29678,7 +29674,7 @@
       </c>
     </row>
     <row r="127" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B127" s="35" t="s">
+      <c r="B127" s="60" t="s">
         <v>309</v>
       </c>
       <c r="C127" s="35">
@@ -30548,7 +30544,7 @@
       </c>
     </row>
     <row r="133" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B133" s="35" t="s">
+      <c r="B133" s="60" t="s">
         <v>323</v>
       </c>
       <c r="C133" s="35">
@@ -31273,7 +31269,7 @@
       </c>
     </row>
     <row r="138" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B138" s="35" t="s">
+      <c r="B138" s="60" t="s">
         <v>333</v>
       </c>
       <c r="C138" s="35">
@@ -32723,7 +32719,7 @@
       </c>
     </row>
     <row r="148" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B148" s="35" t="s">
+      <c r="B148" s="60" t="s">
         <v>355</v>
       </c>
       <c r="C148" s="35">
@@ -33158,7 +33154,7 @@
       </c>
     </row>
     <row r="151" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B151" s="35" t="s">
+      <c r="B151" s="60" t="s">
         <v>363</v>
       </c>
       <c r="C151" s="35">
@@ -34028,7 +34024,7 @@
       </c>
     </row>
     <row r="157" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B157" s="35" t="s">
+      <c r="B157" s="60" t="s">
         <v>378</v>
       </c>
       <c r="C157" s="35">
@@ -34608,7 +34604,7 @@
       </c>
     </row>
     <row r="161" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B161" s="35" t="s">
+      <c r="B161" s="60" t="s">
         <v>388</v>
       </c>
       <c r="C161" s="35">
@@ -34753,7 +34749,7 @@
       </c>
     </row>
     <row r="162" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B162" s="35" t="s">
+      <c r="B162" s="60" t="s">
         <v>390</v>
       </c>
       <c r="C162" s="35">
@@ -35768,7 +35764,7 @@
       </c>
     </row>
     <row r="169" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B169" s="35" t="s">
+      <c r="B169" s="60" t="s">
         <v>416</v>
       </c>
       <c r="C169" s="35">
@@ -37363,7 +37359,7 @@
       </c>
     </row>
     <row r="180" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B180" s="35" t="s">
+      <c r="B180" s="60" t="s">
         <v>444</v>
       </c>
       <c r="C180" s="35">
@@ -54702,11 +54698,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" style="79" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="79">
+      <c r="C3" s="61">
         <v>0</v>
       </c>
       <c r="D3">
@@ -54715,7 +54711,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="39"/>
-      <c r="C4" s="79">
+      <c r="C4" s="61">
         <v>300000</v>
       </c>
       <c r="D4">
@@ -54724,7 +54720,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="39"/>
-      <c r="C5" s="79">
+      <c r="C5" s="61">
         <v>800000</v>
       </c>
       <c r="D5">
@@ -54733,7 +54729,7 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="39"/>
-      <c r="C6" s="79">
+      <c r="C6" s="61">
         <v>1500000</v>
       </c>
       <c r="D6" s="39">
@@ -54742,7 +54738,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="39"/>
-      <c r="C7" s="79">
+      <c r="C7" s="61">
         <v>2500000</v>
       </c>
       <c r="D7" s="39">
@@ -54751,7 +54747,7 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="39"/>
-      <c r="C8" s="79">
+      <c r="C8" s="61">
         <v>3800000</v>
       </c>
       <c r="D8" s="39">
@@ -54760,7 +54756,7 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="39"/>
-      <c r="C9" s="79">
+      <c r="C9" s="61">
         <v>5200000</v>
       </c>
       <c r="D9" s="39">
@@ -54769,7 +54765,7 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="39"/>
-      <c r="C10" s="79">
+      <c r="C10" s="61">
         <v>6800000</v>
       </c>
       <c r="D10" s="39">
@@ -54778,7 +54774,7 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="39"/>
-      <c r="C11" s="79">
+      <c r="C11" s="61">
         <v>8500000</v>
       </c>
       <c r="D11" s="39">
@@ -54787,7 +54783,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="39"/>
-      <c r="C12" s="79">
+      <c r="C12" s="61">
         <v>10500000</v>
       </c>
       <c r="D12" s="39">
@@ -54796,7 +54792,7 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="39"/>
-      <c r="C13" s="79">
+      <c r="C13" s="61">
         <v>13000000</v>
       </c>
       <c r="D13" s="39">
@@ -54805,7 +54801,7 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="39"/>
-      <c r="C14" s="79">
+      <c r="C14" s="61">
         <v>16000000</v>
       </c>
       <c r="D14" s="39">
@@ -54814,7 +54810,7 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="39"/>
-      <c r="C15" s="79">
+      <c r="C15" s="61">
         <v>19000000</v>
       </c>
       <c r="D15" s="39">
@@ -54823,7 +54819,7 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="39"/>
-      <c r="C16" s="79">
+      <c r="C16" s="61">
         <v>23000000</v>
       </c>
       <c r="D16" s="39">
@@ -54832,7 +54828,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="39"/>
-      <c r="C17" s="79">
+      <c r="C17" s="61">
         <v>27000000</v>
       </c>
       <c r="D17" s="39">
@@ -54841,7 +54837,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="39"/>
-      <c r="C18" s="79">
+      <c r="C18" s="61">
         <v>34000000</v>
       </c>
       <c r="D18" s="39">
@@ -54850,7 +54846,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="39"/>
-      <c r="C19" s="79">
+      <c r="C19" s="61">
         <v>42000000</v>
       </c>
       <c r="D19" s="39">
@@ -54859,7 +54855,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="39"/>
-      <c r="C20" s="79">
+      <c r="C20" s="61">
         <v>52000000</v>
       </c>
       <c r="D20" s="39">
@@ -54868,7 +54864,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="39"/>
-      <c r="C21" s="79">
+      <c r="C21" s="61">
         <v>65000000</v>
       </c>
       <c r="D21" s="39">

</xml_diff>

<commit_message>
Factory rework - Turkey + Caucasus
</commit_message>
<xml_diff>
--- a/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
+++ b/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\economy spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1904943-E2F7-4FBE-BB51-247328DE03E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20DB268-3616-450B-9254-E0E1FB09896F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C93B8E2A-6318-41E2-B454-20DC41C43396}"/>
   </bookViews>
@@ -2377,11 +2377,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2398,20 +2407,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8440,246 +8440,246 @@
   <sheetData>
     <row r="1" spans="2:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:70" x14ac:dyDescent="0.25">
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="71" t="s">
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="71" t="s">
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="71" t="s">
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="71" t="s">
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="72"/>
-      <c r="U2" s="72"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="71" t="s">
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="71" t="s">
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="72"/>
-      <c r="AC2" s="72"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="71" t="s">
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="72"/>
-      <c r="AG2" s="72"/>
-      <c r="AH2" s="73"/>
-      <c r="AI2" s="71" t="s">
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="AJ2" s="72"/>
-      <c r="AK2" s="72"/>
-      <c r="AL2" s="73"/>
-      <c r="AM2" s="71" t="s">
+      <c r="AJ2" s="65"/>
+      <c r="AK2" s="65"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="AN2" s="72"/>
-      <c r="AO2" s="72"/>
-      <c r="AP2" s="73"/>
-      <c r="AQ2" s="71" t="s">
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="AR2" s="72"/>
-      <c r="AS2" s="72"/>
-      <c r="AT2" s="73"/>
-      <c r="AU2" s="71" t="s">
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="AV2" s="72"/>
-      <c r="AW2" s="72"/>
-      <c r="AX2" s="73"/>
-      <c r="AY2" s="71" t="s">
+      <c r="AV2" s="65"/>
+      <c r="AW2" s="65"/>
+      <c r="AX2" s="66"/>
+      <c r="AY2" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="AZ2" s="72"/>
-      <c r="BA2" s="72"/>
-      <c r="BB2" s="73"/>
-      <c r="BC2" s="71" t="s">
+      <c r="AZ2" s="65"/>
+      <c r="BA2" s="65"/>
+      <c r="BB2" s="66"/>
+      <c r="BC2" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="BD2" s="72"/>
-      <c r="BE2" s="72"/>
-      <c r="BF2" s="73"/>
-      <c r="BG2" s="71" t="s">
+      <c r="BD2" s="65"/>
+      <c r="BE2" s="65"/>
+      <c r="BF2" s="66"/>
+      <c r="BG2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="BH2" s="72"/>
-      <c r="BI2" s="72"/>
-      <c r="BJ2" s="73"/>
-      <c r="BK2" s="71" t="s">
+      <c r="BH2" s="65"/>
+      <c r="BI2" s="65"/>
+      <c r="BJ2" s="66"/>
+      <c r="BK2" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="BL2" s="72"/>
-      <c r="BM2" s="72"/>
-      <c r="BN2" s="73"/>
-      <c r="BO2" s="71" t="s">
+      <c r="BL2" s="65"/>
+      <c r="BM2" s="65"/>
+      <c r="BN2" s="66"/>
+      <c r="BO2" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="BP2" s="72"/>
-      <c r="BQ2" s="72"/>
-      <c r="BR2" s="73"/>
+      <c r="BP2" s="65"/>
+      <c r="BQ2" s="65"/>
+      <c r="BR2" s="66"/>
     </row>
     <row r="3" spans="2:70" x14ac:dyDescent="0.25">
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65" t="s">
+      <c r="D3" s="68"/>
+      <c r="E3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="64" t="s">
+      <c r="F3" s="69"/>
+      <c r="G3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65" t="s">
+      <c r="H3" s="68"/>
+      <c r="I3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="66"/>
-      <c r="K3" s="64" t="s">
+      <c r="J3" s="69"/>
+      <c r="K3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65" t="s">
+      <c r="L3" s="68"/>
+      <c r="M3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="66"/>
-      <c r="O3" s="64" t="s">
+      <c r="N3" s="69"/>
+      <c r="O3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65" t="s">
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="66"/>
-      <c r="S3" s="64" t="s">
+      <c r="R3" s="69"/>
+      <c r="S3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65" t="s">
+      <c r="T3" s="68"/>
+      <c r="U3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="66"/>
-      <c r="W3" s="64" t="s">
+      <c r="V3" s="69"/>
+      <c r="W3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="65"/>
-      <c r="Y3" s="65" t="s">
+      <c r="X3" s="68"/>
+      <c r="Y3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="66"/>
-      <c r="AA3" s="64" t="s">
+      <c r="Z3" s="69"/>
+      <c r="AA3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65" t="s">
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AD3" s="66"/>
-      <c r="AE3" s="64" t="s">
+      <c r="AD3" s="69"/>
+      <c r="AE3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65" t="s">
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AH3" s="66"/>
-      <c r="AI3" s="64" t="s">
+      <c r="AH3" s="69"/>
+      <c r="AI3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AJ3" s="65"/>
-      <c r="AK3" s="65" t="s">
+      <c r="AJ3" s="68"/>
+      <c r="AK3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AL3" s="66"/>
-      <c r="AM3" s="64" t="s">
+      <c r="AL3" s="69"/>
+      <c r="AM3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65" t="s">
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AP3" s="66"/>
-      <c r="AQ3" s="64" t="s">
+      <c r="AP3" s="69"/>
+      <c r="AQ3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65" t="s">
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AT3" s="66"/>
-      <c r="AU3" s="64" t="s">
+      <c r="AT3" s="69"/>
+      <c r="AU3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AV3" s="65"/>
-      <c r="AW3" s="65" t="s">
+      <c r="AV3" s="68"/>
+      <c r="AW3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AX3" s="66"/>
-      <c r="AY3" s="64" t="s">
+      <c r="AX3" s="69"/>
+      <c r="AY3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AZ3" s="65"/>
-      <c r="BA3" s="65" t="s">
+      <c r="AZ3" s="68"/>
+      <c r="BA3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BB3" s="66"/>
-      <c r="BC3" s="64" t="s">
+      <c r="BB3" s="69"/>
+      <c r="BC3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BD3" s="65"/>
-      <c r="BE3" s="65" t="s">
+      <c r="BD3" s="68"/>
+      <c r="BE3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BF3" s="66"/>
-      <c r="BG3" s="64" t="s">
+      <c r="BF3" s="69"/>
+      <c r="BG3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BH3" s="65"/>
-      <c r="BI3" s="65" t="s">
+      <c r="BH3" s="68"/>
+      <c r="BI3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BJ3" s="66"/>
-      <c r="BK3" s="64" t="s">
+      <c r="BJ3" s="69"/>
+      <c r="BK3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BL3" s="65"/>
-      <c r="BM3" s="65" t="s">
+      <c r="BL3" s="68"/>
+      <c r="BM3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BN3" s="66"/>
-      <c r="BO3" s="64" t="s">
+      <c r="BN3" s="69"/>
+      <c r="BO3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BP3" s="65"/>
-      <c r="BQ3" s="65" t="s">
+      <c r="BP3" s="68"/>
+      <c r="BQ3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BR3" s="66"/>
+      <c r="BR3" s="69"/>
     </row>
     <row r="4" spans="2:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
@@ -8891,10 +8891,10 @@
       <c r="B5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="67">
+      <c r="C5" s="70">
         <v>1</v>
       </c>
-      <c r="D5" s="68"/>
+      <c r="D5" s="71"/>
       <c r="E5" s="22">
         <v>2.9780000000000002</v>
       </c>
@@ -8902,10 +8902,10 @@
         <f>E5/C5-1</f>
         <v>1.9780000000000002</v>
       </c>
-      <c r="G5" s="67">
+      <c r="G5" s="70">
         <v>1</v>
       </c>
-      <c r="H5" s="68"/>
+      <c r="H5" s="71"/>
       <c r="I5" s="22">
         <v>1.84</v>
       </c>
@@ -8913,10 +8913,10 @@
         <f>I5/G5-1</f>
         <v>0.84000000000000008</v>
       </c>
-      <c r="K5" s="67">
+      <c r="K5" s="70">
         <v>1</v>
       </c>
-      <c r="L5" s="68"/>
+      <c r="L5" s="71"/>
       <c r="M5" s="22">
         <v>2.2770000000000001</v>
       </c>
@@ -8924,10 +8924,10 @@
         <f>M5/K5-1</f>
         <v>1.2770000000000001</v>
       </c>
-      <c r="O5" s="67">
+      <c r="O5" s="70">
         <v>1</v>
       </c>
-      <c r="P5" s="68"/>
+      <c r="P5" s="71"/>
       <c r="Q5" s="22">
         <v>2.8029999999999999</v>
       </c>
@@ -8938,7 +8938,7 @@
       <c r="S5" s="74">
         <v>2</v>
       </c>
-      <c r="T5" s="68"/>
+      <c r="T5" s="71"/>
       <c r="U5" s="22">
         <v>12.585000000000001</v>
       </c>
@@ -8946,10 +8946,10 @@
         <f>U5/S5-1</f>
         <v>5.2925000000000004</v>
       </c>
-      <c r="W5" s="67">
+      <c r="W5" s="70">
         <v>2</v>
       </c>
-      <c r="X5" s="68"/>
+      <c r="X5" s="71"/>
       <c r="Y5" s="22">
         <v>10.067</v>
       </c>
@@ -8957,10 +8957,10 @@
         <f>Y5/W5-1</f>
         <v>4.0335000000000001</v>
       </c>
-      <c r="AA5" s="67">
+      <c r="AA5" s="70">
         <v>2</v>
       </c>
-      <c r="AB5" s="68"/>
+      <c r="AB5" s="71"/>
       <c r="AC5" s="22">
         <v>9.9779999999999998</v>
       </c>
@@ -8968,10 +8968,10 @@
         <f>AC5/AA5-1</f>
         <v>3.9889999999999999</v>
       </c>
-      <c r="AE5" s="67">
+      <c r="AE5" s="70">
         <v>7</v>
       </c>
-      <c r="AF5" s="68"/>
+      <c r="AF5" s="71"/>
       <c r="AG5" s="22">
         <v>15.536</v>
       </c>
@@ -8979,10 +8979,10 @@
         <f>AG5/AE5-1</f>
         <v>1.2194285714285713</v>
       </c>
-      <c r="AI5" s="67">
+      <c r="AI5" s="70">
         <v>7</v>
       </c>
-      <c r="AJ5" s="68"/>
+      <c r="AJ5" s="71"/>
       <c r="AK5" s="22">
         <v>24.87</v>
       </c>
@@ -8990,10 +8990,10 @@
         <f>AK5/AI5-1</f>
         <v>2.5528571428571429</v>
       </c>
-      <c r="AM5" s="67">
+      <c r="AM5" s="70">
         <v>7</v>
       </c>
-      <c r="AN5" s="68"/>
+      <c r="AN5" s="71"/>
       <c r="AO5" s="22">
         <v>14.685</v>
       </c>
@@ -9001,10 +9001,10 @@
         <f>AO5/AM5-1</f>
         <v>1.0978571428571429</v>
       </c>
-      <c r="AQ5" s="67">
+      <c r="AQ5" s="70">
         <v>10</v>
       </c>
-      <c r="AR5" s="68"/>
+      <c r="AR5" s="71"/>
       <c r="AS5" s="22">
         <v>13.314</v>
       </c>
@@ -9012,10 +9012,10 @@
         <f>AS5/AQ5-1</f>
         <v>0.33139999999999992</v>
       </c>
-      <c r="AU5" s="67">
+      <c r="AU5" s="70">
         <v>15</v>
       </c>
-      <c r="AV5" s="68"/>
+      <c r="AV5" s="71"/>
       <c r="AW5" s="22">
         <v>35.488</v>
       </c>
@@ -9023,10 +9023,10 @@
         <f>AW5/AU5-1</f>
         <v>1.3658666666666668</v>
       </c>
-      <c r="AY5" s="67">
+      <c r="AY5" s="70">
         <v>20</v>
       </c>
-      <c r="AZ5" s="68"/>
+      <c r="AZ5" s="71"/>
       <c r="BA5" s="22">
         <v>46.418999999999997</v>
       </c>
@@ -9034,10 +9034,10 @@
         <f>BA5/AY5-1</f>
         <v>1.3209499999999998</v>
       </c>
-      <c r="BC5" s="67">
+      <c r="BC5" s="70">
         <v>20</v>
       </c>
-      <c r="BD5" s="68"/>
+      <c r="BD5" s="71"/>
       <c r="BE5" s="22">
         <v>77.132000000000005</v>
       </c>
@@ -9045,10 +9045,10 @@
         <f>BE5/BC5-1</f>
         <v>2.8566000000000003</v>
       </c>
-      <c r="BG5" s="67">
+      <c r="BG5" s="70">
         <v>20</v>
       </c>
-      <c r="BH5" s="68"/>
+      <c r="BH5" s="71"/>
       <c r="BI5" s="22">
         <v>50.906999999999996</v>
       </c>
@@ -9056,10 +9056,10 @@
         <f>BI5/BG5-1</f>
         <v>1.54535</v>
       </c>
-      <c r="BK5" s="67">
+      <c r="BK5" s="70">
         <v>30</v>
       </c>
-      <c r="BL5" s="68"/>
+      <c r="BL5" s="71"/>
       <c r="BM5" s="22">
         <v>39.054000000000002</v>
       </c>
@@ -9067,10 +9067,10 @@
         <f>BM5/BK5-1</f>
         <v>0.30180000000000007</v>
       </c>
-      <c r="BO5" s="67">
+      <c r="BO5" s="70">
         <v>30</v>
       </c>
-      <c r="BP5" s="68"/>
+      <c r="BP5" s="71"/>
       <c r="BQ5" s="22">
         <v>40.4</v>
       </c>
@@ -9083,34 +9083,34 @@
       <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="62">
+      <c r="C6" s="72">
         <v>11</v>
       </c>
-      <c r="D6" s="63"/>
+      <c r="D6" s="73"/>
       <c r="E6" s="23">
         <v>10</v>
       </c>
       <c r="F6" s="26"/>
-      <c r="G6" s="62">
+      <c r="G6" s="72">
         <v>17</v>
       </c>
-      <c r="H6" s="63"/>
+      <c r="H6" s="73"/>
       <c r="I6" s="23">
         <v>30</v>
       </c>
       <c r="J6" s="26"/>
-      <c r="K6" s="62">
+      <c r="K6" s="72">
         <v>10</v>
       </c>
-      <c r="L6" s="63"/>
+      <c r="L6" s="73"/>
       <c r="M6" s="23">
         <v>18</v>
       </c>
       <c r="N6" s="26"/>
-      <c r="O6" s="62">
+      <c r="O6" s="72">
         <v>18</v>
       </c>
-      <c r="P6" s="63"/>
+      <c r="P6" s="73"/>
       <c r="Q6" s="23">
         <v>22</v>
       </c>
@@ -9118,103 +9118,103 @@
       <c r="S6" s="75">
         <v>40</v>
       </c>
-      <c r="T6" s="63"/>
+      <c r="T6" s="73"/>
       <c r="U6" s="23">
         <v>37</v>
       </c>
       <c r="V6" s="26"/>
-      <c r="W6" s="62">
+      <c r="W6" s="72">
         <v>18</v>
       </c>
-      <c r="X6" s="63"/>
+      <c r="X6" s="73"/>
       <c r="Y6" s="23">
         <v>18</v>
       </c>
       <c r="Z6" s="26"/>
-      <c r="AA6" s="62">
+      <c r="AA6" s="72">
         <v>18</v>
       </c>
-      <c r="AB6" s="63"/>
+      <c r="AB6" s="73"/>
       <c r="AC6" s="23">
         <v>20</v>
       </c>
       <c r="AD6" s="26"/>
-      <c r="AE6" s="62">
+      <c r="AE6" s="72">
         <v>14</v>
       </c>
-      <c r="AF6" s="63"/>
+      <c r="AF6" s="73"/>
       <c r="AG6" s="23">
         <v>19</v>
       </c>
       <c r="AH6" s="26"/>
-      <c r="AI6" s="62">
+      <c r="AI6" s="72">
         <v>23</v>
       </c>
-      <c r="AJ6" s="63"/>
+      <c r="AJ6" s="73"/>
       <c r="AK6" s="23">
         <v>21</v>
       </c>
       <c r="AL6" s="26"/>
-      <c r="AM6" s="62">
+      <c r="AM6" s="72">
         <v>7</v>
       </c>
-      <c r="AN6" s="63"/>
+      <c r="AN6" s="73"/>
       <c r="AO6" s="23">
         <v>9</v>
       </c>
       <c r="AP6" s="26"/>
-      <c r="AQ6" s="62">
+      <c r="AQ6" s="72">
         <v>14</v>
       </c>
-      <c r="AR6" s="63"/>
+      <c r="AR6" s="73"/>
       <c r="AS6" s="23">
         <v>22</v>
       </c>
       <c r="AT6" s="26"/>
-      <c r="AU6" s="62">
+      <c r="AU6" s="72">
         <v>12</v>
       </c>
-      <c r="AV6" s="63"/>
+      <c r="AV6" s="73"/>
       <c r="AW6" s="23">
         <v>40</v>
       </c>
       <c r="AX6" s="26"/>
-      <c r="AY6" s="62">
+      <c r="AY6" s="72">
         <v>37</v>
       </c>
-      <c r="AZ6" s="63"/>
+      <c r="AZ6" s="73"/>
       <c r="BA6" s="23">
         <v>44</v>
       </c>
       <c r="BB6" s="26"/>
-      <c r="BC6" s="62">
+      <c r="BC6" s="72">
         <v>30</v>
       </c>
-      <c r="BD6" s="63"/>
+      <c r="BD6" s="73"/>
       <c r="BE6" s="23">
         <v>58</v>
       </c>
       <c r="BF6" s="26"/>
-      <c r="BG6" s="62">
+      <c r="BG6" s="72">
         <v>23</v>
       </c>
-      <c r="BH6" s="63"/>
+      <c r="BH6" s="73"/>
       <c r="BI6" s="23">
         <v>47</v>
       </c>
       <c r="BJ6" s="26"/>
-      <c r="BK6" s="62">
+      <c r="BK6" s="72">
         <v>37</v>
       </c>
-      <c r="BL6" s="63"/>
+      <c r="BL6" s="73"/>
       <c r="BM6" s="23">
         <v>40</v>
       </c>
       <c r="BN6" s="26"/>
-      <c r="BO6" s="62">
+      <c r="BO6" s="72">
         <v>36</v>
       </c>
-      <c r="BP6" s="63"/>
+      <c r="BP6" s="73"/>
       <c r="BQ6" s="23">
         <v>23</v>
       </c>
@@ -9224,104 +9224,104 @@
       <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="23">
         <v>18</v>
       </c>
       <c r="F7" s="26"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="63"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="73"/>
       <c r="I7" s="23">
         <v>30</v>
       </c>
       <c r="J7" s="26"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="63"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="73"/>
       <c r="M7" s="23">
         <v>32</v>
       </c>
       <c r="N7" s="26"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="63"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="73"/>
       <c r="Q7" s="23">
         <v>18</v>
       </c>
       <c r="R7" s="26"/>
       <c r="S7" s="75"/>
-      <c r="T7" s="63"/>
+      <c r="T7" s="73"/>
       <c r="U7" s="23">
         <v>22</v>
       </c>
       <c r="V7" s="26"/>
-      <c r="W7" s="62"/>
-      <c r="X7" s="63"/>
+      <c r="W7" s="72"/>
+      <c r="X7" s="73"/>
       <c r="Y7" s="23">
         <v>22</v>
       </c>
       <c r="Z7" s="26"/>
-      <c r="AA7" s="62"/>
-      <c r="AB7" s="63"/>
+      <c r="AA7" s="72"/>
+      <c r="AB7" s="73"/>
       <c r="AC7" s="23">
         <v>10</v>
       </c>
       <c r="AD7" s="26"/>
-      <c r="AE7" s="62"/>
-      <c r="AF7" s="63"/>
+      <c r="AE7" s="72"/>
+      <c r="AF7" s="73"/>
       <c r="AG7" s="23">
         <v>43</v>
       </c>
       <c r="AH7" s="26"/>
-      <c r="AI7" s="62"/>
-      <c r="AJ7" s="63"/>
+      <c r="AI7" s="72"/>
+      <c r="AJ7" s="73"/>
       <c r="AK7" s="23">
         <v>27</v>
       </c>
       <c r="AL7" s="26"/>
-      <c r="AM7" s="62"/>
-      <c r="AN7" s="63"/>
+      <c r="AM7" s="72"/>
+      <c r="AN7" s="73"/>
       <c r="AO7" s="23">
         <v>6</v>
       </c>
       <c r="AP7" s="26"/>
-      <c r="AQ7" s="62"/>
-      <c r="AR7" s="63"/>
+      <c r="AQ7" s="72"/>
+      <c r="AR7" s="73"/>
       <c r="AS7" s="23">
         <v>15</v>
       </c>
       <c r="AT7" s="26"/>
-      <c r="AU7" s="62"/>
-      <c r="AV7" s="63"/>
+      <c r="AU7" s="72"/>
+      <c r="AV7" s="73"/>
       <c r="AW7" s="23">
         <v>25</v>
       </c>
       <c r="AX7" s="26"/>
-      <c r="AY7" s="62"/>
-      <c r="AZ7" s="63"/>
+      <c r="AY7" s="72"/>
+      <c r="AZ7" s="73"/>
       <c r="BA7" s="23">
         <v>18</v>
       </c>
       <c r="BB7" s="26"/>
-      <c r="BC7" s="62"/>
-      <c r="BD7" s="63"/>
+      <c r="BC7" s="72"/>
+      <c r="BD7" s="73"/>
       <c r="BE7" s="23">
         <v>26</v>
       </c>
       <c r="BF7" s="26"/>
-      <c r="BG7" s="62"/>
-      <c r="BH7" s="63"/>
+      <c r="BG7" s="72"/>
+      <c r="BH7" s="73"/>
       <c r="BI7" s="23">
         <v>36</v>
       </c>
       <c r="BJ7" s="26"/>
-      <c r="BK7" s="62"/>
-      <c r="BL7" s="63"/>
+      <c r="BK7" s="72"/>
+      <c r="BL7" s="73"/>
       <c r="BM7" s="23">
         <v>23</v>
       </c>
       <c r="BN7" s="26"/>
-      <c r="BO7" s="62"/>
-      <c r="BP7" s="63"/>
+      <c r="BO7" s="72"/>
+      <c r="BP7" s="73"/>
       <c r="BQ7" s="23">
         <v>33</v>
       </c>
@@ -9331,11 +9331,11 @@
       <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="69">
+      <c r="C8" s="62">
         <f>C6</f>
         <v>11</v>
       </c>
-      <c r="D8" s="70"/>
+      <c r="D8" s="63"/>
       <c r="E8" s="24">
         <f>(E6+E7)/2</f>
         <v>14</v>
@@ -9344,11 +9344,11 @@
         <f>E8/C8-1</f>
         <v>0.27272727272727271</v>
       </c>
-      <c r="G8" s="69">
+      <c r="G8" s="62">
         <f>G6</f>
         <v>17</v>
       </c>
-      <c r="H8" s="70"/>
+      <c r="H8" s="63"/>
       <c r="I8" s="24">
         <f>(I6+I7)/2</f>
         <v>30</v>
@@ -9357,11 +9357,11 @@
         <f>I8/G8-1</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="K8" s="69">
+      <c r="K8" s="62">
         <f>K6</f>
         <v>10</v>
       </c>
-      <c r="L8" s="70"/>
+      <c r="L8" s="63"/>
       <c r="M8" s="24">
         <f>(M6+M7)/2</f>
         <v>25</v>
@@ -9370,11 +9370,11 @@
         <f>M8/K8-1</f>
         <v>1.5</v>
       </c>
-      <c r="O8" s="69">
+      <c r="O8" s="62">
         <f>O6</f>
         <v>18</v>
       </c>
-      <c r="P8" s="70"/>
+      <c r="P8" s="63"/>
       <c r="Q8" s="24">
         <f>(Q6+Q7)/2</f>
         <v>20</v>
@@ -9387,7 +9387,7 @@
         <f>S6</f>
         <v>40</v>
       </c>
-      <c r="T8" s="70"/>
+      <c r="T8" s="63"/>
       <c r="U8" s="24">
         <f>(U6+U7)/2</f>
         <v>29.5</v>
@@ -9396,11 +9396,11 @@
         <f>U8/S8-1</f>
         <v>-0.26249999999999996</v>
       </c>
-      <c r="W8" s="69">
+      <c r="W8" s="62">
         <f>W6</f>
         <v>18</v>
       </c>
-      <c r="X8" s="70"/>
+      <c r="X8" s="63"/>
       <c r="Y8" s="24">
         <f>(Y6+Y7)/2</f>
         <v>20</v>
@@ -9409,11 +9409,11 @@
         <f>Y8/W8-1</f>
         <v>0.11111111111111116</v>
       </c>
-      <c r="AA8" s="69">
+      <c r="AA8" s="62">
         <f>AA6</f>
         <v>18</v>
       </c>
-      <c r="AB8" s="70"/>
+      <c r="AB8" s="63"/>
       <c r="AC8" s="24">
         <f>(AC6+AC7)/2</f>
         <v>15</v>
@@ -9422,11 +9422,11 @@
         <f>AC8/AA8-1</f>
         <v>-0.16666666666666663</v>
       </c>
-      <c r="AE8" s="69">
+      <c r="AE8" s="62">
         <f>AE6</f>
         <v>14</v>
       </c>
-      <c r="AF8" s="70"/>
+      <c r="AF8" s="63"/>
       <c r="AG8" s="24">
         <f>(AG6+AG7)/2</f>
         <v>31</v>
@@ -9435,11 +9435,11 @@
         <f>AG8/AE8-1</f>
         <v>1.2142857142857144</v>
       </c>
-      <c r="AI8" s="69">
+      <c r="AI8" s="62">
         <f>AI6</f>
         <v>23</v>
       </c>
-      <c r="AJ8" s="70"/>
+      <c r="AJ8" s="63"/>
       <c r="AK8" s="24">
         <f>(AK6+AK7)/2</f>
         <v>24</v>
@@ -9448,11 +9448,11 @@
         <f>AK8/AI8-1</f>
         <v>4.3478260869565188E-2</v>
       </c>
-      <c r="AM8" s="69">
+      <c r="AM8" s="62">
         <f>AM6</f>
         <v>7</v>
       </c>
-      <c r="AN8" s="70"/>
+      <c r="AN8" s="63"/>
       <c r="AO8" s="24">
         <f>(AO6+AO7)/2</f>
         <v>7.5</v>
@@ -9461,11 +9461,11 @@
         <f>AO8/AM8-1</f>
         <v>7.1428571428571397E-2</v>
       </c>
-      <c r="AQ8" s="69">
+      <c r="AQ8" s="62">
         <f>AQ6</f>
         <v>14</v>
       </c>
-      <c r="AR8" s="70"/>
+      <c r="AR8" s="63"/>
       <c r="AS8" s="24">
         <f>(AS6+AS7)/2</f>
         <v>18.5</v>
@@ -9474,11 +9474,11 @@
         <f>AS8/AQ8-1</f>
         <v>0.3214285714285714</v>
       </c>
-      <c r="AU8" s="69">
+      <c r="AU8" s="62">
         <f>AU6</f>
         <v>12</v>
       </c>
-      <c r="AV8" s="70"/>
+      <c r="AV8" s="63"/>
       <c r="AW8" s="24">
         <f>(AW6+AW7)/2</f>
         <v>32.5</v>
@@ -9487,11 +9487,11 @@
         <f>AW8/AU8-1</f>
         <v>1.7083333333333335</v>
       </c>
-      <c r="AY8" s="69">
+      <c r="AY8" s="62">
         <f>AY6</f>
         <v>37</v>
       </c>
-      <c r="AZ8" s="70"/>
+      <c r="AZ8" s="63"/>
       <c r="BA8" s="24">
         <f>(BA6+BA7)/2</f>
         <v>31</v>
@@ -9500,11 +9500,11 @@
         <f>BA8/AY8-1</f>
         <v>-0.16216216216216217</v>
       </c>
-      <c r="BC8" s="69">
+      <c r="BC8" s="62">
         <f>BC6</f>
         <v>30</v>
       </c>
-      <c r="BD8" s="70"/>
+      <c r="BD8" s="63"/>
       <c r="BE8" s="24">
         <f>(BE6+BE7)/2</f>
         <v>42</v>
@@ -9513,11 +9513,11 @@
         <f>BE8/BC8-1</f>
         <v>0.39999999999999991</v>
       </c>
-      <c r="BG8" s="69">
+      <c r="BG8" s="62">
         <f>BG6</f>
         <v>23</v>
       </c>
-      <c r="BH8" s="70"/>
+      <c r="BH8" s="63"/>
       <c r="BI8" s="24">
         <f>(BI6+BI7)/2</f>
         <v>41.5</v>
@@ -9526,11 +9526,11 @@
         <f>BI8/BG8-1</f>
         <v>0.80434782608695654</v>
       </c>
-      <c r="BK8" s="69">
+      <c r="BK8" s="62">
         <f>BK6</f>
         <v>37</v>
       </c>
-      <c r="BL8" s="70"/>
+      <c r="BL8" s="63"/>
       <c r="BM8" s="24">
         <f>(BM6+BM7)/2</f>
         <v>31.5</v>
@@ -9539,11 +9539,11 @@
         <f>BM8/BK8-1</f>
         <v>-0.14864864864864868</v>
       </c>
-      <c r="BO8" s="69">
+      <c r="BO8" s="62">
         <f>BO6</f>
         <v>36</v>
       </c>
-      <c r="BP8" s="70"/>
+      <c r="BP8" s="63"/>
       <c r="BQ8" s="24">
         <f>(BQ6+BQ7)/2</f>
         <v>28</v>
@@ -12527,15 +12527,92 @@
     </row>
   </sheetData>
   <mergeCells count="119">
-    <mergeCell ref="BC8:BD8"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="BO7:BP7"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AU7:AV7"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="BE3:BF3"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BC7:BD7"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="AY7:AZ7"/>
+    <mergeCell ref="BK8:BL8"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AQ3:AR3"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AI7:AJ7"/>
+    <mergeCell ref="AU2:AX2"/>
+    <mergeCell ref="AY8:AZ8"/>
+    <mergeCell ref="BG8:BH8"/>
+    <mergeCell ref="BG2:BJ2"/>
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BI3:BJ3"/>
+    <mergeCell ref="BG5:BH5"/>
+    <mergeCell ref="BG6:BH6"/>
+    <mergeCell ref="BG7:BH7"/>
+    <mergeCell ref="AU8:AV8"/>
+    <mergeCell ref="AI8:AJ8"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="BO8:BP8"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="BO2:BR2"/>
+    <mergeCell ref="BO3:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="AY2:BB2"/>
+    <mergeCell ref="AY3:AZ3"/>
+    <mergeCell ref="BA3:BB3"/>
+    <mergeCell ref="BK2:BN2"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="BM3:BN3"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BK7:BL7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="G5:H5"/>
@@ -12560,92 +12637,15 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="W8:X8"/>
     <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="BO8:BP8"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="BO2:BR2"/>
-    <mergeCell ref="BO3:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BO5:BP5"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="AY2:BB2"/>
-    <mergeCell ref="AY3:AZ3"/>
-    <mergeCell ref="BA3:BB3"/>
-    <mergeCell ref="BK2:BN2"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="BM3:BN3"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BK7:BL7"/>
-    <mergeCell ref="BK8:BL8"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AQ3:AR3"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AI7:AJ7"/>
-    <mergeCell ref="AU2:AX2"/>
-    <mergeCell ref="AY8:AZ8"/>
-    <mergeCell ref="BG8:BH8"/>
-    <mergeCell ref="BG2:BJ2"/>
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BI3:BJ3"/>
-    <mergeCell ref="BG5:BH5"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="BG7:BH7"/>
-    <mergeCell ref="AU8:AV8"/>
-    <mergeCell ref="AI8:AJ8"/>
-    <mergeCell ref="AS3:AT3"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="BO7:BP7"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AW3:AX3"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AU7:AV7"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="BE3:BF3"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BC7:BD7"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="AY7:AZ7"/>
+    <mergeCell ref="BC8:BD8"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="BC2:BF2"/>
   </mergeCells>
   <conditionalFormatting sqref="BP21">
     <cfRule type="cellIs" dxfId="63" priority="103" operator="lessThan">
@@ -13095,10 +13095,10 @@
   <dimension ref="B1:AN187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="15" topLeftCell="C166" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="15" topLeftCell="C161" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="B180" sqref="B180"/>
+      <selection pane="bottomRight" activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14594,7 +14594,7 @@
       </c>
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="60" t="s">
         <v>68</v>
       </c>
       <c r="C23" s="35">
@@ -15029,7 +15029,7 @@
       </c>
     </row>
     <row r="26" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="60" t="s">
         <v>75</v>
       </c>
       <c r="C26" s="35">
@@ -22424,7 +22424,7 @@
       </c>
     </row>
     <row r="77" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B77" s="35" t="s">
+      <c r="B77" s="60" t="s">
         <v>192</v>
       </c>
       <c r="C77" s="35">
@@ -36924,7 +36924,7 @@
       </c>
     </row>
     <row r="177" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B177" s="35" t="s">
+      <c r="B177" s="60" t="s">
         <v>42</v>
       </c>
       <c r="C177" s="35">

</xml_diff>

<commit_message>
Factories - Middle East
</commit_message>
<xml_diff>
--- a/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
+++ b/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\economy spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3085796E-FE9A-402B-A422-1A4A4940C462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579257D7-553E-4F21-99DD-FB0E7E750C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C93B8E2A-6318-41E2-B454-20DC41C43396}"/>
   </bookViews>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4197" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4198" uniqueCount="508">
   <si>
     <t>Population Tax Rate</t>
   </si>
@@ -1703,6 +1703,9 @@
   <si>
     <t>Syria</t>
   </si>
+  <si>
+    <t>Yemen</t>
+  </si>
 </sst>
 </file>
 
@@ -2380,11 +2383,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2401,20 +2413,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8443,246 +8446,246 @@
   <sheetData>
     <row r="1" spans="2:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:70" x14ac:dyDescent="0.25">
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="71" t="s">
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="71" t="s">
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="71" t="s">
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="71" t="s">
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="72"/>
-      <c r="U2" s="72"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="71" t="s">
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="71" t="s">
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="72"/>
-      <c r="AC2" s="72"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="71" t="s">
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="72"/>
-      <c r="AG2" s="72"/>
-      <c r="AH2" s="73"/>
-      <c r="AI2" s="71" t="s">
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="AJ2" s="72"/>
-      <c r="AK2" s="72"/>
-      <c r="AL2" s="73"/>
-      <c r="AM2" s="71" t="s">
+      <c r="AJ2" s="65"/>
+      <c r="AK2" s="65"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="AN2" s="72"/>
-      <c r="AO2" s="72"/>
-      <c r="AP2" s="73"/>
-      <c r="AQ2" s="71" t="s">
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="AR2" s="72"/>
-      <c r="AS2" s="72"/>
-      <c r="AT2" s="73"/>
-      <c r="AU2" s="71" t="s">
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="AV2" s="72"/>
-      <c r="AW2" s="72"/>
-      <c r="AX2" s="73"/>
-      <c r="AY2" s="71" t="s">
+      <c r="AV2" s="65"/>
+      <c r="AW2" s="65"/>
+      <c r="AX2" s="66"/>
+      <c r="AY2" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="AZ2" s="72"/>
-      <c r="BA2" s="72"/>
-      <c r="BB2" s="73"/>
-      <c r="BC2" s="71" t="s">
+      <c r="AZ2" s="65"/>
+      <c r="BA2" s="65"/>
+      <c r="BB2" s="66"/>
+      <c r="BC2" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="BD2" s="72"/>
-      <c r="BE2" s="72"/>
-      <c r="BF2" s="73"/>
-      <c r="BG2" s="71" t="s">
+      <c r="BD2" s="65"/>
+      <c r="BE2" s="65"/>
+      <c r="BF2" s="66"/>
+      <c r="BG2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="BH2" s="72"/>
-      <c r="BI2" s="72"/>
-      <c r="BJ2" s="73"/>
-      <c r="BK2" s="71" t="s">
+      <c r="BH2" s="65"/>
+      <c r="BI2" s="65"/>
+      <c r="BJ2" s="66"/>
+      <c r="BK2" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="BL2" s="72"/>
-      <c r="BM2" s="72"/>
-      <c r="BN2" s="73"/>
-      <c r="BO2" s="71" t="s">
+      <c r="BL2" s="65"/>
+      <c r="BM2" s="65"/>
+      <c r="BN2" s="66"/>
+      <c r="BO2" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="BP2" s="72"/>
-      <c r="BQ2" s="72"/>
-      <c r="BR2" s="73"/>
+      <c r="BP2" s="65"/>
+      <c r="BQ2" s="65"/>
+      <c r="BR2" s="66"/>
     </row>
     <row r="3" spans="2:70" x14ac:dyDescent="0.25">
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65" t="s">
+      <c r="D3" s="68"/>
+      <c r="E3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="64" t="s">
+      <c r="F3" s="69"/>
+      <c r="G3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65" t="s">
+      <c r="H3" s="68"/>
+      <c r="I3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="66"/>
-      <c r="K3" s="64" t="s">
+      <c r="J3" s="69"/>
+      <c r="K3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65" t="s">
+      <c r="L3" s="68"/>
+      <c r="M3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="66"/>
-      <c r="O3" s="64" t="s">
+      <c r="N3" s="69"/>
+      <c r="O3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65" t="s">
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="66"/>
-      <c r="S3" s="64" t="s">
+      <c r="R3" s="69"/>
+      <c r="S3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65" t="s">
+      <c r="T3" s="68"/>
+      <c r="U3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="66"/>
-      <c r="W3" s="64" t="s">
+      <c r="V3" s="69"/>
+      <c r="W3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="65"/>
-      <c r="Y3" s="65" t="s">
+      <c r="X3" s="68"/>
+      <c r="Y3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="66"/>
-      <c r="AA3" s="64" t="s">
+      <c r="Z3" s="69"/>
+      <c r="AA3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65" t="s">
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AD3" s="66"/>
-      <c r="AE3" s="64" t="s">
+      <c r="AD3" s="69"/>
+      <c r="AE3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65" t="s">
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AH3" s="66"/>
-      <c r="AI3" s="64" t="s">
+      <c r="AH3" s="69"/>
+      <c r="AI3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AJ3" s="65"/>
-      <c r="AK3" s="65" t="s">
+      <c r="AJ3" s="68"/>
+      <c r="AK3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AL3" s="66"/>
-      <c r="AM3" s="64" t="s">
+      <c r="AL3" s="69"/>
+      <c r="AM3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65" t="s">
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AP3" s="66"/>
-      <c r="AQ3" s="64" t="s">
+      <c r="AP3" s="69"/>
+      <c r="AQ3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65" t="s">
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AT3" s="66"/>
-      <c r="AU3" s="64" t="s">
+      <c r="AT3" s="69"/>
+      <c r="AU3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AV3" s="65"/>
-      <c r="AW3" s="65" t="s">
+      <c r="AV3" s="68"/>
+      <c r="AW3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AX3" s="66"/>
-      <c r="AY3" s="64" t="s">
+      <c r="AX3" s="69"/>
+      <c r="AY3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AZ3" s="65"/>
-      <c r="BA3" s="65" t="s">
+      <c r="AZ3" s="68"/>
+      <c r="BA3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BB3" s="66"/>
-      <c r="BC3" s="64" t="s">
+      <c r="BB3" s="69"/>
+      <c r="BC3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BD3" s="65"/>
-      <c r="BE3" s="65" t="s">
+      <c r="BD3" s="68"/>
+      <c r="BE3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BF3" s="66"/>
-      <c r="BG3" s="64" t="s">
+      <c r="BF3" s="69"/>
+      <c r="BG3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BH3" s="65"/>
-      <c r="BI3" s="65" t="s">
+      <c r="BH3" s="68"/>
+      <c r="BI3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BJ3" s="66"/>
-      <c r="BK3" s="64" t="s">
+      <c r="BJ3" s="69"/>
+      <c r="BK3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BL3" s="65"/>
-      <c r="BM3" s="65" t="s">
+      <c r="BL3" s="68"/>
+      <c r="BM3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BN3" s="66"/>
-      <c r="BO3" s="64" t="s">
+      <c r="BN3" s="69"/>
+      <c r="BO3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BP3" s="65"/>
-      <c r="BQ3" s="65" t="s">
+      <c r="BP3" s="68"/>
+      <c r="BQ3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BR3" s="66"/>
+      <c r="BR3" s="69"/>
     </row>
     <row r="4" spans="2:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
@@ -8894,10 +8897,10 @@
       <c r="B5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="67">
-        <v>1</v>
-      </c>
-      <c r="D5" s="68"/>
+      <c r="C5" s="70">
+        <v>1</v>
+      </c>
+      <c r="D5" s="71"/>
       <c r="E5" s="22">
         <v>2.9780000000000002</v>
       </c>
@@ -8905,10 +8908,10 @@
         <f>E5/C5-1</f>
         <v>1.9780000000000002</v>
       </c>
-      <c r="G5" s="67">
-        <v>1</v>
-      </c>
-      <c r="H5" s="68"/>
+      <c r="G5" s="70">
+        <v>1</v>
+      </c>
+      <c r="H5" s="71"/>
       <c r="I5" s="22">
         <v>1.84</v>
       </c>
@@ -8916,10 +8919,10 @@
         <f>I5/G5-1</f>
         <v>0.84000000000000008</v>
       </c>
-      <c r="K5" s="67">
-        <v>1</v>
-      </c>
-      <c r="L5" s="68"/>
+      <c r="K5" s="70">
+        <v>1</v>
+      </c>
+      <c r="L5" s="71"/>
       <c r="M5" s="22">
         <v>2.2770000000000001</v>
       </c>
@@ -8927,10 +8930,10 @@
         <f>M5/K5-1</f>
         <v>1.2770000000000001</v>
       </c>
-      <c r="O5" s="67">
-        <v>1</v>
-      </c>
-      <c r="P5" s="68"/>
+      <c r="O5" s="70">
+        <v>1</v>
+      </c>
+      <c r="P5" s="71"/>
       <c r="Q5" s="22">
         <v>2.8029999999999999</v>
       </c>
@@ -8941,7 +8944,7 @@
       <c r="S5" s="74">
         <v>2</v>
       </c>
-      <c r="T5" s="68"/>
+      <c r="T5" s="71"/>
       <c r="U5" s="22">
         <v>12.585000000000001</v>
       </c>
@@ -8949,10 +8952,10 @@
         <f>U5/S5-1</f>
         <v>5.2925000000000004</v>
       </c>
-      <c r="W5" s="67">
+      <c r="W5" s="70">
         <v>2</v>
       </c>
-      <c r="X5" s="68"/>
+      <c r="X5" s="71"/>
       <c r="Y5" s="22">
         <v>10.067</v>
       </c>
@@ -8960,10 +8963,10 @@
         <f>Y5/W5-1</f>
         <v>4.0335000000000001</v>
       </c>
-      <c r="AA5" s="67">
+      <c r="AA5" s="70">
         <v>2</v>
       </c>
-      <c r="AB5" s="68"/>
+      <c r="AB5" s="71"/>
       <c r="AC5" s="22">
         <v>9.9779999999999998</v>
       </c>
@@ -8971,10 +8974,10 @@
         <f>AC5/AA5-1</f>
         <v>3.9889999999999999</v>
       </c>
-      <c r="AE5" s="67">
+      <c r="AE5" s="70">
         <v>7</v>
       </c>
-      <c r="AF5" s="68"/>
+      <c r="AF5" s="71"/>
       <c r="AG5" s="22">
         <v>15.536</v>
       </c>
@@ -8982,10 +8985,10 @@
         <f>AG5/AE5-1</f>
         <v>1.2194285714285713</v>
       </c>
-      <c r="AI5" s="67">
+      <c r="AI5" s="70">
         <v>7</v>
       </c>
-      <c r="AJ5" s="68"/>
+      <c r="AJ5" s="71"/>
       <c r="AK5" s="22">
         <v>24.87</v>
       </c>
@@ -8993,10 +8996,10 @@
         <f>AK5/AI5-1</f>
         <v>2.5528571428571429</v>
       </c>
-      <c r="AM5" s="67">
+      <c r="AM5" s="70">
         <v>7</v>
       </c>
-      <c r="AN5" s="68"/>
+      <c r="AN5" s="71"/>
       <c r="AO5" s="22">
         <v>14.685</v>
       </c>
@@ -9004,10 +9007,10 @@
         <f>AO5/AM5-1</f>
         <v>1.0978571428571429</v>
       </c>
-      <c r="AQ5" s="67">
+      <c r="AQ5" s="70">
         <v>10</v>
       </c>
-      <c r="AR5" s="68"/>
+      <c r="AR5" s="71"/>
       <c r="AS5" s="22">
         <v>13.314</v>
       </c>
@@ -9015,10 +9018,10 @@
         <f>AS5/AQ5-1</f>
         <v>0.33139999999999992</v>
       </c>
-      <c r="AU5" s="67">
+      <c r="AU5" s="70">
         <v>15</v>
       </c>
-      <c r="AV5" s="68"/>
+      <c r="AV5" s="71"/>
       <c r="AW5" s="22">
         <v>35.488</v>
       </c>
@@ -9026,10 +9029,10 @@
         <f>AW5/AU5-1</f>
         <v>1.3658666666666668</v>
       </c>
-      <c r="AY5" s="67">
+      <c r="AY5" s="70">
         <v>20</v>
       </c>
-      <c r="AZ5" s="68"/>
+      <c r="AZ5" s="71"/>
       <c r="BA5" s="22">
         <v>46.418999999999997</v>
       </c>
@@ -9037,10 +9040,10 @@
         <f>BA5/AY5-1</f>
         <v>1.3209499999999998</v>
       </c>
-      <c r="BC5" s="67">
+      <c r="BC5" s="70">
         <v>20</v>
       </c>
-      <c r="BD5" s="68"/>
+      <c r="BD5" s="71"/>
       <c r="BE5" s="22">
         <v>77.132000000000005</v>
       </c>
@@ -9048,10 +9051,10 @@
         <f>BE5/BC5-1</f>
         <v>2.8566000000000003</v>
       </c>
-      <c r="BG5" s="67">
+      <c r="BG5" s="70">
         <v>20</v>
       </c>
-      <c r="BH5" s="68"/>
+      <c r="BH5" s="71"/>
       <c r="BI5" s="22">
         <v>50.906999999999996</v>
       </c>
@@ -9059,10 +9062,10 @@
         <f>BI5/BG5-1</f>
         <v>1.54535</v>
       </c>
-      <c r="BK5" s="67">
+      <c r="BK5" s="70">
         <v>30</v>
       </c>
-      <c r="BL5" s="68"/>
+      <c r="BL5" s="71"/>
       <c r="BM5" s="22">
         <v>39.054000000000002</v>
       </c>
@@ -9070,10 +9073,10 @@
         <f>BM5/BK5-1</f>
         <v>0.30180000000000007</v>
       </c>
-      <c r="BO5" s="67">
+      <c r="BO5" s="70">
         <v>30</v>
       </c>
-      <c r="BP5" s="68"/>
+      <c r="BP5" s="71"/>
       <c r="BQ5" s="22">
         <v>40.4</v>
       </c>
@@ -9086,34 +9089,34 @@
       <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="62">
+      <c r="C6" s="72">
         <v>11</v>
       </c>
-      <c r="D6" s="63"/>
+      <c r="D6" s="73"/>
       <c r="E6" s="23">
         <v>10</v>
       </c>
       <c r="F6" s="26"/>
-      <c r="G6" s="62">
+      <c r="G6" s="72">
         <v>17</v>
       </c>
-      <c r="H6" s="63"/>
+      <c r="H6" s="73"/>
       <c r="I6" s="23">
         <v>30</v>
       </c>
       <c r="J6" s="26"/>
-      <c r="K6" s="62">
+      <c r="K6" s="72">
         <v>10</v>
       </c>
-      <c r="L6" s="63"/>
+      <c r="L6" s="73"/>
       <c r="M6" s="23">
         <v>18</v>
       </c>
       <c r="N6" s="26"/>
-      <c r="O6" s="62">
+      <c r="O6" s="72">
         <v>18</v>
       </c>
-      <c r="P6" s="63"/>
+      <c r="P6" s="73"/>
       <c r="Q6" s="23">
         <v>22</v>
       </c>
@@ -9121,103 +9124,103 @@
       <c r="S6" s="75">
         <v>40</v>
       </c>
-      <c r="T6" s="63"/>
+      <c r="T6" s="73"/>
       <c r="U6" s="23">
         <v>37</v>
       </c>
       <c r="V6" s="26"/>
-      <c r="W6" s="62">
+      <c r="W6" s="72">
         <v>18</v>
       </c>
-      <c r="X6" s="63"/>
+      <c r="X6" s="73"/>
       <c r="Y6" s="23">
         <v>18</v>
       </c>
       <c r="Z6" s="26"/>
-      <c r="AA6" s="62">
+      <c r="AA6" s="72">
         <v>18</v>
       </c>
-      <c r="AB6" s="63"/>
+      <c r="AB6" s="73"/>
       <c r="AC6" s="23">
         <v>20</v>
       </c>
       <c r="AD6" s="26"/>
-      <c r="AE6" s="62">
+      <c r="AE6" s="72">
         <v>14</v>
       </c>
-      <c r="AF6" s="63"/>
+      <c r="AF6" s="73"/>
       <c r="AG6" s="23">
         <v>19</v>
       </c>
       <c r="AH6" s="26"/>
-      <c r="AI6" s="62">
+      <c r="AI6" s="72">
         <v>23</v>
       </c>
-      <c r="AJ6" s="63"/>
+      <c r="AJ6" s="73"/>
       <c r="AK6" s="23">
         <v>21</v>
       </c>
       <c r="AL6" s="26"/>
-      <c r="AM6" s="62">
+      <c r="AM6" s="72">
         <v>7</v>
       </c>
-      <c r="AN6" s="63"/>
+      <c r="AN6" s="73"/>
       <c r="AO6" s="23">
         <v>9</v>
       </c>
       <c r="AP6" s="26"/>
-      <c r="AQ6" s="62">
+      <c r="AQ6" s="72">
         <v>14</v>
       </c>
-      <c r="AR6" s="63"/>
+      <c r="AR6" s="73"/>
       <c r="AS6" s="23">
         <v>22</v>
       </c>
       <c r="AT6" s="26"/>
-      <c r="AU6" s="62">
+      <c r="AU6" s="72">
         <v>12</v>
       </c>
-      <c r="AV6" s="63"/>
+      <c r="AV6" s="73"/>
       <c r="AW6" s="23">
         <v>40</v>
       </c>
       <c r="AX6" s="26"/>
-      <c r="AY6" s="62">
+      <c r="AY6" s="72">
         <v>37</v>
       </c>
-      <c r="AZ6" s="63"/>
+      <c r="AZ6" s="73"/>
       <c r="BA6" s="23">
         <v>44</v>
       </c>
       <c r="BB6" s="26"/>
-      <c r="BC6" s="62">
+      <c r="BC6" s="72">
         <v>30</v>
       </c>
-      <c r="BD6" s="63"/>
+      <c r="BD6" s="73"/>
       <c r="BE6" s="23">
         <v>58</v>
       </c>
       <c r="BF6" s="26"/>
-      <c r="BG6" s="62">
+      <c r="BG6" s="72">
         <v>23</v>
       </c>
-      <c r="BH6" s="63"/>
+      <c r="BH6" s="73"/>
       <c r="BI6" s="23">
         <v>47</v>
       </c>
       <c r="BJ6" s="26"/>
-      <c r="BK6" s="62">
+      <c r="BK6" s="72">
         <v>37</v>
       </c>
-      <c r="BL6" s="63"/>
+      <c r="BL6" s="73"/>
       <c r="BM6" s="23">
         <v>40</v>
       </c>
       <c r="BN6" s="26"/>
-      <c r="BO6" s="62">
+      <c r="BO6" s="72">
         <v>36</v>
       </c>
-      <c r="BP6" s="63"/>
+      <c r="BP6" s="73"/>
       <c r="BQ6" s="23">
         <v>23</v>
       </c>
@@ -9227,104 +9230,104 @@
       <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="23">
         <v>18</v>
       </c>
       <c r="F7" s="26"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="63"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="73"/>
       <c r="I7" s="23">
         <v>30</v>
       </c>
       <c r="J7" s="26"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="63"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="73"/>
       <c r="M7" s="23">
         <v>32</v>
       </c>
       <c r="N7" s="26"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="63"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="73"/>
       <c r="Q7" s="23">
         <v>18</v>
       </c>
       <c r="R7" s="26"/>
       <c r="S7" s="75"/>
-      <c r="T7" s="63"/>
+      <c r="T7" s="73"/>
       <c r="U7" s="23">
         <v>22</v>
       </c>
       <c r="V7" s="26"/>
-      <c r="W7" s="62"/>
-      <c r="X7" s="63"/>
+      <c r="W7" s="72"/>
+      <c r="X7" s="73"/>
       <c r="Y7" s="23">
         <v>22</v>
       </c>
       <c r="Z7" s="26"/>
-      <c r="AA7" s="62"/>
-      <c r="AB7" s="63"/>
+      <c r="AA7" s="72"/>
+      <c r="AB7" s="73"/>
       <c r="AC7" s="23">
         <v>10</v>
       </c>
       <c r="AD7" s="26"/>
-      <c r="AE7" s="62"/>
-      <c r="AF7" s="63"/>
+      <c r="AE7" s="72"/>
+      <c r="AF7" s="73"/>
       <c r="AG7" s="23">
         <v>43</v>
       </c>
       <c r="AH7" s="26"/>
-      <c r="AI7" s="62"/>
-      <c r="AJ7" s="63"/>
+      <c r="AI7" s="72"/>
+      <c r="AJ7" s="73"/>
       <c r="AK7" s="23">
         <v>27</v>
       </c>
       <c r="AL7" s="26"/>
-      <c r="AM7" s="62"/>
-      <c r="AN7" s="63"/>
+      <c r="AM7" s="72"/>
+      <c r="AN7" s="73"/>
       <c r="AO7" s="23">
         <v>6</v>
       </c>
       <c r="AP7" s="26"/>
-      <c r="AQ7" s="62"/>
-      <c r="AR7" s="63"/>
+      <c r="AQ7" s="72"/>
+      <c r="AR7" s="73"/>
       <c r="AS7" s="23">
         <v>15</v>
       </c>
       <c r="AT7" s="26"/>
-      <c r="AU7" s="62"/>
-      <c r="AV7" s="63"/>
+      <c r="AU7" s="72"/>
+      <c r="AV7" s="73"/>
       <c r="AW7" s="23">
         <v>25</v>
       </c>
       <c r="AX7" s="26"/>
-      <c r="AY7" s="62"/>
-      <c r="AZ7" s="63"/>
+      <c r="AY7" s="72"/>
+      <c r="AZ7" s="73"/>
       <c r="BA7" s="23">
         <v>18</v>
       </c>
       <c r="BB7" s="26"/>
-      <c r="BC7" s="62"/>
-      <c r="BD7" s="63"/>
+      <c r="BC7" s="72"/>
+      <c r="BD7" s="73"/>
       <c r="BE7" s="23">
         <v>26</v>
       </c>
       <c r="BF7" s="26"/>
-      <c r="BG7" s="62"/>
-      <c r="BH7" s="63"/>
+      <c r="BG7" s="72"/>
+      <c r="BH7" s="73"/>
       <c r="BI7" s="23">
         <v>36</v>
       </c>
       <c r="BJ7" s="26"/>
-      <c r="BK7" s="62"/>
-      <c r="BL7" s="63"/>
+      <c r="BK7" s="72"/>
+      <c r="BL7" s="73"/>
       <c r="BM7" s="23">
         <v>23</v>
       </c>
       <c r="BN7" s="26"/>
-      <c r="BO7" s="62"/>
-      <c r="BP7" s="63"/>
+      <c r="BO7" s="72"/>
+      <c r="BP7" s="73"/>
       <c r="BQ7" s="23">
         <v>33</v>
       </c>
@@ -9334,11 +9337,11 @@
       <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="69">
+      <c r="C8" s="62">
         <f>C6</f>
         <v>11</v>
       </c>
-      <c r="D8" s="70"/>
+      <c r="D8" s="63"/>
       <c r="E8" s="24">
         <f>(E6+E7)/2</f>
         <v>14</v>
@@ -9347,11 +9350,11 @@
         <f>E8/C8-1</f>
         <v>0.27272727272727271</v>
       </c>
-      <c r="G8" s="69">
+      <c r="G8" s="62">
         <f>G6</f>
         <v>17</v>
       </c>
-      <c r="H8" s="70"/>
+      <c r="H8" s="63"/>
       <c r="I8" s="24">
         <f>(I6+I7)/2</f>
         <v>30</v>
@@ -9360,11 +9363,11 @@
         <f>I8/G8-1</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="K8" s="69">
+      <c r="K8" s="62">
         <f>K6</f>
         <v>10</v>
       </c>
-      <c r="L8" s="70"/>
+      <c r="L8" s="63"/>
       <c r="M8" s="24">
         <f>(M6+M7)/2</f>
         <v>25</v>
@@ -9373,11 +9376,11 @@
         <f>M8/K8-1</f>
         <v>1.5</v>
       </c>
-      <c r="O8" s="69">
+      <c r="O8" s="62">
         <f>O6</f>
         <v>18</v>
       </c>
-      <c r="P8" s="70"/>
+      <c r="P8" s="63"/>
       <c r="Q8" s="24">
         <f>(Q6+Q7)/2</f>
         <v>20</v>
@@ -9390,7 +9393,7 @@
         <f>S6</f>
         <v>40</v>
       </c>
-      <c r="T8" s="70"/>
+      <c r="T8" s="63"/>
       <c r="U8" s="24">
         <f>(U6+U7)/2</f>
         <v>29.5</v>
@@ -9399,11 +9402,11 @@
         <f>U8/S8-1</f>
         <v>-0.26249999999999996</v>
       </c>
-      <c r="W8" s="69">
+      <c r="W8" s="62">
         <f>W6</f>
         <v>18</v>
       </c>
-      <c r="X8" s="70"/>
+      <c r="X8" s="63"/>
       <c r="Y8" s="24">
         <f>(Y6+Y7)/2</f>
         <v>20</v>
@@ -9412,11 +9415,11 @@
         <f>Y8/W8-1</f>
         <v>0.11111111111111116</v>
       </c>
-      <c r="AA8" s="69">
+      <c r="AA8" s="62">
         <f>AA6</f>
         <v>18</v>
       </c>
-      <c r="AB8" s="70"/>
+      <c r="AB8" s="63"/>
       <c r="AC8" s="24">
         <f>(AC6+AC7)/2</f>
         <v>15</v>
@@ -9425,11 +9428,11 @@
         <f>AC8/AA8-1</f>
         <v>-0.16666666666666663</v>
       </c>
-      <c r="AE8" s="69">
+      <c r="AE8" s="62">
         <f>AE6</f>
         <v>14</v>
       </c>
-      <c r="AF8" s="70"/>
+      <c r="AF8" s="63"/>
       <c r="AG8" s="24">
         <f>(AG6+AG7)/2</f>
         <v>31</v>
@@ -9438,11 +9441,11 @@
         <f>AG8/AE8-1</f>
         <v>1.2142857142857144</v>
       </c>
-      <c r="AI8" s="69">
+      <c r="AI8" s="62">
         <f>AI6</f>
         <v>23</v>
       </c>
-      <c r="AJ8" s="70"/>
+      <c r="AJ8" s="63"/>
       <c r="AK8" s="24">
         <f>(AK6+AK7)/2</f>
         <v>24</v>
@@ -9451,11 +9454,11 @@
         <f>AK8/AI8-1</f>
         <v>4.3478260869565188E-2</v>
       </c>
-      <c r="AM8" s="69">
+      <c r="AM8" s="62">
         <f>AM6</f>
         <v>7</v>
       </c>
-      <c r="AN8" s="70"/>
+      <c r="AN8" s="63"/>
       <c r="AO8" s="24">
         <f>(AO6+AO7)/2</f>
         <v>7.5</v>
@@ -9464,11 +9467,11 @@
         <f>AO8/AM8-1</f>
         <v>7.1428571428571397E-2</v>
       </c>
-      <c r="AQ8" s="69">
+      <c r="AQ8" s="62">
         <f>AQ6</f>
         <v>14</v>
       </c>
-      <c r="AR8" s="70"/>
+      <c r="AR8" s="63"/>
       <c r="AS8" s="24">
         <f>(AS6+AS7)/2</f>
         <v>18.5</v>
@@ -9477,11 +9480,11 @@
         <f>AS8/AQ8-1</f>
         <v>0.3214285714285714</v>
       </c>
-      <c r="AU8" s="69">
+      <c r="AU8" s="62">
         <f>AU6</f>
         <v>12</v>
       </c>
-      <c r="AV8" s="70"/>
+      <c r="AV8" s="63"/>
       <c r="AW8" s="24">
         <f>(AW6+AW7)/2</f>
         <v>32.5</v>
@@ -9490,11 +9493,11 @@
         <f>AW8/AU8-1</f>
         <v>1.7083333333333335</v>
       </c>
-      <c r="AY8" s="69">
+      <c r="AY8" s="62">
         <f>AY6</f>
         <v>37</v>
       </c>
-      <c r="AZ8" s="70"/>
+      <c r="AZ8" s="63"/>
       <c r="BA8" s="24">
         <f>(BA6+BA7)/2</f>
         <v>31</v>
@@ -9503,11 +9506,11 @@
         <f>BA8/AY8-1</f>
         <v>-0.16216216216216217</v>
       </c>
-      <c r="BC8" s="69">
+      <c r="BC8" s="62">
         <f>BC6</f>
         <v>30</v>
       </c>
-      <c r="BD8" s="70"/>
+      <c r="BD8" s="63"/>
       <c r="BE8" s="24">
         <f>(BE6+BE7)/2</f>
         <v>42</v>
@@ -9516,11 +9519,11 @@
         <f>BE8/BC8-1</f>
         <v>0.39999999999999991</v>
       </c>
-      <c r="BG8" s="69">
+      <c r="BG8" s="62">
         <f>BG6</f>
         <v>23</v>
       </c>
-      <c r="BH8" s="70"/>
+      <c r="BH8" s="63"/>
       <c r="BI8" s="24">
         <f>(BI6+BI7)/2</f>
         <v>41.5</v>
@@ -9529,11 +9532,11 @@
         <f>BI8/BG8-1</f>
         <v>0.80434782608695654</v>
       </c>
-      <c r="BK8" s="69">
+      <c r="BK8" s="62">
         <f>BK6</f>
         <v>37</v>
       </c>
-      <c r="BL8" s="70"/>
+      <c r="BL8" s="63"/>
       <c r="BM8" s="24">
         <f>(BM6+BM7)/2</f>
         <v>31.5</v>
@@ -9542,11 +9545,11 @@
         <f>BM8/BK8-1</f>
         <v>-0.14864864864864868</v>
       </c>
-      <c r="BO8" s="69">
+      <c r="BO8" s="62">
         <f>BO6</f>
         <v>36</v>
       </c>
-      <c r="BP8" s="70"/>
+      <c r="BP8" s="63"/>
       <c r="BQ8" s="24">
         <f>(BQ6+BQ7)/2</f>
         <v>28</v>
@@ -12530,15 +12533,92 @@
     </row>
   </sheetData>
   <mergeCells count="119">
-    <mergeCell ref="BC8:BD8"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="BO7:BP7"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AU7:AV7"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="BE3:BF3"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BC7:BD7"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="AY7:AZ7"/>
+    <mergeCell ref="BK8:BL8"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AQ3:AR3"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AI7:AJ7"/>
+    <mergeCell ref="AU2:AX2"/>
+    <mergeCell ref="AY8:AZ8"/>
+    <mergeCell ref="BG8:BH8"/>
+    <mergeCell ref="BG2:BJ2"/>
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BI3:BJ3"/>
+    <mergeCell ref="BG5:BH5"/>
+    <mergeCell ref="BG6:BH6"/>
+    <mergeCell ref="BG7:BH7"/>
+    <mergeCell ref="AU8:AV8"/>
+    <mergeCell ref="AI8:AJ8"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="BO8:BP8"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="BO2:BR2"/>
+    <mergeCell ref="BO3:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="AY2:BB2"/>
+    <mergeCell ref="AY3:AZ3"/>
+    <mergeCell ref="BA3:BB3"/>
+    <mergeCell ref="BK2:BN2"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="BM3:BN3"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BK7:BL7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="G5:H5"/>
@@ -12563,92 +12643,15 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="W8:X8"/>
     <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="BO8:BP8"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="BO2:BR2"/>
-    <mergeCell ref="BO3:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BO5:BP5"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="AY2:BB2"/>
-    <mergeCell ref="AY3:AZ3"/>
-    <mergeCell ref="BA3:BB3"/>
-    <mergeCell ref="BK2:BN2"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="BM3:BN3"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BK7:BL7"/>
-    <mergeCell ref="BK8:BL8"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AQ3:AR3"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AI7:AJ7"/>
-    <mergeCell ref="AU2:AX2"/>
-    <mergeCell ref="AY8:AZ8"/>
-    <mergeCell ref="BG8:BH8"/>
-    <mergeCell ref="BG2:BJ2"/>
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BI3:BJ3"/>
-    <mergeCell ref="BG5:BH5"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="BG7:BH7"/>
-    <mergeCell ref="AU8:AV8"/>
-    <mergeCell ref="AI8:AJ8"/>
-    <mergeCell ref="AS3:AT3"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="BO7:BP7"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AW3:AX3"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AU7:AV7"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="BE3:BF3"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BC7:BD7"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="AY7:AZ7"/>
+    <mergeCell ref="BC8:BD8"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="BC2:BF2"/>
   </mergeCells>
   <conditionalFormatting sqref="BP21">
     <cfRule type="cellIs" dxfId="63" priority="103" operator="lessThan">
@@ -13095,13 +13098,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4D9EFE-8FC7-4B01-807E-922034333148}">
-  <dimension ref="B1:AN188"/>
+  <dimension ref="B1:AN189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="15" topLeftCell="C98" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="15" topLeftCell="C138" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="B105" sqref="B105"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13195,6 +13198,13 @@
       <c r="K5" s="39" t="s">
         <v>499</v>
       </c>
+      <c r="N5" s="39">
+        <v>2</v>
+      </c>
+      <c r="O5" s="39">
+        <f>N5*J7</f>
+        <v>4.9035689664929496</v>
+      </c>
       <c r="T5" s="44"/>
       <c r="U5" s="44"/>
       <c r="V5" s="44"/>
@@ -13226,6 +13236,13 @@
       <c r="K6" s="39" t="s">
         <v>500</v>
       </c>
+      <c r="N6" s="39">
+        <v>4</v>
+      </c>
+      <c r="O6" s="39">
+        <f>N6*J6</f>
+        <v>6.4747880254911108</v>
+      </c>
       <c r="T6" s="44"/>
       <c r="U6" s="44"/>
       <c r="V6" s="44"/>
@@ -13235,6 +13252,13 @@
       <c r="Z6" s="44"/>
       <c r="AA6" s="44"/>
       <c r="AB6" s="57"/>
+      <c r="AK6" s="39">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="39">
+        <f>AK6*2.5</f>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="7" spans="2:40" s="39" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="43">
@@ -13255,6 +13279,10 @@
       </c>
       <c r="K7" s="39" t="s">
         <v>501</v>
+      </c>
+      <c r="O7" s="39">
+        <f>O5+O6</f>
+        <v>11.378356991984059</v>
       </c>
       <c r="T7" s="58"/>
       <c r="U7" s="58"/>
@@ -13265,6 +13293,13 @@
       <c r="Z7" s="44"/>
       <c r="AA7" s="44"/>
       <c r="AB7" s="57"/>
+      <c r="AK7" s="39">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="39">
+        <f>AK7*1.6</f>
+        <v>1.6</v>
+      </c>
     </row>
     <row r="8" spans="2:40" s="39" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="42">
@@ -13290,6 +13325,10 @@
       <c r="Z8" s="44"/>
       <c r="AA8" s="44"/>
       <c r="AB8" s="44"/>
+      <c r="AL8" s="39">
+        <f>AL6+AL7</f>
+        <v>4.0999999999999996</v>
+      </c>
     </row>
     <row r="9" spans="2:40" s="39" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" s="45">
@@ -15322,7 +15361,7 @@
       </c>
     </row>
     <row r="28" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="60" t="s">
         <v>79</v>
       </c>
       <c r="C28" s="35">
@@ -26487,7 +26526,7 @@
       </c>
     </row>
     <row r="105" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B105" s="35" t="s">
+      <c r="B105" s="60" t="s">
         <v>257</v>
       </c>
       <c r="C105" s="35">
@@ -31562,7 +31601,7 @@
       </c>
     </row>
     <row r="140" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B140" s="35" t="s">
+      <c r="B140" s="60" t="s">
         <v>339</v>
       </c>
       <c r="C140" s="35">
@@ -32446,60 +32485,60 @@
         <v>3040143002.0130162</v>
       </c>
       <c r="F146" s="34">
-        <f t="shared" ref="F146:F188" si="85">ROUND(E146/$C$6,0)</f>
+        <f t="shared" ref="F146:F189" si="85">ROUND(E146/$C$6,0)</f>
         <v>1</v>
       </c>
       <c r="G146" s="34">
-        <f t="shared" ref="G146:G188" si="86">F146*$C$6*$C$8</f>
+        <f t="shared" ref="G146:G189" si="86">F146*$C$6*$C$8</f>
         <v>14096578622.930536</v>
       </c>
       <c r="H146" s="34">
-        <f t="shared" ref="H146:H188" si="87">C146-G146</f>
+        <f t="shared" ref="H146:H189" si="87">C146-G146</f>
         <v>155841897555.6507</v>
       </c>
       <c r="I146" s="37">
         <v>54.027488592566343</v>
       </c>
       <c r="J146" s="39">
-        <f t="shared" ref="J146:J188" si="88">I146/(I146+L146)*H146*$F$7</f>
+        <f t="shared" ref="J146:J189" si="88">I146/(I146+L146)*H146*$F$7</f>
         <v>76025601024.445969</v>
       </c>
       <c r="K146" s="39">
-        <f t="shared" ref="K146:K188" si="89">ROUND(J146/$F$9,0)</f>
+        <f t="shared" ref="K146:K189" si="89">ROUND(J146/$F$9,0)</f>
         <v>2</v>
       </c>
       <c r="L146" s="39">
         <v>29.034133699552562</v>
       </c>
       <c r="M146" s="39">
-        <f t="shared" ref="M146:M188" si="90">L146/(I146+L146)*H146*(2-$F$7)</f>
+        <f t="shared" ref="M146:M189" si="90">L146/(I146+L146)*H146*(2-$F$7)</f>
         <v>68093036903.820114</v>
       </c>
       <c r="N146" s="39">
-        <f t="shared" ref="N146:N188" si="91">ROUND(M146/$F$8,0)</f>
+        <f t="shared" ref="N146:N189" si="91">ROUND(M146/$F$8,0)</f>
         <v>3</v>
       </c>
       <c r="O146" s="49">
-        <f t="shared" ref="O146:O188" si="92">F146</f>
+        <f t="shared" ref="O146:O189" si="92">F146</f>
         <v>1</v>
       </c>
       <c r="P146" s="50">
-        <f t="shared" ref="P146:P188" si="93">N146</f>
+        <f t="shared" ref="P146:P189" si="93">N146</f>
         <v>3</v>
       </c>
       <c r="Q146" s="50">
-        <f t="shared" ref="Q146:Q188" si="94">K146</f>
+        <f t="shared" ref="Q146:Q189" si="94">K146</f>
         <v>2</v>
       </c>
       <c r="R146" s="51">
-        <f t="shared" ref="R146:R188" si="95">O146+P146+Q146</f>
+        <f t="shared" ref="R146:R189" si="95">O146+P146+Q146</f>
         <v>6</v>
       </c>
       <c r="T146" s="39">
         <v>393259049121.62598</v>
       </c>
       <c r="U146" s="39">
-        <f t="shared" ref="U146:U188" si="96">(T146-C146)*$U$11+C146</f>
+        <f t="shared" ref="U146:U189" si="96">(T146-C146)*$U$11+C146</f>
         <v>260450304392.39728</v>
       </c>
       <c r="V146" s="35">
@@ -32510,11 +32549,11 @@
         <v>3245100890.1077366</v>
       </c>
       <c r="X146" s="34">
-        <f t="shared" ref="X146:X188" si="97">ROUND(W146/$C$6,0)</f>
+        <f t="shared" ref="X146:X189" si="97">ROUND(W146/$C$6,0)</f>
         <v>1</v>
       </c>
       <c r="Y146" s="34">
-        <f t="shared" ref="Y146:Y188" si="98">X146*$C$6*$C$8</f>
+        <f t="shared" ref="Y146:Y189" si="98">X146*$C$6*$C$8</f>
         <v>14096578622.930536</v>
       </c>
       <c r="Z146" s="34">
@@ -32525,54 +32564,54 @@
         <v>53.928333156489416</v>
       </c>
       <c r="AB146" s="39">
-        <f t="shared" ref="AB146:AB188" si="99">AA146/(AA146+AD146)*Z146*$F$7</f>
+        <f t="shared" ref="AB146:AB189" si="99">AA146/(AA146+AD146)*Z146*$F$7</f>
         <v>116913370864.92297</v>
       </c>
       <c r="AC146" s="39">
-        <f t="shared" ref="AC146:AC188" si="100">ROUND(AB146/$F$9,0)</f>
+        <f t="shared" ref="AC146:AC189" si="100">ROUND(AB146/$F$9,0)</f>
         <v>3</v>
       </c>
       <c r="AD146" s="39">
         <v>31.29788412314732</v>
       </c>
       <c r="AE146" s="39">
-        <f t="shared" ref="AE146:AE188" si="101">AD146/(AA146+AD146)*Z146*(2-$F$7)</f>
+        <f t="shared" ref="AE146:AE189" si="101">AD146/(AA146+AD146)*Z146*(2-$F$7)</f>
         <v>113086539103.62848</v>
       </c>
       <c r="AF146" s="39">
-        <f t="shared" ref="AF146:AF188" si="102">ROUND(AE146/$F$8,0)</f>
+        <f t="shared" ref="AF146:AF189" si="102">ROUND(AE146/$F$8,0)</f>
         <v>5</v>
       </c>
       <c r="AG146" s="49">
-        <f t="shared" ref="AG146:AG188" si="103">X146</f>
+        <f t="shared" ref="AG146:AG189" si="103">X146</f>
         <v>1</v>
       </c>
       <c r="AH146" s="50">
-        <f t="shared" ref="AH146:AH188" si="104">AF146</f>
+        <f t="shared" ref="AH146:AH189" si="104">AF146</f>
         <v>5</v>
       </c>
       <c r="AI146" s="50">
-        <f t="shared" ref="AI146:AI188" si="105">AC146</f>
+        <f t="shared" ref="AI146:AI189" si="105">AC146</f>
         <v>3</v>
       </c>
       <c r="AJ146" s="51">
-        <f t="shared" ref="AJ146:AJ188" si="106">AG146+AH146+AI146</f>
+        <f t="shared" ref="AJ146:AJ189" si="106">AG146+AH146+AI146</f>
         <v>9</v>
       </c>
       <c r="AK146" s="49">
-        <f t="shared" ref="AK146:AK188" si="107">AG146-O146</f>
+        <f t="shared" ref="AK146:AK189" si="107">AG146-O146</f>
         <v>0</v>
       </c>
       <c r="AL146" s="50">
-        <f t="shared" ref="AL146:AL188" si="108">AH146-P146</f>
+        <f t="shared" ref="AL146:AL189" si="108">AH146-P146</f>
         <v>2</v>
       </c>
       <c r="AM146" s="50">
-        <f t="shared" ref="AM146:AM188" si="109">AI146-Q146</f>
+        <f t="shared" ref="AM146:AM189" si="109">AI146-Q146</f>
         <v>1</v>
       </c>
       <c r="AN146" s="51">
-        <f t="shared" ref="AN146:AN188" si="110">AJ146-R146</f>
+        <f t="shared" ref="AN146:AN189" si="110">AJ146-R146</f>
         <v>3</v>
       </c>
     </row>
@@ -33012,7 +33051,7 @@
       </c>
     </row>
     <row r="150" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B150" s="35" t="s">
+      <c r="B150" s="60" t="s">
         <v>361</v>
       </c>
       <c r="C150" s="35">
@@ -33737,7 +33776,7 @@
       </c>
     </row>
     <row r="155" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B155" s="35" t="s">
+      <c r="B155" s="60" t="s">
         <v>26</v>
       </c>
       <c r="C155" s="35">
@@ -36498,7 +36537,7 @@
         <v>0.85501148400089511</v>
       </c>
       <c r="E174" s="35">
-        <f t="shared" ref="E174:E188" si="139">D174/100*C174</f>
+        <f t="shared" ref="E174:E189" si="139">D174/100*C174</f>
         <v>17605314.763955552</v>
       </c>
       <c r="F174" s="34">
@@ -37142,7 +37181,7 @@
         <v>2.0652596724157299</v>
       </c>
       <c r="W178" s="35">
-        <f t="shared" ref="W178:W188" si="140">V178/100*U178</f>
+        <f t="shared" ref="W178:W189" si="140">V178/100*U178</f>
         <v>31039471752.397705</v>
       </c>
       <c r="X178" s="34">
@@ -37154,7 +37193,7 @@
         <v>197352100721.0275</v>
       </c>
       <c r="Z178" s="34">
-        <f t="shared" ref="Z178:Z188" si="141">U178-Y178</f>
+        <f t="shared" ref="Z178:Z189" si="141">U178-Y178</f>
         <v>1305581025169.6697</v>
       </c>
       <c r="AA178" s="37">
@@ -37648,7 +37687,7 @@
       </c>
     </row>
     <row r="182" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B182" s="35" t="s">
+      <c r="B182" s="60" t="s">
         <v>446</v>
       </c>
       <c r="C182" s="35">
@@ -38372,292 +38411,433 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B187" s="35" t="s">
+    <row r="187" spans="2:40" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B187" s="60" t="s">
+        <v>507</v>
+      </c>
+      <c r="C187" s="39">
+        <v>24153264424</v>
+      </c>
+      <c r="D187" s="39">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E187" s="39">
+        <f t="shared" ref="E187" si="142">D187/100*C187</f>
+        <v>1183509956.776</v>
+      </c>
+      <c r="F187" s="34">
+        <f t="shared" ref="F187" si="143">ROUND(E187/$C$6,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G187" s="34">
+        <f t="shared" ref="G187" si="144">F187*$C$6*$C$8</f>
+        <v>14096578622.930536</v>
+      </c>
+      <c r="H187" s="34">
+        <f t="shared" ref="H187" si="145">C187-G187</f>
+        <v>10056685801.069464</v>
+      </c>
+      <c r="I187" s="39">
+        <v>31</v>
+      </c>
+      <c r="J187" s="39">
+        <f t="shared" ref="J187" si="146">I187/(I187+L187)*H187*$F$7</f>
+        <v>3036596686.6865592</v>
+      </c>
+      <c r="K187" s="39">
+        <f t="shared" ref="K187" si="147">ROUND(J187/$F$9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L187" s="39">
+        <v>46</v>
+      </c>
+      <c r="M187" s="39">
+        <f t="shared" ref="M187" si="148">L187/(I187+L187)*H187*(2-$F$7)</f>
+        <v>7509862773.525898</v>
+      </c>
+      <c r="N187" s="39">
+        <f t="shared" ref="N187" si="149">ROUND(M187/$F$8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O187" s="49">
+        <f t="shared" ref="O187" si="150">F187</f>
+        <v>1</v>
+      </c>
+      <c r="P187" s="50">
+        <f t="shared" ref="P187" si="151">N187</f>
+        <v>0</v>
+      </c>
+      <c r="Q187" s="50">
+        <f t="shared" ref="Q187" si="152">K187</f>
+        <v>0</v>
+      </c>
+      <c r="R187" s="51">
+        <f t="shared" ref="R187" si="153">O187+P187+Q187</f>
+        <v>1</v>
+      </c>
+      <c r="U187" s="39">
+        <v>66914452000</v>
+      </c>
+      <c r="V187" s="39">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="W187" s="39">
+        <f t="shared" ref="W187" si="154">V187/100*U187</f>
+        <v>3278808148</v>
+      </c>
+      <c r="X187" s="34">
+        <f t="shared" ref="X187" si="155">ROUND(W187/$C$6,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y187" s="34">
+        <f t="shared" ref="Y187" si="156">X187*$C$6*$C$8</f>
+        <v>14096578622.930536</v>
+      </c>
+      <c r="Z187" s="34">
+        <f t="shared" ref="Z187" si="157">U187-Y187</f>
+        <v>52817873377.069466</v>
+      </c>
+      <c r="AA187" s="39">
+        <v>19</v>
+      </c>
+      <c r="AB187" s="39">
+        <f t="shared" ref="AB187" si="158">AA187/(AA187+AD187)*Z187*$F$7</f>
+        <v>12338601567.594097</v>
+      </c>
+      <c r="AC187" s="39">
+        <f t="shared" ref="AC187" si="159">ROUND(AB187/$F$9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD187" s="39">
+        <v>42</v>
+      </c>
+      <c r="AE187" s="39">
+        <f t="shared" ref="AE187" si="160">AD187/(AA187+AD187)*Z187*(2-$F$7)</f>
+        <v>45458005775.346672</v>
+      </c>
+      <c r="AF187" s="39">
+        <f t="shared" ref="AF187" si="161">ROUND(AE187/$F$8,0)</f>
+        <v>2</v>
+      </c>
+      <c r="AG187" s="49">
+        <f t="shared" ref="AG187" si="162">X187</f>
+        <v>1</v>
+      </c>
+      <c r="AH187" s="50">
+        <f t="shared" ref="AH187" si="163">AF187</f>
+        <v>2</v>
+      </c>
+      <c r="AI187" s="50">
+        <f t="shared" ref="AI187" si="164">AC187</f>
+        <v>0</v>
+      </c>
+      <c r="AJ187" s="51">
+        <f t="shared" ref="AJ187" si="165">AG187+AH187+AI187</f>
+        <v>3</v>
+      </c>
+      <c r="AK187" s="49">
+        <f t="shared" ref="AK187" si="166">AG187-O187</f>
+        <v>0</v>
+      </c>
+      <c r="AL187" s="50">
+        <f t="shared" ref="AL187" si="167">AH187-P187</f>
+        <v>2</v>
+      </c>
+      <c r="AM187" s="50">
+        <f t="shared" ref="AM187" si="168">AI187-Q187</f>
+        <v>0</v>
+      </c>
+      <c r="AN187" s="51">
+        <f t="shared" ref="AN187" si="169">AJ187-R187</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B188" s="35" t="s">
         <v>467</v>
       </c>
-      <c r="C187" s="35">
+      <c r="C188" s="35">
         <v>20736671783.489033</v>
       </c>
-      <c r="D187" s="39">
+      <c r="D188" s="39">
         <v>1.3095961053559599</v>
       </c>
-      <c r="E187" s="35">
+      <c r="E188" s="35">
         <f t="shared" si="139"/>
         <v>271566646.05702066</v>
       </c>
-      <c r="F187" s="34">
+      <c r="F188" s="34">
         <f t="shared" si="85"/>
         <v>0</v>
       </c>
-      <c r="G187" s="34">
+      <c r="G188" s="34">
         <f t="shared" si="86"/>
         <v>0</v>
       </c>
-      <c r="H187" s="34">
+      <c r="H188" s="34">
         <f t="shared" si="87"/>
         <v>20736671783.489033</v>
       </c>
-      <c r="I187" s="37">
+      <c r="I188" s="37">
         <v>48.959533523278196</v>
       </c>
-      <c r="J187" s="39">
+      <c r="J188" s="39">
         <f t="shared" si="88"/>
         <v>10545805891.685978</v>
       </c>
-      <c r="K187" s="39">
+      <c r="K188" s="39">
         <f t="shared" si="89"/>
         <v>0</v>
       </c>
-      <c r="L187" s="39">
+      <c r="L188" s="39">
         <v>23.243894154924387</v>
       </c>
-      <c r="M187" s="39">
+      <c r="M188" s="39">
         <f t="shared" si="90"/>
         <v>8344496576.5513248</v>
       </c>
-      <c r="N187" s="39">
+      <c r="N188" s="39">
         <f t="shared" si="91"/>
         <v>0</v>
       </c>
-      <c r="O187" s="49">
+      <c r="O188" s="49">
         <f t="shared" si="92"/>
         <v>0</v>
       </c>
-      <c r="P187" s="50">
+      <c r="P188" s="50">
         <f t="shared" si="93"/>
         <v>0</v>
       </c>
-      <c r="Q187" s="50">
+      <c r="Q188" s="50">
         <f t="shared" si="94"/>
         <v>0</v>
       </c>
-      <c r="R187" s="51">
+      <c r="R188" s="51">
         <f t="shared" si="95"/>
         <v>0</v>
       </c>
-      <c r="T187" s="39">
+      <c r="T188" s="39">
         <v>58735190955.723938</v>
       </c>
-      <c r="U187" s="39">
+      <c r="U188" s="39">
         <f t="shared" si="96"/>
         <v>36137471603.995842</v>
       </c>
-      <c r="V187" s="35">
+      <c r="V188" s="35">
         <v>1.3095961053559599</v>
       </c>
-      <c r="W187" s="35">
+      <c r="W188" s="35">
         <f t="shared" si="140"/>
         <v>473254920.70004547</v>
       </c>
-      <c r="X187" s="34">
+      <c r="X188" s="34">
         <f t="shared" si="97"/>
         <v>0</v>
       </c>
-      <c r="Y187" s="34">
+      <c r="Y188" s="34">
         <f t="shared" si="98"/>
         <v>0</v>
       </c>
-      <c r="Z187" s="34">
+      <c r="Z188" s="34">
         <f t="shared" si="141"/>
         <v>36137471603.995842</v>
       </c>
-      <c r="AA187" s="37">
+      <c r="AA188" s="37">
         <v>52.093884963370854</v>
       </c>
-      <c r="AB187" s="39">
+      <c r="AB188" s="39">
         <f t="shared" si="99"/>
         <v>15793497324.52545</v>
       </c>
-      <c r="AC187" s="39">
+      <c r="AC188" s="39">
         <f t="shared" si="100"/>
         <v>0</v>
       </c>
-      <c r="AD187" s="39">
+      <c r="AD188" s="39">
         <v>37.304044921462562</v>
       </c>
-      <c r="AE187" s="39">
+      <c r="AE188" s="39">
         <f t="shared" si="101"/>
         <v>18849343964.119057</v>
       </c>
-      <c r="AF187" s="39">
+      <c r="AF188" s="39">
         <f t="shared" si="102"/>
         <v>1</v>
       </c>
-      <c r="AG187" s="49">
+      <c r="AG188" s="49">
         <f t="shared" si="103"/>
         <v>0</v>
       </c>
-      <c r="AH187" s="50">
+      <c r="AH188" s="50">
         <f t="shared" si="104"/>
         <v>1</v>
       </c>
-      <c r="AI187" s="50">
+      <c r="AI188" s="50">
         <f t="shared" si="105"/>
         <v>0</v>
       </c>
-      <c r="AJ187" s="51">
+      <c r="AJ188" s="51">
         <f t="shared" si="106"/>
         <v>1</v>
       </c>
-      <c r="AK187" s="49">
+      <c r="AK188" s="49">
         <f t="shared" si="107"/>
         <v>0</v>
       </c>
-      <c r="AL187" s="50">
+      <c r="AL188" s="50">
         <f t="shared" si="108"/>
         <v>1</v>
       </c>
-      <c r="AM187" s="50">
+      <c r="AM188" s="50">
         <f t="shared" si="109"/>
         <v>0</v>
       </c>
-      <c r="AN187" s="51">
+      <c r="AN188" s="51">
         <f t="shared" si="110"/>
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B188" s="35" t="s">
+    <row r="189" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B189" s="35" t="s">
         <v>469</v>
       </c>
-      <c r="C188" s="35">
+      <c r="C189" s="35">
         <v>41269476289.344582</v>
       </c>
-      <c r="D188" s="35">
+      <c r="D189" s="35">
         <v>3.4163479325265604</v>
       </c>
-      <c r="E188" s="35">
+      <c r="E189" s="35">
         <f t="shared" si="139"/>
         <v>1409908899.9755626</v>
       </c>
-      <c r="F188" s="34">
+      <c r="F189" s="34">
         <f t="shared" si="85"/>
         <v>1</v>
       </c>
-      <c r="G188" s="34">
+      <c r="G189" s="34">
         <f t="shared" si="86"/>
         <v>14096578622.930536</v>
       </c>
-      <c r="H188" s="34">
+      <c r="H189" s="34">
         <f t="shared" si="87"/>
         <v>27172897666.414047</v>
       </c>
-      <c r="I188" s="37">
+      <c r="I189" s="37">
         <v>70.125341302611545</v>
       </c>
-      <c r="J188" s="39">
+      <c r="J189" s="39">
         <f t="shared" si="88"/>
         <v>15613746641.292751</v>
       </c>
-      <c r="K188" s="39">
+      <c r="K189" s="39">
         <f t="shared" si="89"/>
         <v>0</v>
       </c>
-      <c r="L188" s="39">
+      <c r="L189" s="39">
         <v>21.404998923297256</v>
       </c>
-      <c r="M188" s="39">
+      <c r="M189" s="39">
         <f t="shared" si="90"/>
         <v>7943211014.1963062</v>
       </c>
-      <c r="N188" s="39">
+      <c r="N189" s="39">
         <f t="shared" si="91"/>
         <v>0</v>
       </c>
-      <c r="O188" s="52">
+      <c r="O189" s="52">
         <f t="shared" si="92"/>
         <v>1</v>
       </c>
-      <c r="P188" s="53">
+      <c r="P189" s="53">
         <f t="shared" si="93"/>
         <v>0</v>
       </c>
-      <c r="Q188" s="53">
+      <c r="Q189" s="53">
         <f t="shared" si="94"/>
         <v>0</v>
       </c>
-      <c r="R188" s="54">
+      <c r="R189" s="54">
         <f t="shared" si="95"/>
         <v>1</v>
       </c>
-      <c r="T188" s="39">
+      <c r="T189" s="39">
         <v>43112365756.24472</v>
       </c>
-      <c r="U188" s="39">
+      <c r="U189" s="39">
         <f t="shared" si="96"/>
         <v>42016399390.279205</v>
       </c>
-      <c r="V188" s="35">
+      <c r="V189" s="35">
         <v>1.5449480513588301</v>
       </c>
-      <c r="W188" s="35">
+      <c r="W189" s="35">
         <f t="shared" si="140"/>
         <v>649131543.63126194</v>
       </c>
-      <c r="X188" s="34">
+      <c r="X189" s="34">
         <f t="shared" si="97"/>
         <v>0</v>
       </c>
-      <c r="Y188" s="34">
+      <c r="Y189" s="34">
         <f t="shared" si="98"/>
         <v>0</v>
       </c>
-      <c r="Z188" s="34">
+      <c r="Z189" s="34">
         <f t="shared" si="141"/>
         <v>42016399390.279205</v>
       </c>
-      <c r="AA188" s="37">
+      <c r="AA189" s="37">
         <v>60.591645107015424</v>
       </c>
-      <c r="AB188" s="39">
+      <c r="AB189" s="39">
         <f t="shared" si="99"/>
         <v>23286100217.613159</v>
       </c>
-      <c r="AC188" s="39">
+      <c r="AC189" s="39">
         <f t="shared" si="100"/>
         <v>1</v>
       </c>
-      <c r="AD188" s="39">
+      <c r="AD189" s="39">
         <v>21.404998923297256</v>
       </c>
-      <c r="AE188" s="39">
+      <c r="AE189" s="39">
         <f t="shared" si="101"/>
         <v>13710332208.493746</v>
       </c>
-      <c r="AF188" s="39">
+      <c r="AF189" s="39">
         <f t="shared" si="102"/>
         <v>1</v>
       </c>
-      <c r="AG188" s="52">
+      <c r="AG189" s="52">
         <f t="shared" si="103"/>
         <v>0</v>
       </c>
-      <c r="AH188" s="53">
+      <c r="AH189" s="53">
         <f t="shared" si="104"/>
         <v>1</v>
       </c>
-      <c r="AI188" s="53">
+      <c r="AI189" s="53">
         <f t="shared" si="105"/>
         <v>1</v>
       </c>
-      <c r="AJ188" s="54">
+      <c r="AJ189" s="54">
         <f t="shared" si="106"/>
         <v>2</v>
       </c>
-      <c r="AK188" s="52">
+      <c r="AK189" s="52">
         <f t="shared" si="107"/>
         <v>-1</v>
       </c>
-      <c r="AL188" s="53">
+      <c r="AL189" s="53">
         <f t="shared" si="108"/>
         <v>1</v>
       </c>
-      <c r="AM188" s="53">
+      <c r="AM189" s="53">
         <f t="shared" si="109"/>
         <v>1</v>
       </c>
-      <c r="AN188" s="54">
+      <c r="AN189" s="54">
         <f t="shared" si="110"/>
         <v>1</v>
       </c>
@@ -38676,8 +38856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A9ED62-1A49-45D7-8157-2940EBDC52F1}">
   <dimension ref="A1:AA218"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="I181" workbookViewId="0">
+      <selection activeCell="AA216" sqref="AA216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Factories - South America
</commit_message>
<xml_diff>
--- a/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
+++ b/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\economy spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75F10A4-D3F7-4E4D-B193-C52A0D5B7BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D539AA9-9888-44FD-8B6B-DE0AC4540675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C93B8E2A-6318-41E2-B454-20DC41C43396}"/>
   </bookViews>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4201" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4202" uniqueCount="509">
   <si>
     <t>Population Tax Rate</t>
   </si>
@@ -1705,6 +1705,9 @@
   </si>
   <si>
     <t>Yemen</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
   </si>
 </sst>
 </file>
@@ -13098,13 +13101,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4D9EFE-8FC7-4B01-807E-922034333148}">
-  <dimension ref="B1:AN192"/>
+  <dimension ref="B1:AN193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="15" topLeftCell="C148" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="15" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="B160" sqref="B160"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14491,7 +14494,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="60" t="s">
         <v>66</v>
       </c>
       <c r="C22" s="35">
@@ -16521,7 +16524,7 @@
       </c>
     </row>
     <row r="36" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="60" t="s">
         <v>97</v>
       </c>
       <c r="C36" s="35">
@@ -16956,7 +16959,7 @@
       </c>
     </row>
     <row r="39" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="60" t="s">
         <v>18</v>
       </c>
       <c r="C39" s="35">
@@ -17101,7 +17104,7 @@
       </c>
     </row>
     <row r="40" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="60" t="s">
         <v>106</v>
       </c>
       <c r="C40" s="35">
@@ -17826,7 +17829,7 @@
       </c>
     </row>
     <row r="45" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="60" t="s">
         <v>116</v>
       </c>
       <c r="C45" s="35">
@@ -18551,7 +18554,7 @@
       </c>
     </row>
     <row r="50" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B50" s="35" t="s">
+      <c r="B50" s="60" t="s">
         <v>130</v>
       </c>
       <c r="C50" s="35">
@@ -18696,7 +18699,7 @@
       </c>
     </row>
     <row r="51" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="60" t="s">
         <v>29</v>
       </c>
       <c r="C51" s="35">
@@ -18841,7 +18844,7 @@
       </c>
     </row>
     <row r="52" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="60" t="s">
         <v>133</v>
       </c>
       <c r="C52" s="35">
@@ -20726,7 +20729,7 @@
       </c>
     </row>
     <row r="65" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B65" s="35" t="s">
+      <c r="B65" s="60" t="s">
         <v>162</v>
       </c>
       <c r="C65" s="35">
@@ -23771,7 +23774,7 @@
       </c>
     </row>
     <row r="86" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B86" s="35" t="s">
+      <c r="B86" s="60" t="s">
         <v>213</v>
       </c>
       <c r="C86" s="35">
@@ -24641,7 +24644,7 @@
       </c>
     </row>
     <row r="92" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B92" s="35" t="s">
+      <c r="B92" s="60" t="s">
         <v>226</v>
       </c>
       <c r="C92" s="35">
@@ -25656,7 +25659,7 @@
       </c>
     </row>
     <row r="99" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B99" s="35" t="s">
+      <c r="B99" s="60" t="s">
         <v>31</v>
       </c>
       <c r="C99" s="35">
@@ -26381,7 +26384,7 @@
       </c>
     </row>
     <row r="104" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B104" s="35" t="s">
+      <c r="B104" s="60" t="s">
         <v>253</v>
       </c>
       <c r="C104" s="35">
@@ -26961,7 +26964,7 @@
       </c>
     </row>
     <row r="108" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B108" s="35" t="s">
+      <c r="B108" s="60" t="s">
         <v>261</v>
       </c>
       <c r="C108" s="35">
@@ -28407,7 +28410,7 @@
       </c>
     </row>
     <row r="118" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B118" s="35" t="s">
+      <c r="B118" s="60" t="s">
         <v>285</v>
       </c>
       <c r="C118" s="35">
@@ -29857,7 +29860,7 @@
       </c>
     </row>
     <row r="128" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B128" s="35" t="s">
+      <c r="B128" s="60" t="s">
         <v>307</v>
       </c>
       <c r="C128" s="35">
@@ -30437,7 +30440,7 @@
       </c>
     </row>
     <row r="132" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B132" s="35" t="s">
+      <c r="B132" s="60" t="s">
         <v>315</v>
       </c>
       <c r="C132" s="35">
@@ -32612,7 +32615,7 @@
       </c>
     </row>
     <row r="147" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B147" s="35" t="s">
+      <c r="B147" s="60" t="s">
         <v>349</v>
       </c>
       <c r="C147" s="35">
@@ -32757,7 +32760,7 @@
       </c>
     </row>
     <row r="148" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B148" s="35" t="s">
+      <c r="B148" s="60" t="s">
         <v>351</v>
       </c>
       <c r="C148" s="35">
@@ -32771,60 +32774,60 @@
         <v>3040143002.0130162</v>
       </c>
       <c r="F148" s="34">
-        <f t="shared" ref="F148:F192" si="141">ROUND(E148/$C$6,0)</f>
+        <f t="shared" ref="F148:F193" si="141">ROUND(E148/$C$6,0)</f>
         <v>1</v>
       </c>
       <c r="G148" s="34">
-        <f t="shared" ref="G148:G192" si="142">F148*$C$6*$C$8</f>
+        <f t="shared" ref="G148:G193" si="142">F148*$C$6*$C$8</f>
         <v>14096578622.930536</v>
       </c>
       <c r="H148" s="34">
-        <f t="shared" ref="H148:H192" si="143">C148-G148</f>
+        <f t="shared" ref="H148:H193" si="143">C148-G148</f>
         <v>155841897555.6507</v>
       </c>
       <c r="I148" s="37">
         <v>54.027488592566343</v>
       </c>
       <c r="J148" s="39">
-        <f t="shared" ref="J148:J192" si="144">I148/(I148+L148)*H148*$F$7</f>
+        <f t="shared" ref="J148:J193" si="144">I148/(I148+L148)*H148*$F$7</f>
         <v>76025601024.445969</v>
       </c>
       <c r="K148" s="39">
-        <f t="shared" ref="K148:K192" si="145">ROUND(J148/$F$9,0)</f>
+        <f t="shared" ref="K148:K193" si="145">ROUND(J148/$F$9,0)</f>
         <v>2</v>
       </c>
       <c r="L148" s="39">
         <v>29.034133699552562</v>
       </c>
       <c r="M148" s="39">
-        <f t="shared" ref="M148:M192" si="146">L148/(I148+L148)*H148*(2-$F$7)</f>
+        <f t="shared" ref="M148:M193" si="146">L148/(I148+L148)*H148*(2-$F$7)</f>
         <v>68093036903.820114</v>
       </c>
       <c r="N148" s="39">
-        <f t="shared" ref="N148:N192" si="147">ROUND(M148/$F$8,0)</f>
+        <f t="shared" ref="N148:N193" si="147">ROUND(M148/$F$8,0)</f>
         <v>3</v>
       </c>
       <c r="O148" s="49">
-        <f t="shared" ref="O148:O192" si="148">F148</f>
+        <f t="shared" ref="O148:O193" si="148">F148</f>
         <v>1</v>
       </c>
       <c r="P148" s="50">
-        <f t="shared" ref="P148:P192" si="149">N148</f>
+        <f t="shared" ref="P148:P193" si="149">N148</f>
         <v>3</v>
       </c>
       <c r="Q148" s="50">
-        <f t="shared" ref="Q148:Q192" si="150">K148</f>
+        <f t="shared" ref="Q148:Q193" si="150">K148</f>
         <v>2</v>
       </c>
       <c r="R148" s="51">
-        <f t="shared" ref="R148:R192" si="151">O148+P148+Q148</f>
+        <f t="shared" ref="R148:R193" si="151">O148+P148+Q148</f>
         <v>6</v>
       </c>
       <c r="T148" s="39">
         <v>393259049121.62598</v>
       </c>
       <c r="U148" s="39">
-        <f t="shared" ref="U148:U192" si="152">(T148-C148)*$U$11+C148</f>
+        <f t="shared" ref="U148:U193" si="152">(T148-C148)*$U$11+C148</f>
         <v>260450304392.39728</v>
       </c>
       <c r="V148" s="35">
@@ -32835,11 +32838,11 @@
         <v>3245100890.1077366</v>
       </c>
       <c r="X148" s="34">
-        <f t="shared" ref="X148:X192" si="153">ROUND(W148/$C$6,0)</f>
+        <f t="shared" ref="X148:X193" si="153">ROUND(W148/$C$6,0)</f>
         <v>1</v>
       </c>
       <c r="Y148" s="34">
-        <f t="shared" ref="Y148:Y192" si="154">X148*$C$6*$C$8</f>
+        <f t="shared" ref="Y148:Y193" si="154">X148*$C$6*$C$8</f>
         <v>14096578622.930536</v>
       </c>
       <c r="Z148" s="34">
@@ -32850,59 +32853,59 @@
         <v>53.928333156489416</v>
       </c>
       <c r="AB148" s="39">
-        <f t="shared" ref="AB148:AB192" si="155">AA148/(AA148+AD148)*Z148*$F$7</f>
+        <f t="shared" ref="AB148:AB193" si="155">AA148/(AA148+AD148)*Z148*$F$7</f>
         <v>116913370864.92297</v>
       </c>
       <c r="AC148" s="39">
-        <f t="shared" ref="AC148:AC192" si="156">ROUND(AB148/$F$9,0)</f>
+        <f t="shared" ref="AC148:AC193" si="156">ROUND(AB148/$F$9,0)</f>
         <v>3</v>
       </c>
       <c r="AD148" s="39">
         <v>31.29788412314732</v>
       </c>
       <c r="AE148" s="39">
-        <f t="shared" ref="AE148:AE192" si="157">AD148/(AA148+AD148)*Z148*(2-$F$7)</f>
+        <f t="shared" ref="AE148:AE193" si="157">AD148/(AA148+AD148)*Z148*(2-$F$7)</f>
         <v>113086539103.62848</v>
       </c>
       <c r="AF148" s="39">
-        <f t="shared" ref="AF148:AF192" si="158">ROUND(AE148/$F$8,0)</f>
+        <f t="shared" ref="AF148:AF193" si="158">ROUND(AE148/$F$8,0)</f>
         <v>5</v>
       </c>
       <c r="AG148" s="49">
-        <f t="shared" ref="AG148:AG192" si="159">X148</f>
+        <f t="shared" ref="AG148:AG193" si="159">X148</f>
         <v>1</v>
       </c>
       <c r="AH148" s="50">
-        <f t="shared" ref="AH148:AH192" si="160">AF148</f>
+        <f t="shared" ref="AH148:AH193" si="160">AF148</f>
         <v>5</v>
       </c>
       <c r="AI148" s="50">
-        <f t="shared" ref="AI148:AI192" si="161">AC148</f>
+        <f t="shared" ref="AI148:AI193" si="161">AC148</f>
         <v>3</v>
       </c>
       <c r="AJ148" s="51">
-        <f t="shared" ref="AJ148:AJ192" si="162">AG148+AH148+AI148</f>
+        <f t="shared" ref="AJ148:AJ193" si="162">AG148+AH148+AI148</f>
         <v>9</v>
       </c>
       <c r="AK148" s="49">
-        <f t="shared" ref="AK148:AK192" si="163">AG148-O148</f>
+        <f t="shared" ref="AK148:AK193" si="163">AG148-O148</f>
         <v>0</v>
       </c>
       <c r="AL148" s="50">
-        <f t="shared" ref="AL148:AL192" si="164">AH148-P148</f>
+        <f t="shared" ref="AL148:AL193" si="164">AH148-P148</f>
         <v>2</v>
       </c>
       <c r="AM148" s="50">
-        <f t="shared" ref="AM148:AM192" si="165">AI148-Q148</f>
+        <f t="shared" ref="AM148:AM193" si="165">AI148-Q148</f>
         <v>1</v>
       </c>
       <c r="AN148" s="51">
-        <f t="shared" ref="AN148:AN192" si="166">AJ148-R148</f>
+        <f t="shared" ref="AN148:AN193" si="166">AJ148-R148</f>
         <v>3</v>
       </c>
     </row>
     <row r="149" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B149" s="35" t="s">
+      <c r="B149" s="60" t="s">
         <v>353</v>
       </c>
       <c r="C149" s="35">
@@ -35949,7 +35952,7 @@
       </c>
     </row>
     <row r="170" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B170" s="35" t="s">
+      <c r="B170" s="60" t="s">
         <v>413</v>
       </c>
       <c r="C170" s="35">
@@ -36815,7 +36818,7 @@
       </c>
     </row>
     <row r="176" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B176" s="35" t="s">
+      <c r="B176" s="60" t="s">
         <v>423</v>
       </c>
       <c r="C176" s="35">
@@ -36960,7 +36963,7 @@
       </c>
     </row>
     <row r="177" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B177" s="35" t="s">
+      <c r="B177" s="60" t="s">
         <v>425</v>
       </c>
       <c r="C177" s="35">
@@ -36970,7 +36973,7 @@
         <v>0.85501148400089511</v>
       </c>
       <c r="E177" s="35">
-        <f t="shared" ref="E177:E192" si="223">D177/100*C177</f>
+        <f t="shared" ref="E177:E193" si="223">D177/100*C177</f>
         <v>17605314.763955552</v>
       </c>
       <c r="F177" s="34">
@@ -37614,7 +37617,7 @@
         <v>2.0652596724157299</v>
       </c>
       <c r="W181" s="35">
-        <f t="shared" ref="W181:W192" si="224">V181/100*U181</f>
+        <f t="shared" ref="W181:W193" si="224">V181/100*U181</f>
         <v>31039471752.397705</v>
       </c>
       <c r="X181" s="34">
@@ -37626,7 +37629,7 @@
         <v>197352100721.0275</v>
       </c>
       <c r="Z181" s="34">
-        <f t="shared" ref="Z181:Z192" si="225">U181-Y181</f>
+        <f t="shared" ref="Z181:Z193" si="225">U181-Y181</f>
         <v>1305581025169.6697</v>
       </c>
       <c r="AA181" s="37">
@@ -38410,7 +38413,7 @@
       </c>
     </row>
     <row r="187" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B187" s="35" t="s">
+      <c r="B187" s="60" t="s">
         <v>451</v>
       </c>
       <c r="C187" s="35">
@@ -38699,578 +38702,723 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B189" s="35" t="s">
+    <row r="189" spans="2:40" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B189" s="60" t="s">
+        <v>508</v>
+      </c>
+      <c r="C189" s="39">
+        <v>168548247978</v>
+      </c>
+      <c r="D189" s="39">
+        <v>1.5265701288490501</v>
+      </c>
+      <c r="E189" s="39">
+        <f t="shared" ref="E189" si="226">D189/100*C189</f>
+        <v>2573007206.3305712</v>
+      </c>
+      <c r="F189" s="34">
+        <f t="shared" ref="F189" si="227">ROUND(E189/$C$6,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G189" s="34">
+        <f t="shared" ref="G189" si="228">F189*$C$6*$C$8</f>
+        <v>14096578622.930536</v>
+      </c>
+      <c r="H189" s="34">
+        <f t="shared" ref="H189" si="229">C189-G189</f>
+        <v>154451669355.06946</v>
+      </c>
+      <c r="I189" s="39">
+        <v>43.081849066103153</v>
+      </c>
+      <c r="J189" s="39">
+        <f t="shared" ref="J189" si="230">I189/(I189+L189)*H189*$F$7</f>
+        <v>55768597788.333916</v>
+      </c>
+      <c r="K189" s="39">
+        <f t="shared" ref="K189" si="231">ROUND(J189/$F$9,0)</f>
+        <v>2</v>
+      </c>
+      <c r="L189" s="39">
+        <v>46.404848256167305</v>
+      </c>
+      <c r="M189" s="39">
+        <f t="shared" ref="M189" si="232">L189/(I189+L189)*H189*(2-$F$7)</f>
+        <v>100116923713.2803</v>
+      </c>
+      <c r="N189" s="39">
+        <f t="shared" ref="N189" si="233">ROUND(M189/$F$8,0)</f>
+        <v>4</v>
+      </c>
+      <c r="O189" s="49">
+        <f t="shared" ref="O189" si="234">F189</f>
+        <v>1</v>
+      </c>
+      <c r="P189" s="50">
+        <f t="shared" ref="P189" si="235">N189</f>
+        <v>4</v>
+      </c>
+      <c r="Q189" s="50">
+        <f t="shared" ref="Q189" si="236">K189</f>
+        <v>2</v>
+      </c>
+      <c r="R189" s="51">
+        <f t="shared" ref="R189" si="237">O189+P189+Q189</f>
+        <v>7</v>
+      </c>
+      <c r="T189" s="39">
+        <v>141632345013</v>
+      </c>
+      <c r="U189" s="39">
+        <f t="shared" ref="U189" si="238">(T189-C189)*$U$11+C189</f>
+        <v>157639232506.28549</v>
+      </c>
+      <c r="V189" s="39">
+        <v>0.48784414488216299</v>
+      </c>
+      <c r="W189" s="39">
+        <f t="shared" ref="W189" si="239">V189/100*U189</f>
+        <v>769033765.81909323</v>
+      </c>
+      <c r="X189" s="34">
+        <f t="shared" ref="X189" si="240">ROUND(W189/$C$6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y189" s="34">
+        <f t="shared" ref="Y189" si="241">X189*$C$6*$C$8</f>
+        <v>0</v>
+      </c>
+      <c r="Z189" s="34">
+        <f t="shared" ref="Z189" si="242">U189-Y189</f>
+        <v>157639232506.28549</v>
+      </c>
+      <c r="AA189" s="39">
+        <v>43.081849066103153</v>
+      </c>
+      <c r="AB189" s="39">
+        <f t="shared" ref="AB189" si="243">AA189/(AA189+AD189)*Z189*$F$7</f>
+        <v>56919546353.97496</v>
+      </c>
+      <c r="AC189" s="39">
+        <f t="shared" ref="AC189" si="244">ROUND(AB189/$F$9,0)</f>
+        <v>2</v>
+      </c>
+      <c r="AD189" s="39">
+        <v>46.404848256167305</v>
+      </c>
+      <c r="AE189" s="39">
+        <f t="shared" ref="AE189" si="245">AD189/(AA189+AD189)*Z189*(2-$F$7)</f>
+        <v>102183130042.89862</v>
+      </c>
+      <c r="AF189" s="39">
+        <f t="shared" ref="AF189" si="246">ROUND(AE189/$F$8,0)</f>
+        <v>4</v>
+      </c>
+      <c r="AG189" s="49">
+        <f t="shared" ref="AG189" si="247">X189</f>
+        <v>0</v>
+      </c>
+      <c r="AH189" s="50">
+        <f t="shared" ref="AH189" si="248">AF189</f>
+        <v>4</v>
+      </c>
+      <c r="AI189" s="50">
+        <f t="shared" ref="AI189" si="249">AC189</f>
+        <v>2</v>
+      </c>
+      <c r="AJ189" s="51">
+        <f t="shared" ref="AJ189" si="250">AG189+AH189+AI189</f>
+        <v>6</v>
+      </c>
+      <c r="AK189" s="49">
+        <f t="shared" ref="AK189" si="251">AG189-O189</f>
+        <v>-1</v>
+      </c>
+      <c r="AL189" s="50">
+        <f t="shared" ref="AL189" si="252">AH189-P189</f>
+        <v>0</v>
+      </c>
+      <c r="AM189" s="50">
+        <f t="shared" ref="AM189" si="253">AI189-Q189</f>
+        <v>0</v>
+      </c>
+      <c r="AN189" s="51">
+        <f t="shared" ref="AN189" si="254">AJ189-R189</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="190" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B190" s="60" t="s">
         <v>459</v>
       </c>
-      <c r="C189" s="35">
+      <c r="C190" s="35">
         <v>236133898430.63821</v>
       </c>
-      <c r="D189" s="35">
-        <v>0</v>
-      </c>
-      <c r="E189" s="35">
+      <c r="D190" s="35">
+        <v>0</v>
+      </c>
+      <c r="E190" s="35">
         <f t="shared" si="223"/>
         <v>0</v>
       </c>
-      <c r="F189" s="34">
+      <c r="F190" s="34">
         <f t="shared" si="141"/>
         <v>0</v>
       </c>
-      <c r="G189" s="34">
+      <c r="G190" s="34">
         <f t="shared" si="142"/>
         <v>0</v>
       </c>
-      <c r="H189" s="34">
+      <c r="H190" s="34">
         <f t="shared" si="143"/>
         <v>236133898430.63821</v>
       </c>
-      <c r="I189" s="37">
+      <c r="I190" s="37">
         <v>38.734642677619632</v>
       </c>
-      <c r="J189" s="39">
+      <c r="J190" s="39">
         <f t="shared" si="144"/>
         <v>90901525708.53299</v>
       </c>
-      <c r="K189" s="39">
+      <c r="K190" s="39">
         <f t="shared" si="145"/>
         <v>3</v>
       </c>
-      <c r="L189" s="39">
+      <c r="L190" s="39">
         <v>36.730775326845482</v>
       </c>
-      <c r="M189" s="39">
+      <c r="M190" s="39">
         <f t="shared" si="146"/>
         <v>143664830190.7428</v>
       </c>
-      <c r="N189" s="39">
+      <c r="N190" s="39">
         <f t="shared" si="147"/>
         <v>6</v>
       </c>
-      <c r="O189" s="49">
+      <c r="O190" s="49">
         <f t="shared" si="148"/>
         <v>0</v>
       </c>
-      <c r="P189" s="50">
+      <c r="P190" s="50">
         <f t="shared" si="149"/>
         <v>6</v>
       </c>
-      <c r="Q189" s="50">
+      <c r="Q190" s="50">
         <f t="shared" si="150"/>
         <v>3</v>
       </c>
-      <c r="R189" s="51">
+      <c r="R190" s="51">
         <f t="shared" si="151"/>
         <v>9</v>
       </c>
-      <c r="T189" s="39">
+      <c r="T190" s="39">
         <v>676909526449.60107</v>
       </c>
-      <c r="U189" s="39">
+      <c r="U190" s="39">
         <f t="shared" si="152"/>
         <v>414780260466.72388</v>
       </c>
-      <c r="V189" s="35">
-        <v>0</v>
-      </c>
-      <c r="W189" s="35">
+      <c r="V190" s="35">
+        <v>0</v>
+      </c>
+      <c r="W190" s="35">
         <f t="shared" si="224"/>
         <v>0</v>
       </c>
-      <c r="X189" s="34">
+      <c r="X190" s="34">
         <f t="shared" si="153"/>
         <v>0</v>
       </c>
-      <c r="Y189" s="34">
+      <c r="Y190" s="34">
         <f t="shared" si="154"/>
         <v>0</v>
       </c>
-      <c r="Z189" s="34">
+      <c r="Z190" s="34">
         <f t="shared" si="225"/>
         <v>414780260466.72388</v>
       </c>
-      <c r="AA189" s="37">
+      <c r="AA190" s="37">
         <v>41.260453757759478</v>
       </c>
-      <c r="AB189" s="39">
+      <c r="AB190" s="39">
         <f t="shared" si="155"/>
         <v>171920549352.81085</v>
       </c>
-      <c r="AC189" s="39">
+      <c r="AC190" s="39">
         <f t="shared" si="156"/>
         <v>5</v>
       </c>
-      <c r="AD189" s="39">
+      <c r="AD190" s="39">
         <v>33.399128041989826</v>
       </c>
-      <c r="AE189" s="39">
+      <c r="AE190" s="39">
         <f t="shared" si="157"/>
         <v>231941076662.05341</v>
       </c>
-      <c r="AF189" s="39">
+      <c r="AF190" s="39">
         <f t="shared" si="158"/>
         <v>10</v>
       </c>
-      <c r="AG189" s="49">
+      <c r="AG190" s="49">
         <f t="shared" si="159"/>
         <v>0</v>
       </c>
-      <c r="AH189" s="50">
+      <c r="AH190" s="50">
         <f t="shared" si="160"/>
         <v>10</v>
       </c>
-      <c r="AI189" s="50">
+      <c r="AI190" s="50">
         <f t="shared" si="161"/>
         <v>5</v>
       </c>
-      <c r="AJ189" s="51">
+      <c r="AJ190" s="51">
         <f t="shared" si="162"/>
         <v>15</v>
       </c>
-      <c r="AK189" s="49">
+      <c r="AK190" s="49">
         <f t="shared" si="163"/>
         <v>0</v>
       </c>
-      <c r="AL189" s="50">
+      <c r="AL190" s="50">
         <f t="shared" si="164"/>
         <v>4</v>
       </c>
-      <c r="AM189" s="50">
+      <c r="AM190" s="50">
         <f t="shared" si="165"/>
         <v>2</v>
       </c>
-      <c r="AN189" s="51">
+      <c r="AN190" s="51">
         <f t="shared" si="166"/>
         <v>6</v>
       </c>
     </row>
-    <row r="190" spans="2:40" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="60" t="s">
+    <row r="191" spans="2:40" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B191" s="60" t="s">
         <v>507</v>
       </c>
-      <c r="C190" s="39">
+      <c r="C191" s="39">
         <v>24153264424</v>
       </c>
-      <c r="D190" s="39">
+      <c r="D191" s="39">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E190" s="39">
-        <f t="shared" ref="E190" si="226">D190/100*C190</f>
+      <c r="E191" s="39">
+        <f t="shared" ref="E191" si="255">D191/100*C191</f>
         <v>1183509956.776</v>
       </c>
-      <c r="F190" s="34">
-        <f t="shared" ref="F190" si="227">ROUND(E190/$C$6,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G190" s="34">
-        <f t="shared" ref="G190" si="228">F190*$C$6*$C$8</f>
+      <c r="F191" s="34">
+        <f t="shared" ref="F191" si="256">ROUND(E191/$C$6,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G191" s="34">
+        <f t="shared" ref="G191" si="257">F191*$C$6*$C$8</f>
         <v>14096578622.930536</v>
       </c>
-      <c r="H190" s="34">
-        <f t="shared" ref="H190" si="229">C190-G190</f>
+      <c r="H191" s="34">
+        <f t="shared" ref="H191" si="258">C191-G191</f>
         <v>10056685801.069464</v>
       </c>
-      <c r="I190" s="39">
+      <c r="I191" s="39">
         <v>31</v>
       </c>
-      <c r="J190" s="39">
-        <f t="shared" ref="J190" si="230">I190/(I190+L190)*H190*$F$7</f>
+      <c r="J191" s="39">
+        <f t="shared" ref="J191" si="259">I191/(I191+L191)*H191*$F$7</f>
         <v>3036596686.6865592</v>
       </c>
-      <c r="K190" s="39">
-        <f t="shared" ref="K190" si="231">ROUND(J190/$F$9,0)</f>
-        <v>0</v>
-      </c>
-      <c r="L190" s="39">
+      <c r="K191" s="39">
+        <f t="shared" ref="K191" si="260">ROUND(J191/$F$9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L191" s="39">
         <v>46</v>
       </c>
-      <c r="M190" s="39">
-        <f t="shared" ref="M190" si="232">L190/(I190+L190)*H190*(2-$F$7)</f>
+      <c r="M191" s="39">
+        <f t="shared" ref="M191" si="261">L191/(I191+L191)*H191*(2-$F$7)</f>
         <v>7509862773.525898</v>
       </c>
-      <c r="N190" s="39">
-        <f t="shared" ref="N190" si="233">ROUND(M190/$F$8,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O190" s="49">
-        <f t="shared" ref="O190" si="234">F190</f>
-        <v>1</v>
-      </c>
-      <c r="P190" s="50">
-        <f t="shared" ref="P190" si="235">N190</f>
-        <v>0</v>
-      </c>
-      <c r="Q190" s="50">
-        <f t="shared" ref="Q190" si="236">K190</f>
-        <v>0</v>
-      </c>
-      <c r="R190" s="51">
-        <f t="shared" ref="R190" si="237">O190+P190+Q190</f>
-        <v>1</v>
-      </c>
-      <c r="U190" s="39">
+      <c r="N191" s="39">
+        <f t="shared" ref="N191" si="262">ROUND(M191/$F$8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O191" s="49">
+        <f t="shared" ref="O191" si="263">F191</f>
+        <v>1</v>
+      </c>
+      <c r="P191" s="50">
+        <f t="shared" ref="P191" si="264">N191</f>
+        <v>0</v>
+      </c>
+      <c r="Q191" s="50">
+        <f t="shared" ref="Q191" si="265">K191</f>
+        <v>0</v>
+      </c>
+      <c r="R191" s="51">
+        <f t="shared" ref="R191" si="266">O191+P191+Q191</f>
+        <v>1</v>
+      </c>
+      <c r="U191" s="39">
         <v>66914452000</v>
       </c>
-      <c r="V190" s="39">
+      <c r="V191" s="39">
         <v>4.9000000000000004</v>
       </c>
-      <c r="W190" s="39">
-        <f t="shared" ref="W190" si="238">V190/100*U190</f>
+      <c r="W191" s="39">
+        <f t="shared" ref="W191" si="267">V191/100*U191</f>
         <v>3278808148</v>
       </c>
-      <c r="X190" s="34">
-        <f t="shared" ref="X190" si="239">ROUND(W190/$C$6,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Y190" s="34">
-        <f t="shared" ref="Y190" si="240">X190*$C$6*$C$8</f>
+      <c r="X191" s="34">
+        <f t="shared" ref="X191" si="268">ROUND(W191/$C$6,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y191" s="34">
+        <f t="shared" ref="Y191" si="269">X191*$C$6*$C$8</f>
         <v>14096578622.930536</v>
       </c>
-      <c r="Z190" s="34">
-        <f t="shared" ref="Z190" si="241">U190-Y190</f>
+      <c r="Z191" s="34">
+        <f t="shared" ref="Z191" si="270">U191-Y191</f>
         <v>52817873377.069466</v>
       </c>
-      <c r="AA190" s="39">
+      <c r="AA191" s="39">
         <v>19</v>
       </c>
-      <c r="AB190" s="39">
-        <f t="shared" ref="AB190" si="242">AA190/(AA190+AD190)*Z190*$F$7</f>
+      <c r="AB191" s="39">
+        <f t="shared" ref="AB191" si="271">AA191/(AA191+AD191)*Z191*$F$7</f>
         <v>12338601567.594097</v>
       </c>
-      <c r="AC190" s="39">
-        <f t="shared" ref="AC190" si="243">ROUND(AB190/$F$9,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AD190" s="39">
+      <c r="AC191" s="39">
+        <f t="shared" ref="AC191" si="272">ROUND(AB191/$F$9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD191" s="39">
         <v>42</v>
       </c>
-      <c r="AE190" s="39">
-        <f t="shared" ref="AE190" si="244">AD190/(AA190+AD190)*Z190*(2-$F$7)</f>
+      <c r="AE191" s="39">
+        <f t="shared" ref="AE191" si="273">AD191/(AA191+AD191)*Z191*(2-$F$7)</f>
         <v>45458005775.346672</v>
       </c>
-      <c r="AF190" s="39">
-        <f t="shared" ref="AF190" si="245">ROUND(AE190/$F$8,0)</f>
+      <c r="AF191" s="39">
+        <f t="shared" ref="AF191" si="274">ROUND(AE191/$F$8,0)</f>
         <v>2</v>
       </c>
-      <c r="AG190" s="49">
-        <f t="shared" ref="AG190" si="246">X190</f>
-        <v>1</v>
-      </c>
-      <c r="AH190" s="50">
-        <f t="shared" ref="AH190" si="247">AF190</f>
+      <c r="AG191" s="49">
+        <f t="shared" ref="AG191" si="275">X191</f>
+        <v>1</v>
+      </c>
+      <c r="AH191" s="50">
+        <f t="shared" ref="AH191" si="276">AF191</f>
         <v>2</v>
       </c>
-      <c r="AI190" s="50">
-        <f t="shared" ref="AI190" si="248">AC190</f>
-        <v>0</v>
-      </c>
-      <c r="AJ190" s="51">
-        <f t="shared" ref="AJ190" si="249">AG190+AH190+AI190</f>
+      <c r="AI191" s="50">
+        <f t="shared" ref="AI191" si="277">AC191</f>
+        <v>0</v>
+      </c>
+      <c r="AJ191" s="51">
+        <f t="shared" ref="AJ191" si="278">AG191+AH191+AI191</f>
         <v>3</v>
       </c>
-      <c r="AK190" s="49">
-        <f t="shared" ref="AK190" si="250">AG190-O190</f>
-        <v>0</v>
-      </c>
-      <c r="AL190" s="50">
-        <f t="shared" ref="AL190" si="251">AH190-P190</f>
+      <c r="AK191" s="49">
+        <f t="shared" ref="AK191" si="279">AG191-O191</f>
+        <v>0</v>
+      </c>
+      <c r="AL191" s="50">
+        <f t="shared" ref="AL191" si="280">AH191-P191</f>
         <v>2</v>
       </c>
-      <c r="AM190" s="50">
-        <f t="shared" ref="AM190" si="252">AI190-Q190</f>
-        <v>0</v>
-      </c>
-      <c r="AN190" s="51">
-        <f t="shared" ref="AN190" si="253">AJ190-R190</f>
+      <c r="AM191" s="50">
+        <f t="shared" ref="AM191" si="281">AI191-Q191</f>
+        <v>0</v>
+      </c>
+      <c r="AN191" s="51">
+        <f t="shared" ref="AN191" si="282">AJ191-R191</f>
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B191" s="60" t="s">
+    <row r="192" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B192" s="60" t="s">
         <v>467</v>
       </c>
-      <c r="C191" s="35">
+      <c r="C192" s="35">
         <v>20736671783.489033</v>
       </c>
-      <c r="D191" s="39">
+      <c r="D192" s="39">
         <v>1.3095961053559599</v>
       </c>
-      <c r="E191" s="35">
+      <c r="E192" s="35">
         <f t="shared" si="223"/>
         <v>271566646.05702066</v>
       </c>
-      <c r="F191" s="34">
+      <c r="F192" s="34">
         <f t="shared" si="141"/>
         <v>0</v>
       </c>
-      <c r="G191" s="34">
+      <c r="G192" s="34">
         <f t="shared" si="142"/>
         <v>0</v>
       </c>
-      <c r="H191" s="34">
+      <c r="H192" s="34">
         <f t="shared" si="143"/>
         <v>20736671783.489033</v>
       </c>
-      <c r="I191" s="37">
+      <c r="I192" s="37">
         <v>48.959533523278196</v>
       </c>
-      <c r="J191" s="39">
+      <c r="J192" s="39">
         <f t="shared" si="144"/>
         <v>10545805891.685978</v>
       </c>
-      <c r="K191" s="39">
+      <c r="K192" s="39">
         <f t="shared" si="145"/>
         <v>0</v>
       </c>
-      <c r="L191" s="39">
+      <c r="L192" s="39">
         <v>23.243894154924387</v>
       </c>
-      <c r="M191" s="39">
+      <c r="M192" s="39">
         <f t="shared" si="146"/>
         <v>8344496576.5513248</v>
       </c>
-      <c r="N191" s="39">
+      <c r="N192" s="39">
         <f t="shared" si="147"/>
         <v>0</v>
       </c>
-      <c r="O191" s="49">
+      <c r="O192" s="49">
         <f t="shared" si="148"/>
         <v>0</v>
       </c>
-      <c r="P191" s="50">
+      <c r="P192" s="50">
         <f t="shared" si="149"/>
         <v>0</v>
       </c>
-      <c r="Q191" s="50">
+      <c r="Q192" s="50">
         <f t="shared" si="150"/>
         <v>0</v>
       </c>
-      <c r="R191" s="51">
+      <c r="R192" s="51">
         <f t="shared" si="151"/>
         <v>0</v>
       </c>
-      <c r="T191" s="39">
+      <c r="T192" s="39">
         <v>58735190955.723938</v>
       </c>
-      <c r="U191" s="39">
+      <c r="U192" s="39">
         <f t="shared" si="152"/>
         <v>36137471603.995842</v>
       </c>
-      <c r="V191" s="35">
+      <c r="V192" s="35">
         <v>1.3095961053559599</v>
       </c>
-      <c r="W191" s="35">
+      <c r="W192" s="35">
         <f t="shared" si="224"/>
         <v>473254920.70004547</v>
       </c>
-      <c r="X191" s="34">
+      <c r="X192" s="34">
         <f t="shared" si="153"/>
         <v>0</v>
       </c>
-      <c r="Y191" s="34">
+      <c r="Y192" s="34">
         <f t="shared" si="154"/>
         <v>0</v>
       </c>
-      <c r="Z191" s="34">
+      <c r="Z192" s="34">
         <f t="shared" si="225"/>
         <v>36137471603.995842</v>
       </c>
-      <c r="AA191" s="37">
+      <c r="AA192" s="37">
         <v>52.093884963370854</v>
       </c>
-      <c r="AB191" s="39">
+      <c r="AB192" s="39">
         <f t="shared" si="155"/>
         <v>15793497324.52545</v>
       </c>
-      <c r="AC191" s="39">
+      <c r="AC192" s="39">
         <f t="shared" si="156"/>
         <v>0</v>
       </c>
-      <c r="AD191" s="39">
+      <c r="AD192" s="39">
         <v>37.304044921462562</v>
       </c>
-      <c r="AE191" s="39">
+      <c r="AE192" s="39">
         <f t="shared" si="157"/>
         <v>18849343964.119057</v>
       </c>
-      <c r="AF191" s="39">
+      <c r="AF192" s="39">
         <f t="shared" si="158"/>
         <v>1</v>
       </c>
-      <c r="AG191" s="49">
+      <c r="AG192" s="49">
         <f t="shared" si="159"/>
         <v>0</v>
       </c>
-      <c r="AH191" s="50">
+      <c r="AH192" s="50">
         <f t="shared" si="160"/>
         <v>1</v>
       </c>
-      <c r="AI191" s="50">
+      <c r="AI192" s="50">
         <f t="shared" si="161"/>
         <v>0</v>
       </c>
-      <c r="AJ191" s="51">
+      <c r="AJ192" s="51">
         <f t="shared" si="162"/>
         <v>1</v>
       </c>
-      <c r="AK191" s="49">
+      <c r="AK192" s="49">
         <f t="shared" si="163"/>
         <v>0</v>
       </c>
-      <c r="AL191" s="50">
+      <c r="AL192" s="50">
         <f t="shared" si="164"/>
         <v>1</v>
       </c>
-      <c r="AM191" s="50">
+      <c r="AM192" s="50">
         <f t="shared" si="165"/>
         <v>0</v>
       </c>
-      <c r="AN191" s="51">
+      <c r="AN192" s="51">
         <f t="shared" si="166"/>
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="60" t="s">
+    <row r="193" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B193" s="60" t="s">
         <v>469</v>
       </c>
-      <c r="C192" s="35">
+      <c r="C193" s="35">
         <v>41269476289.344582</v>
       </c>
-      <c r="D192" s="35">
+      <c r="D193" s="35">
         <v>3.4163479325265604</v>
       </c>
-      <c r="E192" s="35">
+      <c r="E193" s="35">
         <f t="shared" si="223"/>
         <v>1409908899.9755626</v>
       </c>
-      <c r="F192" s="34">
+      <c r="F193" s="34">
         <f t="shared" si="141"/>
         <v>1</v>
       </c>
-      <c r="G192" s="34">
+      <c r="G193" s="34">
         <f t="shared" si="142"/>
         <v>14096578622.930536</v>
       </c>
-      <c r="H192" s="34">
+      <c r="H193" s="34">
         <f t="shared" si="143"/>
         <v>27172897666.414047</v>
       </c>
-      <c r="I192" s="37">
+      <c r="I193" s="37">
         <v>70.125341302611545</v>
       </c>
-      <c r="J192" s="39">
+      <c r="J193" s="39">
         <f t="shared" si="144"/>
         <v>15613746641.292751</v>
       </c>
-      <c r="K192" s="39">
+      <c r="K193" s="39">
         <f t="shared" si="145"/>
         <v>0</v>
       </c>
-      <c r="L192" s="39">
+      <c r="L193" s="39">
         <v>21.404998923297256</v>
       </c>
-      <c r="M192" s="39">
+      <c r="M193" s="39">
         <f t="shared" si="146"/>
         <v>7943211014.1963062</v>
       </c>
-      <c r="N192" s="39">
+      <c r="N193" s="39">
         <f t="shared" si="147"/>
         <v>0</v>
       </c>
-      <c r="O192" s="52">
+      <c r="O193" s="52">
         <f t="shared" si="148"/>
         <v>1</v>
       </c>
-      <c r="P192" s="53">
+      <c r="P193" s="53">
         <f t="shared" si="149"/>
         <v>0</v>
       </c>
-      <c r="Q192" s="53">
+      <c r="Q193" s="53">
         <f t="shared" si="150"/>
         <v>0</v>
       </c>
-      <c r="R192" s="54">
+      <c r="R193" s="54">
         <f t="shared" si="151"/>
         <v>1</v>
       </c>
-      <c r="T192" s="39">
+      <c r="T193" s="39">
         <v>43112365756.24472</v>
       </c>
-      <c r="U192" s="39">
+      <c r="U193" s="39">
         <f t="shared" si="152"/>
         <v>42016399390.279205</v>
       </c>
-      <c r="V192" s="35">
+      <c r="V193" s="35">
         <v>1.5449480513588301</v>
       </c>
-      <c r="W192" s="35">
+      <c r="W193" s="35">
         <f t="shared" si="224"/>
         <v>649131543.63126194</v>
       </c>
-      <c r="X192" s="34">
+      <c r="X193" s="34">
         <f t="shared" si="153"/>
         <v>0</v>
       </c>
-      <c r="Y192" s="34">
+      <c r="Y193" s="34">
         <f t="shared" si="154"/>
         <v>0</v>
       </c>
-      <c r="Z192" s="34">
+      <c r="Z193" s="34">
         <f t="shared" si="225"/>
         <v>42016399390.279205</v>
       </c>
-      <c r="AA192" s="37">
+      <c r="AA193" s="37">
         <v>60.591645107015424</v>
       </c>
-      <c r="AB192" s="39">
+      <c r="AB193" s="39">
         <f t="shared" si="155"/>
         <v>23286100217.613159</v>
       </c>
-      <c r="AC192" s="39">
+      <c r="AC193" s="39">
         <f t="shared" si="156"/>
         <v>1</v>
       </c>
-      <c r="AD192" s="39">
+      <c r="AD193" s="39">
         <v>21.404998923297256</v>
       </c>
-      <c r="AE192" s="39">
+      <c r="AE193" s="39">
         <f t="shared" si="157"/>
         <v>13710332208.493746</v>
       </c>
-      <c r="AF192" s="39">
+      <c r="AF193" s="39">
         <f t="shared" si="158"/>
         <v>1</v>
       </c>
-      <c r="AG192" s="52">
+      <c r="AG193" s="52">
         <f t="shared" si="159"/>
         <v>0</v>
       </c>
-      <c r="AH192" s="53">
+      <c r="AH193" s="53">
         <f t="shared" si="160"/>
         <v>1</v>
       </c>
-      <c r="AI192" s="53">
+      <c r="AI193" s="53">
         <f t="shared" si="161"/>
         <v>1</v>
       </c>
-      <c r="AJ192" s="54">
+      <c r="AJ193" s="54">
         <f t="shared" si="162"/>
         <v>2</v>
       </c>
-      <c r="AK192" s="52">
+      <c r="AK193" s="52">
         <f t="shared" si="163"/>
         <v>-1</v>
       </c>
-      <c r="AL192" s="53">
+      <c r="AL193" s="53">
         <f t="shared" si="164"/>
         <v>1</v>
       </c>
-      <c r="AM192" s="53">
+      <c r="AM193" s="53">
         <f t="shared" si="165"/>
         <v>1</v>
       </c>
-      <c r="AN192" s="54">
+      <c r="AN193" s="54">
         <f t="shared" si="166"/>
         <v>1</v>
       </c>
@@ -39289,8 +39437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A9ED62-1A49-45D7-8157-2940EBDC52F1}">
   <dimension ref="A1:AA218"/>
   <sheetViews>
-    <sheetView topLeftCell="I40" workbookViewId="0">
-      <selection activeCell="T63" sqref="T63"/>
+    <sheetView topLeftCell="J184" workbookViewId="0">
+      <selection activeCell="Z212" sqref="Z212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Factories - Central America
</commit_message>
<xml_diff>
--- a/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
+++ b/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\economy spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E15180-B560-424C-953A-D7F724A5C4FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B637E2F5-2E89-427A-89DA-730F812C25E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C93B8E2A-6318-41E2-B454-20DC41C43396}"/>
   </bookViews>
@@ -2386,20 +2386,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2416,11 +2407,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8449,246 +8449,246 @@
   <sheetData>
     <row r="1" spans="2:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:70" x14ac:dyDescent="0.25">
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="64" t="s">
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="64" t="s">
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="64" t="s">
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="64" t="s">
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="64" t="s">
+      <c r="T2" s="72"/>
+      <c r="U2" s="72"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="65"/>
-      <c r="Y2" s="65"/>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="64" t="s">
+      <c r="X2" s="72"/>
+      <c r="Y2" s="72"/>
+      <c r="Z2" s="73"/>
+      <c r="AA2" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="64" t="s">
+      <c r="AB2" s="72"/>
+      <c r="AC2" s="72"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="64" t="s">
+      <c r="AF2" s="72"/>
+      <c r="AG2" s="72"/>
+      <c r="AH2" s="73"/>
+      <c r="AI2" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="AJ2" s="65"/>
-      <c r="AK2" s="65"/>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="64" t="s">
+      <c r="AJ2" s="72"/>
+      <c r="AK2" s="72"/>
+      <c r="AL2" s="73"/>
+      <c r="AM2" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="65"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="64" t="s">
+      <c r="AN2" s="72"/>
+      <c r="AO2" s="72"/>
+      <c r="AP2" s="73"/>
+      <c r="AQ2" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
-      <c r="AT2" s="66"/>
-      <c r="AU2" s="64" t="s">
+      <c r="AR2" s="72"/>
+      <c r="AS2" s="72"/>
+      <c r="AT2" s="73"/>
+      <c r="AU2" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="AV2" s="65"/>
-      <c r="AW2" s="65"/>
-      <c r="AX2" s="66"/>
-      <c r="AY2" s="64" t="s">
+      <c r="AV2" s="72"/>
+      <c r="AW2" s="72"/>
+      <c r="AX2" s="73"/>
+      <c r="AY2" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="AZ2" s="65"/>
-      <c r="BA2" s="65"/>
-      <c r="BB2" s="66"/>
-      <c r="BC2" s="64" t="s">
+      <c r="AZ2" s="72"/>
+      <c r="BA2" s="72"/>
+      <c r="BB2" s="73"/>
+      <c r="BC2" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="BD2" s="65"/>
-      <c r="BE2" s="65"/>
-      <c r="BF2" s="66"/>
-      <c r="BG2" s="64" t="s">
+      <c r="BD2" s="72"/>
+      <c r="BE2" s="72"/>
+      <c r="BF2" s="73"/>
+      <c r="BG2" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="BH2" s="65"/>
-      <c r="BI2" s="65"/>
-      <c r="BJ2" s="66"/>
-      <c r="BK2" s="64" t="s">
+      <c r="BH2" s="72"/>
+      <c r="BI2" s="72"/>
+      <c r="BJ2" s="73"/>
+      <c r="BK2" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="BL2" s="65"/>
-      <c r="BM2" s="65"/>
-      <c r="BN2" s="66"/>
-      <c r="BO2" s="64" t="s">
+      <c r="BL2" s="72"/>
+      <c r="BM2" s="72"/>
+      <c r="BN2" s="73"/>
+      <c r="BO2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="BP2" s="65"/>
-      <c r="BQ2" s="65"/>
-      <c r="BR2" s="66"/>
+      <c r="BP2" s="72"/>
+      <c r="BQ2" s="72"/>
+      <c r="BR2" s="73"/>
     </row>
     <row r="3" spans="2:70" x14ac:dyDescent="0.25">
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68" t="s">
+      <c r="D3" s="65"/>
+      <c r="E3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="69"/>
-      <c r="G3" s="67" t="s">
+      <c r="F3" s="66"/>
+      <c r="G3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68" t="s">
+      <c r="H3" s="65"/>
+      <c r="I3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="69"/>
-      <c r="K3" s="67" t="s">
+      <c r="J3" s="66"/>
+      <c r="K3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68" t="s">
+      <c r="L3" s="65"/>
+      <c r="M3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="69"/>
-      <c r="O3" s="67" t="s">
+      <c r="N3" s="66"/>
+      <c r="O3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68" t="s">
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="69"/>
-      <c r="S3" s="67" t="s">
+      <c r="R3" s="66"/>
+      <c r="S3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68" t="s">
+      <c r="T3" s="65"/>
+      <c r="U3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="69"/>
-      <c r="W3" s="67" t="s">
+      <c r="V3" s="66"/>
+      <c r="W3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="68"/>
-      <c r="Y3" s="68" t="s">
+      <c r="X3" s="65"/>
+      <c r="Y3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="69"/>
-      <c r="AA3" s="67" t="s">
+      <c r="Z3" s="66"/>
+      <c r="AA3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68" t="s">
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AD3" s="69"/>
-      <c r="AE3" s="67" t="s">
+      <c r="AD3" s="66"/>
+      <c r="AE3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68" t="s">
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AH3" s="69"/>
-      <c r="AI3" s="67" t="s">
+      <c r="AH3" s="66"/>
+      <c r="AI3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AJ3" s="68"/>
-      <c r="AK3" s="68" t="s">
+      <c r="AJ3" s="65"/>
+      <c r="AK3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AL3" s="69"/>
-      <c r="AM3" s="67" t="s">
+      <c r="AL3" s="66"/>
+      <c r="AM3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AN3" s="68"/>
-      <c r="AO3" s="68" t="s">
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AP3" s="69"/>
-      <c r="AQ3" s="67" t="s">
+      <c r="AP3" s="66"/>
+      <c r="AQ3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="68" t="s">
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AT3" s="69"/>
-      <c r="AU3" s="67" t="s">
+      <c r="AT3" s="66"/>
+      <c r="AU3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AV3" s="68"/>
-      <c r="AW3" s="68" t="s">
+      <c r="AV3" s="65"/>
+      <c r="AW3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AX3" s="69"/>
-      <c r="AY3" s="67" t="s">
+      <c r="AX3" s="66"/>
+      <c r="AY3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="AZ3" s="68"/>
-      <c r="BA3" s="68" t="s">
+      <c r="AZ3" s="65"/>
+      <c r="BA3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="BB3" s="69"/>
-      <c r="BC3" s="67" t="s">
+      <c r="BB3" s="66"/>
+      <c r="BC3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="BD3" s="68"/>
-      <c r="BE3" s="68" t="s">
+      <c r="BD3" s="65"/>
+      <c r="BE3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="BF3" s="69"/>
-      <c r="BG3" s="67" t="s">
+      <c r="BF3" s="66"/>
+      <c r="BG3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="BH3" s="68"/>
-      <c r="BI3" s="68" t="s">
+      <c r="BH3" s="65"/>
+      <c r="BI3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="BJ3" s="69"/>
-      <c r="BK3" s="67" t="s">
+      <c r="BJ3" s="66"/>
+      <c r="BK3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="BL3" s="68"/>
-      <c r="BM3" s="68" t="s">
+      <c r="BL3" s="65"/>
+      <c r="BM3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="BN3" s="69"/>
-      <c r="BO3" s="67" t="s">
+      <c r="BN3" s="66"/>
+      <c r="BO3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="BP3" s="68"/>
-      <c r="BQ3" s="68" t="s">
+      <c r="BP3" s="65"/>
+      <c r="BQ3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="BR3" s="69"/>
+      <c r="BR3" s="66"/>
     </row>
     <row r="4" spans="2:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
@@ -8900,10 +8900,10 @@
       <c r="B5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="70">
-        <v>1</v>
-      </c>
-      <c r="D5" s="71"/>
+      <c r="C5" s="67">
+        <v>1</v>
+      </c>
+      <c r="D5" s="68"/>
       <c r="E5" s="22">
         <v>2.9780000000000002</v>
       </c>
@@ -8911,10 +8911,10 @@
         <f>E5/C5-1</f>
         <v>1.9780000000000002</v>
       </c>
-      <c r="G5" s="70">
-        <v>1</v>
-      </c>
-      <c r="H5" s="71"/>
+      <c r="G5" s="67">
+        <v>1</v>
+      </c>
+      <c r="H5" s="68"/>
       <c r="I5" s="22">
         <v>1.84</v>
       </c>
@@ -8922,10 +8922,10 @@
         <f>I5/G5-1</f>
         <v>0.84000000000000008</v>
       </c>
-      <c r="K5" s="70">
-        <v>1</v>
-      </c>
-      <c r="L5" s="71"/>
+      <c r="K5" s="67">
+        <v>1</v>
+      </c>
+      <c r="L5" s="68"/>
       <c r="M5" s="22">
         <v>2.2770000000000001</v>
       </c>
@@ -8933,10 +8933,10 @@
         <f>M5/K5-1</f>
         <v>1.2770000000000001</v>
       </c>
-      <c r="O5" s="70">
-        <v>1</v>
-      </c>
-      <c r="P5" s="71"/>
+      <c r="O5" s="67">
+        <v>1</v>
+      </c>
+      <c r="P5" s="68"/>
       <c r="Q5" s="22">
         <v>2.8029999999999999</v>
       </c>
@@ -8947,7 +8947,7 @@
       <c r="S5" s="74">
         <v>2</v>
       </c>
-      <c r="T5" s="71"/>
+      <c r="T5" s="68"/>
       <c r="U5" s="22">
         <v>12.585000000000001</v>
       </c>
@@ -8955,10 +8955,10 @@
         <f>U5/S5-1</f>
         <v>5.2925000000000004</v>
       </c>
-      <c r="W5" s="70">
+      <c r="W5" s="67">
         <v>2</v>
       </c>
-      <c r="X5" s="71"/>
+      <c r="X5" s="68"/>
       <c r="Y5" s="22">
         <v>10.067</v>
       </c>
@@ -8966,10 +8966,10 @@
         <f>Y5/W5-1</f>
         <v>4.0335000000000001</v>
       </c>
-      <c r="AA5" s="70">
+      <c r="AA5" s="67">
         <v>2</v>
       </c>
-      <c r="AB5" s="71"/>
+      <c r="AB5" s="68"/>
       <c r="AC5" s="22">
         <v>9.9779999999999998</v>
       </c>
@@ -8977,10 +8977,10 @@
         <f>AC5/AA5-1</f>
         <v>3.9889999999999999</v>
       </c>
-      <c r="AE5" s="70">
+      <c r="AE5" s="67">
         <v>7</v>
       </c>
-      <c r="AF5" s="71"/>
+      <c r="AF5" s="68"/>
       <c r="AG5" s="22">
         <v>15.536</v>
       </c>
@@ -8988,10 +8988,10 @@
         <f>AG5/AE5-1</f>
         <v>1.2194285714285713</v>
       </c>
-      <c r="AI5" s="70">
+      <c r="AI5" s="67">
         <v>7</v>
       </c>
-      <c r="AJ5" s="71"/>
+      <c r="AJ5" s="68"/>
       <c r="AK5" s="22">
         <v>24.87</v>
       </c>
@@ -8999,10 +8999,10 @@
         <f>AK5/AI5-1</f>
         <v>2.5528571428571429</v>
       </c>
-      <c r="AM5" s="70">
+      <c r="AM5" s="67">
         <v>7</v>
       </c>
-      <c r="AN5" s="71"/>
+      <c r="AN5" s="68"/>
       <c r="AO5" s="22">
         <v>14.685</v>
       </c>
@@ -9010,10 +9010,10 @@
         <f>AO5/AM5-1</f>
         <v>1.0978571428571429</v>
       </c>
-      <c r="AQ5" s="70">
+      <c r="AQ5" s="67">
         <v>10</v>
       </c>
-      <c r="AR5" s="71"/>
+      <c r="AR5" s="68"/>
       <c r="AS5" s="22">
         <v>13.314</v>
       </c>
@@ -9021,10 +9021,10 @@
         <f>AS5/AQ5-1</f>
         <v>0.33139999999999992</v>
       </c>
-      <c r="AU5" s="70">
+      <c r="AU5" s="67">
         <v>15</v>
       </c>
-      <c r="AV5" s="71"/>
+      <c r="AV5" s="68"/>
       <c r="AW5" s="22">
         <v>35.488</v>
       </c>
@@ -9032,10 +9032,10 @@
         <f>AW5/AU5-1</f>
         <v>1.3658666666666668</v>
       </c>
-      <c r="AY5" s="70">
+      <c r="AY5" s="67">
         <v>20</v>
       </c>
-      <c r="AZ5" s="71"/>
+      <c r="AZ5" s="68"/>
       <c r="BA5" s="22">
         <v>46.418999999999997</v>
       </c>
@@ -9043,10 +9043,10 @@
         <f>BA5/AY5-1</f>
         <v>1.3209499999999998</v>
       </c>
-      <c r="BC5" s="70">
+      <c r="BC5" s="67">
         <v>20</v>
       </c>
-      <c r="BD5" s="71"/>
+      <c r="BD5" s="68"/>
       <c r="BE5" s="22">
         <v>77.132000000000005</v>
       </c>
@@ -9054,10 +9054,10 @@
         <f>BE5/BC5-1</f>
         <v>2.8566000000000003</v>
       </c>
-      <c r="BG5" s="70">
+      <c r="BG5" s="67">
         <v>20</v>
       </c>
-      <c r="BH5" s="71"/>
+      <c r="BH5" s="68"/>
       <c r="BI5" s="22">
         <v>50.906999999999996</v>
       </c>
@@ -9065,10 +9065,10 @@
         <f>BI5/BG5-1</f>
         <v>1.54535</v>
       </c>
-      <c r="BK5" s="70">
+      <c r="BK5" s="67">
         <v>30</v>
       </c>
-      <c r="BL5" s="71"/>
+      <c r="BL5" s="68"/>
       <c r="BM5" s="22">
         <v>39.054000000000002</v>
       </c>
@@ -9076,10 +9076,10 @@
         <f>BM5/BK5-1</f>
         <v>0.30180000000000007</v>
       </c>
-      <c r="BO5" s="70">
+      <c r="BO5" s="67">
         <v>30</v>
       </c>
-      <c r="BP5" s="71"/>
+      <c r="BP5" s="68"/>
       <c r="BQ5" s="22">
         <v>40.4</v>
       </c>
@@ -9092,34 +9092,34 @@
       <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="72">
+      <c r="C6" s="62">
         <v>11</v>
       </c>
-      <c r="D6" s="73"/>
+      <c r="D6" s="63"/>
       <c r="E6" s="23">
         <v>10</v>
       </c>
       <c r="F6" s="26"/>
-      <c r="G6" s="72">
+      <c r="G6" s="62">
         <v>17</v>
       </c>
-      <c r="H6" s="73"/>
+      <c r="H6" s="63"/>
       <c r="I6" s="23">
         <v>30</v>
       </c>
       <c r="J6" s="26"/>
-      <c r="K6" s="72">
+      <c r="K6" s="62">
         <v>10</v>
       </c>
-      <c r="L6" s="73"/>
+      <c r="L6" s="63"/>
       <c r="M6" s="23">
         <v>18</v>
       </c>
       <c r="N6" s="26"/>
-      <c r="O6" s="72">
+      <c r="O6" s="62">
         <v>18</v>
       </c>
-      <c r="P6" s="73"/>
+      <c r="P6" s="63"/>
       <c r="Q6" s="23">
         <v>22</v>
       </c>
@@ -9127,103 +9127,103 @@
       <c r="S6" s="75">
         <v>40</v>
       </c>
-      <c r="T6" s="73"/>
+      <c r="T6" s="63"/>
       <c r="U6" s="23">
         <v>37</v>
       </c>
       <c r="V6" s="26"/>
-      <c r="W6" s="72">
+      <c r="W6" s="62">
         <v>18</v>
       </c>
-      <c r="X6" s="73"/>
+      <c r="X6" s="63"/>
       <c r="Y6" s="23">
         <v>18</v>
       </c>
       <c r="Z6" s="26"/>
-      <c r="AA6" s="72">
+      <c r="AA6" s="62">
         <v>18</v>
       </c>
-      <c r="AB6" s="73"/>
+      <c r="AB6" s="63"/>
       <c r="AC6" s="23">
         <v>20</v>
       </c>
       <c r="AD6" s="26"/>
-      <c r="AE6" s="72">
+      <c r="AE6" s="62">
         <v>14</v>
       </c>
-      <c r="AF6" s="73"/>
+      <c r="AF6" s="63"/>
       <c r="AG6" s="23">
         <v>19</v>
       </c>
       <c r="AH6" s="26"/>
-      <c r="AI6" s="72">
+      <c r="AI6" s="62">
         <v>23</v>
       </c>
-      <c r="AJ6" s="73"/>
+      <c r="AJ6" s="63"/>
       <c r="AK6" s="23">
         <v>21</v>
       </c>
       <c r="AL6" s="26"/>
-      <c r="AM6" s="72">
+      <c r="AM6" s="62">
         <v>7</v>
       </c>
-      <c r="AN6" s="73"/>
+      <c r="AN6" s="63"/>
       <c r="AO6" s="23">
         <v>9</v>
       </c>
       <c r="AP6" s="26"/>
-      <c r="AQ6" s="72">
+      <c r="AQ6" s="62">
         <v>14</v>
       </c>
-      <c r="AR6" s="73"/>
+      <c r="AR6" s="63"/>
       <c r="AS6" s="23">
         <v>22</v>
       </c>
       <c r="AT6" s="26"/>
-      <c r="AU6" s="72">
+      <c r="AU6" s="62">
         <v>12</v>
       </c>
-      <c r="AV6" s="73"/>
+      <c r="AV6" s="63"/>
       <c r="AW6" s="23">
         <v>40</v>
       </c>
       <c r="AX6" s="26"/>
-      <c r="AY6" s="72">
+      <c r="AY6" s="62">
         <v>37</v>
       </c>
-      <c r="AZ6" s="73"/>
+      <c r="AZ6" s="63"/>
       <c r="BA6" s="23">
         <v>44</v>
       </c>
       <c r="BB6" s="26"/>
-      <c r="BC6" s="72">
+      <c r="BC6" s="62">
         <v>30</v>
       </c>
-      <c r="BD6" s="73"/>
+      <c r="BD6" s="63"/>
       <c r="BE6" s="23">
         <v>58</v>
       </c>
       <c r="BF6" s="26"/>
-      <c r="BG6" s="72">
+      <c r="BG6" s="62">
         <v>23</v>
       </c>
-      <c r="BH6" s="73"/>
+      <c r="BH6" s="63"/>
       <c r="BI6" s="23">
         <v>47</v>
       </c>
       <c r="BJ6" s="26"/>
-      <c r="BK6" s="72">
+      <c r="BK6" s="62">
         <v>37</v>
       </c>
-      <c r="BL6" s="73"/>
+      <c r="BL6" s="63"/>
       <c r="BM6" s="23">
         <v>40</v>
       </c>
       <c r="BN6" s="26"/>
-      <c r="BO6" s="72">
+      <c r="BO6" s="62">
         <v>36</v>
       </c>
-      <c r="BP6" s="73"/>
+      <c r="BP6" s="63"/>
       <c r="BQ6" s="23">
         <v>23</v>
       </c>
@@ -9233,104 +9233,104 @@
       <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="73"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="63"/>
       <c r="E7" s="23">
         <v>18</v>
       </c>
       <c r="F7" s="26"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="73"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="63"/>
       <c r="I7" s="23">
         <v>30</v>
       </c>
       <c r="J7" s="26"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="73"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="63"/>
       <c r="M7" s="23">
         <v>32</v>
       </c>
       <c r="N7" s="26"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="73"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="63"/>
       <c r="Q7" s="23">
         <v>18</v>
       </c>
       <c r="R7" s="26"/>
       <c r="S7" s="75"/>
-      <c r="T7" s="73"/>
+      <c r="T7" s="63"/>
       <c r="U7" s="23">
         <v>22</v>
       </c>
       <c r="V7" s="26"/>
-      <c r="W7" s="72"/>
-      <c r="X7" s="73"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="63"/>
       <c r="Y7" s="23">
         <v>22</v>
       </c>
       <c r="Z7" s="26"/>
-      <c r="AA7" s="72"/>
-      <c r="AB7" s="73"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="63"/>
       <c r="AC7" s="23">
         <v>10</v>
       </c>
       <c r="AD7" s="26"/>
-      <c r="AE7" s="72"/>
-      <c r="AF7" s="73"/>
+      <c r="AE7" s="62"/>
+      <c r="AF7" s="63"/>
       <c r="AG7" s="23">
         <v>43</v>
       </c>
       <c r="AH7" s="26"/>
-      <c r="AI7" s="72"/>
-      <c r="AJ7" s="73"/>
+      <c r="AI7" s="62"/>
+      <c r="AJ7" s="63"/>
       <c r="AK7" s="23">
         <v>27</v>
       </c>
       <c r="AL7" s="26"/>
-      <c r="AM7" s="72"/>
-      <c r="AN7" s="73"/>
+      <c r="AM7" s="62"/>
+      <c r="AN7" s="63"/>
       <c r="AO7" s="23">
         <v>6</v>
       </c>
       <c r="AP7" s="26"/>
-      <c r="AQ7" s="72"/>
-      <c r="AR7" s="73"/>
+      <c r="AQ7" s="62"/>
+      <c r="AR7" s="63"/>
       <c r="AS7" s="23">
         <v>15</v>
       </c>
       <c r="AT7" s="26"/>
-      <c r="AU7" s="72"/>
-      <c r="AV7" s="73"/>
+      <c r="AU7" s="62"/>
+      <c r="AV7" s="63"/>
       <c r="AW7" s="23">
         <v>25</v>
       </c>
       <c r="AX7" s="26"/>
-      <c r="AY7" s="72"/>
-      <c r="AZ7" s="73"/>
+      <c r="AY7" s="62"/>
+      <c r="AZ7" s="63"/>
       <c r="BA7" s="23">
         <v>18</v>
       </c>
       <c r="BB7" s="26"/>
-      <c r="BC7" s="72"/>
-      <c r="BD7" s="73"/>
+      <c r="BC7" s="62"/>
+      <c r="BD7" s="63"/>
       <c r="BE7" s="23">
         <v>26</v>
       </c>
       <c r="BF7" s="26"/>
-      <c r="BG7" s="72"/>
-      <c r="BH7" s="73"/>
+      <c r="BG7" s="62"/>
+      <c r="BH7" s="63"/>
       <c r="BI7" s="23">
         <v>36</v>
       </c>
       <c r="BJ7" s="26"/>
-      <c r="BK7" s="72"/>
-      <c r="BL7" s="73"/>
+      <c r="BK7" s="62"/>
+      <c r="BL7" s="63"/>
       <c r="BM7" s="23">
         <v>23</v>
       </c>
       <c r="BN7" s="26"/>
-      <c r="BO7" s="72"/>
-      <c r="BP7" s="73"/>
+      <c r="BO7" s="62"/>
+      <c r="BP7" s="63"/>
       <c r="BQ7" s="23">
         <v>33</v>
       </c>
@@ -9340,11 +9340,11 @@
       <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="62">
+      <c r="C8" s="69">
         <f>C6</f>
         <v>11</v>
       </c>
-      <c r="D8" s="63"/>
+      <c r="D8" s="70"/>
       <c r="E8" s="24">
         <f>(E6+E7)/2</f>
         <v>14</v>
@@ -9353,11 +9353,11 @@
         <f>E8/C8-1</f>
         <v>0.27272727272727271</v>
       </c>
-      <c r="G8" s="62">
+      <c r="G8" s="69">
         <f>G6</f>
         <v>17</v>
       </c>
-      <c r="H8" s="63"/>
+      <c r="H8" s="70"/>
       <c r="I8" s="24">
         <f>(I6+I7)/2</f>
         <v>30</v>
@@ -9366,11 +9366,11 @@
         <f>I8/G8-1</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="K8" s="62">
+      <c r="K8" s="69">
         <f>K6</f>
         <v>10</v>
       </c>
-      <c r="L8" s="63"/>
+      <c r="L8" s="70"/>
       <c r="M8" s="24">
         <f>(M6+M7)/2</f>
         <v>25</v>
@@ -9379,11 +9379,11 @@
         <f>M8/K8-1</f>
         <v>1.5</v>
       </c>
-      <c r="O8" s="62">
+      <c r="O8" s="69">
         <f>O6</f>
         <v>18</v>
       </c>
-      <c r="P8" s="63"/>
+      <c r="P8" s="70"/>
       <c r="Q8" s="24">
         <f>(Q6+Q7)/2</f>
         <v>20</v>
@@ -9396,7 +9396,7 @@
         <f>S6</f>
         <v>40</v>
       </c>
-      <c r="T8" s="63"/>
+      <c r="T8" s="70"/>
       <c r="U8" s="24">
         <f>(U6+U7)/2</f>
         <v>29.5</v>
@@ -9405,11 +9405,11 @@
         <f>U8/S8-1</f>
         <v>-0.26249999999999996</v>
       </c>
-      <c r="W8" s="62">
+      <c r="W8" s="69">
         <f>W6</f>
         <v>18</v>
       </c>
-      <c r="X8" s="63"/>
+      <c r="X8" s="70"/>
       <c r="Y8" s="24">
         <f>(Y6+Y7)/2</f>
         <v>20</v>
@@ -9418,11 +9418,11 @@
         <f>Y8/W8-1</f>
         <v>0.11111111111111116</v>
       </c>
-      <c r="AA8" s="62">
+      <c r="AA8" s="69">
         <f>AA6</f>
         <v>18</v>
       </c>
-      <c r="AB8" s="63"/>
+      <c r="AB8" s="70"/>
       <c r="AC8" s="24">
         <f>(AC6+AC7)/2</f>
         <v>15</v>
@@ -9431,11 +9431,11 @@
         <f>AC8/AA8-1</f>
         <v>-0.16666666666666663</v>
       </c>
-      <c r="AE8" s="62">
+      <c r="AE8" s="69">
         <f>AE6</f>
         <v>14</v>
       </c>
-      <c r="AF8" s="63"/>
+      <c r="AF8" s="70"/>
       <c r="AG8" s="24">
         <f>(AG6+AG7)/2</f>
         <v>31</v>
@@ -9444,11 +9444,11 @@
         <f>AG8/AE8-1</f>
         <v>1.2142857142857144</v>
       </c>
-      <c r="AI8" s="62">
+      <c r="AI8" s="69">
         <f>AI6</f>
         <v>23</v>
       </c>
-      <c r="AJ8" s="63"/>
+      <c r="AJ8" s="70"/>
       <c r="AK8" s="24">
         <f>(AK6+AK7)/2</f>
         <v>24</v>
@@ -9457,11 +9457,11 @@
         <f>AK8/AI8-1</f>
         <v>4.3478260869565188E-2</v>
       </c>
-      <c r="AM8" s="62">
+      <c r="AM8" s="69">
         <f>AM6</f>
         <v>7</v>
       </c>
-      <c r="AN8" s="63"/>
+      <c r="AN8" s="70"/>
       <c r="AO8" s="24">
         <f>(AO6+AO7)/2</f>
         <v>7.5</v>
@@ -9470,11 +9470,11 @@
         <f>AO8/AM8-1</f>
         <v>7.1428571428571397E-2</v>
       </c>
-      <c r="AQ8" s="62">
+      <c r="AQ8" s="69">
         <f>AQ6</f>
         <v>14</v>
       </c>
-      <c r="AR8" s="63"/>
+      <c r="AR8" s="70"/>
       <c r="AS8" s="24">
         <f>(AS6+AS7)/2</f>
         <v>18.5</v>
@@ -9483,11 +9483,11 @@
         <f>AS8/AQ8-1</f>
         <v>0.3214285714285714</v>
       </c>
-      <c r="AU8" s="62">
+      <c r="AU8" s="69">
         <f>AU6</f>
         <v>12</v>
       </c>
-      <c r="AV8" s="63"/>
+      <c r="AV8" s="70"/>
       <c r="AW8" s="24">
         <f>(AW6+AW7)/2</f>
         <v>32.5</v>
@@ -9496,11 +9496,11 @@
         <f>AW8/AU8-1</f>
         <v>1.7083333333333335</v>
       </c>
-      <c r="AY8" s="62">
+      <c r="AY8" s="69">
         <f>AY6</f>
         <v>37</v>
       </c>
-      <c r="AZ8" s="63"/>
+      <c r="AZ8" s="70"/>
       <c r="BA8" s="24">
         <f>(BA6+BA7)/2</f>
         <v>31</v>
@@ -9509,11 +9509,11 @@
         <f>BA8/AY8-1</f>
         <v>-0.16216216216216217</v>
       </c>
-      <c r="BC8" s="62">
+      <c r="BC8" s="69">
         <f>BC6</f>
         <v>30</v>
       </c>
-      <c r="BD8" s="63"/>
+      <c r="BD8" s="70"/>
       <c r="BE8" s="24">
         <f>(BE6+BE7)/2</f>
         <v>42</v>
@@ -9522,11 +9522,11 @@
         <f>BE8/BC8-1</f>
         <v>0.39999999999999991</v>
       </c>
-      <c r="BG8" s="62">
+      <c r="BG8" s="69">
         <f>BG6</f>
         <v>23</v>
       </c>
-      <c r="BH8" s="63"/>
+      <c r="BH8" s="70"/>
       <c r="BI8" s="24">
         <f>(BI6+BI7)/2</f>
         <v>41.5</v>
@@ -9535,11 +9535,11 @@
         <f>BI8/BG8-1</f>
         <v>0.80434782608695654</v>
       </c>
-      <c r="BK8" s="62">
+      <c r="BK8" s="69">
         <f>BK6</f>
         <v>37</v>
       </c>
-      <c r="BL8" s="63"/>
+      <c r="BL8" s="70"/>
       <c r="BM8" s="24">
         <f>(BM6+BM7)/2</f>
         <v>31.5</v>
@@ -9548,11 +9548,11 @@
         <f>BM8/BK8-1</f>
         <v>-0.14864864864864868</v>
       </c>
-      <c r="BO8" s="62">
+      <c r="BO8" s="69">
         <f>BO6</f>
         <v>36</v>
       </c>
-      <c r="BP8" s="63"/>
+      <c r="BP8" s="70"/>
       <c r="BQ8" s="24">
         <f>(BQ6+BQ7)/2</f>
         <v>28</v>
@@ -12536,20 +12536,87 @@
     </row>
   </sheetData>
   <mergeCells count="119">
-    <mergeCell ref="BO7:BP7"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AW3:AX3"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AU7:AV7"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="BE3:BF3"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BC7:BD7"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="AY7:AZ7"/>
+    <mergeCell ref="BC8:BD8"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="AM8:AN8"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="AO3:AP3"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AM6:AN6"/>
+    <mergeCell ref="AM7:AN7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="BO8:BP8"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="BO2:BR2"/>
+    <mergeCell ref="BO3:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="AY2:BB2"/>
+    <mergeCell ref="AY3:AZ3"/>
+    <mergeCell ref="BA3:BB3"/>
+    <mergeCell ref="BK2:BN2"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="BM3:BN3"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BK7:BL7"/>
     <mergeCell ref="BK8:BL8"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="AQ3:AR3"/>
@@ -12574,87 +12641,20 @@
     <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="AQ6:AR6"/>
     <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="BO8:BP8"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="BO2:BR2"/>
-    <mergeCell ref="BO3:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BO5:BP5"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="AY2:BB2"/>
-    <mergeCell ref="AY3:AZ3"/>
-    <mergeCell ref="BA3:BB3"/>
-    <mergeCell ref="BK2:BN2"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="BM3:BN3"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BK7:BL7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="AM8:AN8"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AM3:AN3"/>
-    <mergeCell ref="AO3:AP3"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="AM7:AN7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="BC8:BD8"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="BO7:BP7"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AU7:AV7"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="BE3:BF3"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BC7:BD7"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="AY7:AZ7"/>
   </mergeCells>
   <conditionalFormatting sqref="BP21">
     <cfRule type="cellIs" dxfId="63" priority="103" operator="lessThan">
@@ -13104,10 +13104,10 @@
   <dimension ref="B1:AN194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="15" topLeftCell="C90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="15" topLeftCell="C180" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16089,7 +16089,7 @@
       </c>
     </row>
     <row r="33" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="60" t="s">
         <v>89</v>
       </c>
       <c r="C33" s="35">
@@ -19424,7 +19424,7 @@
       </c>
     </row>
     <row r="56" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="60" t="s">
         <v>141</v>
       </c>
       <c r="C56" s="35">
@@ -21164,7 +21164,7 @@
       </c>
     </row>
     <row r="68" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B68" s="35" t="s">
+      <c r="B68" s="60" t="s">
         <v>166</v>
       </c>
       <c r="C68" s="35">
@@ -23484,7 +23484,7 @@
       </c>
     </row>
     <row r="84" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B84" s="35" t="s">
+      <c r="B84" s="60" t="s">
         <v>207</v>
       </c>
       <c r="C84" s="35">
@@ -24209,7 +24209,7 @@
       </c>
     </row>
     <row r="89" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B89" s="35" t="s">
+      <c r="B89" s="60" t="s">
         <v>217</v>
       </c>
       <c r="C89" s="35">
@@ -31310,7 +31310,7 @@
       </c>
     </row>
     <row r="138" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B138" s="35" t="s">
+      <c r="B138" s="60" t="s">
         <v>329</v>
       </c>
       <c r="C138" s="35">
@@ -32470,7 +32470,7 @@
       </c>
     </row>
     <row r="146" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B146" s="35" t="s">
+      <c r="B146" s="60" t="s">
         <v>345</v>
       </c>
       <c r="C146" s="35">

</xml_diff>

<commit_message>
Factories - North America
</commit_message>
<xml_diff>
--- a/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
+++ b/Modding resources/economy spreadsheets/Data for Economic Rework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\economy spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B637E2F5-2E89-427A-89DA-730F812C25E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27776EF5-A430-444C-AF76-24E2A84FFC8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C93B8E2A-6318-41E2-B454-20DC41C43396}"/>
   </bookViews>
@@ -2386,11 +2386,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2407,20 +2416,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8449,246 +8449,246 @@
   <sheetData>
     <row r="1" spans="2:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:70" x14ac:dyDescent="0.25">
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="71" t="s">
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="71" t="s">
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="71" t="s">
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="71" t="s">
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="72"/>
-      <c r="U2" s="72"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="71" t="s">
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="71" t="s">
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="72"/>
-      <c r="AC2" s="72"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="71" t="s">
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="72"/>
-      <c r="AG2" s="72"/>
-      <c r="AH2" s="73"/>
-      <c r="AI2" s="71" t="s">
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="AJ2" s="72"/>
-      <c r="AK2" s="72"/>
-      <c r="AL2" s="73"/>
-      <c r="AM2" s="71" t="s">
+      <c r="AJ2" s="65"/>
+      <c r="AK2" s="65"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="AN2" s="72"/>
-      <c r="AO2" s="72"/>
-      <c r="AP2" s="73"/>
-      <c r="AQ2" s="71" t="s">
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="AR2" s="72"/>
-      <c r="AS2" s="72"/>
-      <c r="AT2" s="73"/>
-      <c r="AU2" s="71" t="s">
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="AV2" s="72"/>
-      <c r="AW2" s="72"/>
-      <c r="AX2" s="73"/>
-      <c r="AY2" s="71" t="s">
+      <c r="AV2" s="65"/>
+      <c r="AW2" s="65"/>
+      <c r="AX2" s="66"/>
+      <c r="AY2" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="AZ2" s="72"/>
-      <c r="BA2" s="72"/>
-      <c r="BB2" s="73"/>
-      <c r="BC2" s="71" t="s">
+      <c r="AZ2" s="65"/>
+      <c r="BA2" s="65"/>
+      <c r="BB2" s="66"/>
+      <c r="BC2" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="BD2" s="72"/>
-      <c r="BE2" s="72"/>
-      <c r="BF2" s="73"/>
-      <c r="BG2" s="71" t="s">
+      <c r="BD2" s="65"/>
+      <c r="BE2" s="65"/>
+      <c r="BF2" s="66"/>
+      <c r="BG2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="BH2" s="72"/>
-      <c r="BI2" s="72"/>
-      <c r="BJ2" s="73"/>
-      <c r="BK2" s="71" t="s">
+      <c r="BH2" s="65"/>
+      <c r="BI2" s="65"/>
+      <c r="BJ2" s="66"/>
+      <c r="BK2" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="BL2" s="72"/>
-      <c r="BM2" s="72"/>
-      <c r="BN2" s="73"/>
-      <c r="BO2" s="71" t="s">
+      <c r="BL2" s="65"/>
+      <c r="BM2" s="65"/>
+      <c r="BN2" s="66"/>
+      <c r="BO2" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="BP2" s="72"/>
-      <c r="BQ2" s="72"/>
-      <c r="BR2" s="73"/>
+      <c r="BP2" s="65"/>
+      <c r="BQ2" s="65"/>
+      <c r="BR2" s="66"/>
     </row>
     <row r="3" spans="2:70" x14ac:dyDescent="0.25">
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65" t="s">
+      <c r="D3" s="68"/>
+      <c r="E3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="64" t="s">
+      <c r="F3" s="69"/>
+      <c r="G3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65" t="s">
+      <c r="H3" s="68"/>
+      <c r="I3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="66"/>
-      <c r="K3" s="64" t="s">
+      <c r="J3" s="69"/>
+      <c r="K3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65" t="s">
+      <c r="L3" s="68"/>
+      <c r="M3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="66"/>
-      <c r="O3" s="64" t="s">
+      <c r="N3" s="69"/>
+      <c r="O3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65" t="s">
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="66"/>
-      <c r="S3" s="64" t="s">
+      <c r="R3" s="69"/>
+      <c r="S3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65" t="s">
+      <c r="T3" s="68"/>
+      <c r="U3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="66"/>
-      <c r="W3" s="64" t="s">
+      <c r="V3" s="69"/>
+      <c r="W3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="65"/>
-      <c r="Y3" s="65" t="s">
+      <c r="X3" s="68"/>
+      <c r="Y3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="66"/>
-      <c r="AA3" s="64" t="s">
+      <c r="Z3" s="69"/>
+      <c r="AA3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65" t="s">
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AD3" s="66"/>
-      <c r="AE3" s="64" t="s">
+      <c r="AD3" s="69"/>
+      <c r="AE3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65" t="s">
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AH3" s="66"/>
-      <c r="AI3" s="64" t="s">
+      <c r="AH3" s="69"/>
+      <c r="AI3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AJ3" s="65"/>
-      <c r="AK3" s="65" t="s">
+      <c r="AJ3" s="68"/>
+      <c r="AK3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AL3" s="66"/>
-      <c r="AM3" s="64" t="s">
+      <c r="AL3" s="69"/>
+      <c r="AM3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65" t="s">
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AP3" s="66"/>
-      <c r="AQ3" s="64" t="s">
+      <c r="AP3" s="69"/>
+      <c r="AQ3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65" t="s">
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AT3" s="66"/>
-      <c r="AU3" s="64" t="s">
+      <c r="AT3" s="69"/>
+      <c r="AU3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AV3" s="65"/>
-      <c r="AW3" s="65" t="s">
+      <c r="AV3" s="68"/>
+      <c r="AW3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AX3" s="66"/>
-      <c r="AY3" s="64" t="s">
+      <c r="AX3" s="69"/>
+      <c r="AY3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="AZ3" s="65"/>
-      <c r="BA3" s="65" t="s">
+      <c r="AZ3" s="68"/>
+      <c r="BA3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BB3" s="66"/>
-      <c r="BC3" s="64" t="s">
+      <c r="BB3" s="69"/>
+      <c r="BC3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BD3" s="65"/>
-      <c r="BE3" s="65" t="s">
+      <c r="BD3" s="68"/>
+      <c r="BE3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BF3" s="66"/>
-      <c r="BG3" s="64" t="s">
+      <c r="BF3" s="69"/>
+      <c r="BG3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BH3" s="65"/>
-      <c r="BI3" s="65" t="s">
+      <c r="BH3" s="68"/>
+      <c r="BI3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BJ3" s="66"/>
-      <c r="BK3" s="64" t="s">
+      <c r="BJ3" s="69"/>
+      <c r="BK3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BL3" s="65"/>
-      <c r="BM3" s="65" t="s">
+      <c r="BL3" s="68"/>
+      <c r="BM3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BN3" s="66"/>
-      <c r="BO3" s="64" t="s">
+      <c r="BN3" s="69"/>
+      <c r="BO3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="BP3" s="65"/>
-      <c r="BQ3" s="65" t="s">
+      <c r="BP3" s="68"/>
+      <c r="BQ3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BR3" s="66"/>
+      <c r="BR3" s="69"/>
     </row>
     <row r="4" spans="2:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
@@ -8900,10 +8900,10 @@
       <c r="B5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="67">
-        <v>1</v>
-      </c>
-      <c r="D5" s="68"/>
+      <c r="C5" s="70">
+        <v>1</v>
+      </c>
+      <c r="D5" s="71"/>
       <c r="E5" s="22">
         <v>2.9780000000000002</v>
       </c>
@@ -8911,10 +8911,10 @@
         <f>E5/C5-1</f>
         <v>1.9780000000000002</v>
       </c>
-      <c r="G5" s="67">
-        <v>1</v>
-      </c>
-      <c r="H5" s="68"/>
+      <c r="G5" s="70">
+        <v>1</v>
+      </c>
+      <c r="H5" s="71"/>
       <c r="I5" s="22">
         <v>1.84</v>
       </c>
@@ -8922,10 +8922,10 @@
         <f>I5/G5-1</f>
         <v>0.84000000000000008</v>
       </c>
-      <c r="K5" s="67">
-        <v>1</v>
-      </c>
-      <c r="L5" s="68"/>
+      <c r="K5" s="70">
+        <v>1</v>
+      </c>
+      <c r="L5" s="71"/>
       <c r="M5" s="22">
         <v>2.2770000000000001</v>
       </c>
@@ -8933,10 +8933,10 @@
         <f>M5/K5-1</f>
         <v>1.2770000000000001</v>
       </c>
-      <c r="O5" s="67">
-        <v>1</v>
-      </c>
-      <c r="P5" s="68"/>
+      <c r="O5" s="70">
+        <v>1</v>
+      </c>
+      <c r="P5" s="71"/>
       <c r="Q5" s="22">
         <v>2.8029999999999999</v>
       </c>
@@ -8947,7 +8947,7 @@
       <c r="S5" s="74">
         <v>2</v>
       </c>
-      <c r="T5" s="68"/>
+      <c r="T5" s="71"/>
       <c r="U5" s="22">
         <v>12.585000000000001</v>
       </c>
@@ -8955,10 +8955,10 @@
         <f>U5/S5-1</f>
         <v>5.2925000000000004</v>
       </c>
-      <c r="W5" s="67">
+      <c r="W5" s="70">
         <v>2</v>
       </c>
-      <c r="X5" s="68"/>
+      <c r="X5" s="71"/>
       <c r="Y5" s="22">
         <v>10.067</v>
       </c>
@@ -8966,10 +8966,10 @@
         <f>Y5/W5-1</f>
         <v>4.0335000000000001</v>
       </c>
-      <c r="AA5" s="67">
+      <c r="AA5" s="70">
         <v>2</v>
       </c>
-      <c r="AB5" s="68"/>
+      <c r="AB5" s="71"/>
       <c r="AC5" s="22">
         <v>9.9779999999999998</v>
       </c>
@@ -8977,10 +8977,10 @@
         <f>AC5/AA5-1</f>
         <v>3.9889999999999999</v>
       </c>
-      <c r="AE5" s="67">
+      <c r="AE5" s="70">
         <v>7</v>
       </c>
-      <c r="AF5" s="68"/>
+      <c r="AF5" s="71"/>
       <c r="AG5" s="22">
         <v>15.536</v>
       </c>
@@ -8988,10 +8988,10 @@
         <f>AG5/AE5-1</f>
         <v>1.2194285714285713</v>
       </c>
-      <c r="AI5" s="67">
+      <c r="AI5" s="70">
         <v>7</v>
       </c>
-      <c r="AJ5" s="68"/>
+      <c r="AJ5" s="71"/>
       <c r="AK5" s="22">
         <v>24.87</v>
       </c>
@@ -8999,10 +8999,10 @@
         <f>AK5/AI5-1</f>
         <v>2.5528571428571429</v>
       </c>
-      <c r="AM5" s="67">
+      <c r="AM5" s="70">
         <v>7</v>
       </c>
-      <c r="AN5" s="68"/>
+      <c r="AN5" s="71"/>
       <c r="AO5" s="22">
         <v>14.685</v>
       </c>
@@ -9010,10 +9010,10 @@
         <f>AO5/AM5-1</f>
         <v>1.0978571428571429</v>
       </c>
-      <c r="AQ5" s="67">
+      <c r="AQ5" s="70">
         <v>10</v>
       </c>
-      <c r="AR5" s="68"/>
+      <c r="AR5" s="71"/>
       <c r="AS5" s="22">
         <v>13.314</v>
       </c>
@@ -9021,10 +9021,10 @@
         <f>AS5/AQ5-1</f>
         <v>0.33139999999999992</v>
       </c>
-      <c r="AU5" s="67">
+      <c r="AU5" s="70">
         <v>15</v>
       </c>
-      <c r="AV5" s="68"/>
+      <c r="AV5" s="71"/>
       <c r="AW5" s="22">
         <v>35.488</v>
       </c>
@@ -9032,10 +9032,10 @@
         <f>AW5/AU5-1</f>
         <v>1.3658666666666668</v>
       </c>
-      <c r="AY5" s="67">
+      <c r="AY5" s="70">
         <v>20</v>
       </c>
-      <c r="AZ5" s="68"/>
+      <c r="AZ5" s="71"/>
       <c r="BA5" s="22">
         <v>46.418999999999997</v>
       </c>
@@ -9043,10 +9043,10 @@
         <f>BA5/AY5-1</f>
         <v>1.3209499999999998</v>
       </c>
-      <c r="BC5" s="67">
+      <c r="BC5" s="70">
         <v>20</v>
       </c>
-      <c r="BD5" s="68"/>
+      <c r="BD5" s="71"/>
       <c r="BE5" s="22">
         <v>77.132000000000005</v>
       </c>
@@ -9054,10 +9054,10 @@
         <f>BE5/BC5-1</f>
         <v>2.8566000000000003</v>
       </c>
-      <c r="BG5" s="67">
+      <c r="BG5" s="70">
         <v>20</v>
       </c>
-      <c r="BH5" s="68"/>
+      <c r="BH5" s="71"/>
       <c r="BI5" s="22">
         <v>50.906999999999996</v>
       </c>
@@ -9065,10 +9065,10 @@
         <f>BI5/BG5-1</f>
         <v>1.54535</v>
       </c>
-      <c r="BK5" s="67">
+      <c r="BK5" s="70">
         <v>30</v>
       </c>
-      <c r="BL5" s="68"/>
+      <c r="BL5" s="71"/>
       <c r="BM5" s="22">
         <v>39.054000000000002</v>
       </c>
@@ -9076,10 +9076,10 @@
         <f>BM5/BK5-1</f>
         <v>0.30180000000000007</v>
       </c>
-      <c r="BO5" s="67">
+      <c r="BO5" s="70">
         <v>30</v>
       </c>
-      <c r="BP5" s="68"/>
+      <c r="BP5" s="71"/>
       <c r="BQ5" s="22">
         <v>40.4</v>
       </c>
@@ -9092,34 +9092,34 @@
       <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="62">
+      <c r="C6" s="72">
         <v>11</v>
       </c>
-      <c r="D6" s="63"/>
+      <c r="D6" s="73"/>
       <c r="E6" s="23">
         <v>10</v>
       </c>
       <c r="F6" s="26"/>
-      <c r="G6" s="62">
+      <c r="G6" s="72">
         <v>17</v>
       </c>
-      <c r="H6" s="63"/>
+      <c r="H6" s="73"/>
       <c r="I6" s="23">
         <v>30</v>
       </c>
       <c r="J6" s="26"/>
-      <c r="K6" s="62">
+      <c r="K6" s="72">
         <v>10</v>
       </c>
-      <c r="L6" s="63"/>
+      <c r="L6" s="73"/>
       <c r="M6" s="23">
         <v>18</v>
       </c>
       <c r="N6" s="26"/>
-      <c r="O6" s="62">
+      <c r="O6" s="72">
         <v>18</v>
       </c>
-      <c r="P6" s="63"/>
+      <c r="P6" s="73"/>
       <c r="Q6" s="23">
         <v>22</v>
       </c>
@@ -9127,103 +9127,103 @@
       <c r="S6" s="75">
         <v>40</v>
       </c>
-      <c r="T6" s="63"/>
+      <c r="T6" s="73"/>
       <c r="U6" s="23">
         <v>37</v>
       </c>
       <c r="V6" s="26"/>
-      <c r="W6" s="62">
+      <c r="W6" s="72">
         <v>18</v>
       </c>
-      <c r="X6" s="63"/>
+      <c r="X6" s="73"/>
       <c r="Y6" s="23">
         <v>18</v>
       </c>
       <c r="Z6" s="26"/>
-      <c r="AA6" s="62">
+      <c r="AA6" s="72">
         <v>18</v>
       </c>
-      <c r="AB6" s="63"/>
+      <c r="AB6" s="73"/>
       <c r="AC6" s="23">
         <v>20</v>
       </c>
       <c r="AD6" s="26"/>
-      <c r="AE6" s="62">
+      <c r="AE6" s="72">
         <v>14</v>
       </c>
-      <c r="AF6" s="63"/>
+      <c r="AF6" s="73"/>
       <c r="AG6" s="23">
         <v>19</v>
       </c>
       <c r="AH6" s="26"/>
-      <c r="AI6" s="62">
+      <c r="AI6" s="72">
         <v>23</v>
       </c>
-      <c r="AJ6" s="63"/>
+      <c r="AJ6" s="73"/>
       <c r="AK6" s="23">
         <v>21</v>
       </c>
       <c r="AL6" s="26"/>
-      <c r="AM6" s="62">
+      <c r="AM6" s="72">
         <v>7</v>
       </c>
-      <c r="AN6" s="63"/>
+      <c r="AN6" s="73"/>
       <c r="AO6" s="23">
         <v>9</v>
       </c>
       <c r="AP6" s="26"/>
-      <c r="AQ6" s="62">
+      <c r="AQ6" s="72">
         <v>14</v>
       </c>
-      <c r="AR6" s="63"/>
+      <c r="AR6" s="73"/>
       <c r="AS6" s="23">
         <v>22</v>
       </c>
       <c r="AT6" s="26"/>
-      <c r="AU6" s="62">
+      <c r="AU6" s="72">
         <v>12</v>
       </c>
-      <c r="AV6" s="63"/>
+      <c r="AV6" s="73"/>
       <c r="AW6" s="23">
         <v>40</v>
       </c>
       <c r="AX6" s="26"/>
-      <c r="AY6" s="62">
+      <c r="AY6" s="72">
         <v>37</v>
       </c>
-      <c r="AZ6" s="63"/>
+      <c r="AZ6" s="73"/>
       <c r="BA6" s="23">
         <v>44</v>
       </c>
       <c r="BB6" s="26"/>
-      <c r="BC6" s="62">
+      <c r="BC6" s="72">
         <v>30</v>
       </c>
-      <c r="BD6" s="63"/>
+      <c r="BD6" s="73"/>
       <c r="BE6" s="23">
         <v>58</v>
       </c>
       <c r="BF6" s="26"/>
-      <c r="BG6" s="62">
+      <c r="BG6" s="72">
         <v>23</v>
       </c>
-      <c r="BH6" s="63"/>
+      <c r="BH6" s="73"/>
       <c r="BI6" s="23">
         <v>47</v>
       </c>
       <c r="BJ6" s="26"/>
-      <c r="BK6" s="62">
+      <c r="BK6" s="72">
         <v>37</v>
       </c>
-      <c r="BL6" s="63"/>
+      <c r="BL6" s="73"/>
       <c r="BM6" s="23">
         <v>40</v>
       </c>
       <c r="BN6" s="26"/>
-      <c r="BO6" s="62">
+      <c r="BO6" s="72">
         <v>36</v>
       </c>
-      <c r="BP6" s="63"/>
+      <c r="BP6" s="73"/>
       <c r="BQ6" s="23">
         <v>23</v>
       </c>
@@ -9233,104 +9233,104 @@
       <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="23">
         <v>18</v>
       </c>
       <c r="F7" s="26"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="63"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="73"/>
       <c r="I7" s="23">
         <v>30</v>
       </c>
       <c r="J7" s="26"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="63"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="73"/>
       <c r="M7" s="23">
         <v>32</v>
       </c>
       <c r="N7" s="26"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="63"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="73"/>
       <c r="Q7" s="23">
         <v>18</v>
       </c>
       <c r="R7" s="26"/>
       <c r="S7" s="75"/>
-      <c r="T7" s="63"/>
+      <c r="T7" s="73"/>
       <c r="U7" s="23">
         <v>22</v>
       </c>
       <c r="V7" s="26"/>
-      <c r="W7" s="62"/>
-      <c r="X7" s="63"/>
+      <c r="W7" s="72"/>
+      <c r="X7" s="73"/>
       <c r="Y7" s="23">
         <v>22</v>
       </c>
       <c r="Z7" s="26"/>
-      <c r="AA7" s="62"/>
-      <c r="AB7" s="63"/>
+      <c r="AA7" s="72"/>
+      <c r="AB7" s="73"/>
       <c r="AC7" s="23">
         <v>10</v>
       </c>
       <c r="AD7" s="26"/>
-      <c r="AE7" s="62"/>
-      <c r="AF7" s="63"/>
+      <c r="AE7" s="72"/>
+      <c r="AF7" s="73"/>
       <c r="AG7" s="23">
         <v>43</v>
       </c>
       <c r="AH7" s="26"/>
-      <c r="AI7" s="62"/>
-      <c r="AJ7" s="63"/>
+      <c r="AI7" s="72"/>
+      <c r="AJ7" s="73"/>
       <c r="AK7" s="23">
         <v>27</v>
       </c>
       <c r="AL7" s="26"/>
-      <c r="AM7" s="62"/>
-      <c r="AN7" s="63"/>
+      <c r="AM7" s="72"/>
+      <c r="AN7" s="73"/>
       <c r="AO7" s="23">
         <v>6</v>
       </c>
       <c r="AP7" s="26"/>
-      <c r="AQ7" s="62"/>
-      <c r="AR7" s="63"/>
+      <c r="AQ7" s="72"/>
+      <c r="AR7" s="73"/>
       <c r="AS7" s="23">
         <v>15</v>
       </c>
       <c r="AT7" s="26"/>
-      <c r="AU7" s="62"/>
-      <c r="AV7" s="63"/>
+      <c r="AU7" s="72"/>
+      <c r="AV7" s="73"/>
       <c r="AW7" s="23">
         <v>25</v>
       </c>
       <c r="AX7" s="26"/>
-      <c r="AY7" s="62"/>
-      <c r="AZ7" s="63"/>
+      <c r="AY7" s="72"/>
+      <c r="AZ7" s="73"/>
       <c r="BA7" s="23">
         <v>18</v>
       </c>
       <c r="BB7" s="26"/>
-      <c r="BC7" s="62"/>
-      <c r="BD7" s="63"/>
+      <c r="BC7" s="72"/>
+      <c r="BD7" s="73"/>
       <c r="BE7" s="23">
         <v>26</v>
       </c>
       <c r="BF7" s="26"/>
-      <c r="BG7" s="62"/>
-      <c r="BH7" s="63"/>
+      <c r="BG7" s="72"/>
+      <c r="BH7" s="73"/>
       <c r="BI7" s="23">
         <v>36</v>
       </c>
       <c r="BJ7" s="26"/>
-      <c r="BK7" s="62"/>
-      <c r="BL7" s="63"/>
+      <c r="BK7" s="72"/>
+      <c r="BL7" s="73"/>
       <c r="BM7" s="23">
         <v>23</v>
       </c>
       <c r="BN7" s="26"/>
-      <c r="BO7" s="62"/>
-      <c r="BP7" s="63"/>
+      <c r="BO7" s="72"/>
+      <c r="BP7" s="73"/>
       <c r="BQ7" s="23">
         <v>33</v>
       </c>
@@ -9340,11 +9340,11 @@
       <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="69">
+      <c r="C8" s="62">
         <f>C6</f>
         <v>11</v>
       </c>
-      <c r="D8" s="70"/>
+      <c r="D8" s="63"/>
       <c r="E8" s="24">
         <f>(E6+E7)/2</f>
         <v>14</v>
@@ -9353,11 +9353,11 @@
         <f>E8/C8-1</f>
         <v>0.27272727272727271</v>
       </c>
-      <c r="G8" s="69">
+      <c r="G8" s="62">
         <f>G6</f>
         <v>17</v>
       </c>
-      <c r="H8" s="70"/>
+      <c r="H8" s="63"/>
       <c r="I8" s="24">
         <f>(I6+I7)/2</f>
         <v>30</v>
@@ -9366,11 +9366,11 @@
         <f>I8/G8-1</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="K8" s="69">
+      <c r="K8" s="62">
         <f>K6</f>
         <v>10</v>
       </c>
-      <c r="L8" s="70"/>
+      <c r="L8" s="63"/>
       <c r="M8" s="24">
         <f>(M6+M7)/2</f>
         <v>25</v>
@@ -9379,11 +9379,11 @@
         <f>M8/K8-1</f>
         <v>1.5</v>
       </c>
-      <c r="O8" s="69">
+      <c r="O8" s="62">
         <f>O6</f>
         <v>18</v>
       </c>
-      <c r="P8" s="70"/>
+      <c r="P8" s="63"/>
       <c r="Q8" s="24">
         <f>(Q6+Q7)/2</f>
         <v>20</v>
@@ -9396,7 +9396,7 @@
         <f>S6</f>
         <v>40</v>
       </c>
-      <c r="T8" s="70"/>
+      <c r="T8" s="63"/>
       <c r="U8" s="24">
         <f>(U6+U7)/2</f>
         <v>29.5</v>
@@ -9405,11 +9405,11 @@
         <f>U8/S8-1</f>
         <v>-0.26249999999999996</v>
       </c>
-      <c r="W8" s="69">
+      <c r="W8" s="62">
         <f>W6</f>
         <v>18</v>
       </c>
-      <c r="X8" s="70"/>
+      <c r="X8" s="63"/>
       <c r="Y8" s="24">
         <f>(Y6+Y7)/2</f>
         <v>20</v>
@@ -9418,11 +9418,11 @@
         <f>Y8/W8-1</f>
         <v>0.11111111111111116</v>
       </c>
-      <c r="AA8" s="69">
+      <c r="AA8" s="62">
         <f>AA6</f>
         <v>18</v>
       </c>
-      <c r="AB8" s="70"/>
+      <c r="AB8" s="63"/>
       <c r="AC8" s="24">
         <f>(AC6+AC7)/2</f>
         <v>15</v>
@@ -9431,11 +9431,11 @@
         <f>AC8/AA8-1</f>
         <v>-0.16666666666666663</v>
       </c>
-      <c r="AE8" s="69">
+      <c r="AE8" s="62">
         <f>AE6</f>
         <v>14</v>
       </c>
-      <c r="AF8" s="70"/>
+      <c r="AF8" s="63"/>
       <c r="AG8" s="24">
         <f>(AG6+AG7)/2</f>
         <v>31</v>
@@ -9444,11 +9444,11 @@
         <f>AG8/AE8-1</f>
         <v>1.2142857142857144</v>
       </c>
-      <c r="AI8" s="69">
+      <c r="AI8" s="62">
         <f>AI6</f>
         <v>23</v>
       </c>
-      <c r="AJ8" s="70"/>
+      <c r="AJ8" s="63"/>
       <c r="AK8" s="24">
         <f>(AK6+AK7)/2</f>
         <v>24</v>
@@ -9457,11 +9457,11 @@
         <f>AK8/AI8-1</f>
         <v>4.3478260869565188E-2</v>
       </c>
-      <c r="AM8" s="69">
+      <c r="AM8" s="62">
         <f>AM6</f>
         <v>7</v>
       </c>
-      <c r="AN8" s="70"/>
+      <c r="AN8" s="63"/>
       <c r="AO8" s="24">
         <f>(AO6+AO7)/2</f>
         <v>7.5</v>
@@ -9470,11 +9470,11 @@
         <f>AO8/AM8-1</f>
         <v>7.1428571428571397E-2</v>
       </c>
-      <c r="AQ8" s="69">
+      <c r="AQ8" s="62">
         <f>AQ6</f>
         <v>14</v>
       </c>
-      <c r="AR8" s="70"/>
+      <c r="AR8" s="63"/>
       <c r="AS8" s="24">
         <f>(AS6+AS7)/2</f>
         <v>18.5</v>
@@ -9483,11 +9483,11 @@
         <f>AS8/AQ8-1</f>
         <v>0.3214285714285714</v>
       </c>
-      <c r="AU8" s="69">
+      <c r="AU8" s="62">
         <f>AU6</f>
         <v>12</v>
       </c>
-      <c r="AV8" s="70"/>
+      <c r="AV8" s="63"/>
       <c r="AW8" s="24">
         <f>(AW6+AW7)/2</f>
         <v>32.5</v>
@@ -9496,11 +9496,11 @@
         <f>AW8/AU8-1</f>
         <v>1.7083333333333335</v>
       </c>
-      <c r="AY8" s="69">
+      <c r="AY8" s="62">
         <f>AY6</f>
         <v>37</v>
       </c>
-      <c r="AZ8" s="70"/>
+      <c r="AZ8" s="63"/>
       <c r="BA8" s="24">
         <f>(BA6+BA7)/2</f>
         <v>31</v>
@@ -9509,11 +9509,11 @@
         <f>BA8/AY8-1</f>
         <v>-0.16216216216216217</v>
       </c>
-      <c r="BC8" s="69">
+      <c r="BC8" s="62">
         <f>BC6</f>
         <v>30</v>
       </c>
-      <c r="BD8" s="70"/>
+      <c r="BD8" s="63"/>
       <c r="BE8" s="24">
         <f>(BE6+BE7)/2</f>
         <v>42</v>
@@ -9522,11 +9522,11 @@
         <f>BE8/BC8-1</f>
         <v>0.39999999999999991</v>
       </c>
-      <c r="BG8" s="69">
+      <c r="BG8" s="62">
         <f>BG6</f>
         <v>23</v>
       </c>
-      <c r="BH8" s="70"/>
+      <c r="BH8" s="63"/>
       <c r="BI8" s="24">
         <f>(BI6+BI7)/2</f>
         <v>41.5</v>
@@ -9535,11 +9535,11 @@
         <f>BI8/BG8-1</f>
         <v>0.80434782608695654</v>
       </c>
-      <c r="BK8" s="69">
+      <c r="BK8" s="62">
         <f>BK6</f>
         <v>37</v>
       </c>
-      <c r="BL8" s="70"/>
+      <c r="BL8" s="63"/>
       <c r="BM8" s="24">
         <f>(BM6+BM7)/2</f>
         <v>31.5</v>
@@ -9548,11 +9548,11 @@
         <f>BM8/BK8-1</f>
         <v>-0.14864864864864868</v>
       </c>
-      <c r="BO8" s="69">
+      <c r="BO8" s="62">
         <f>BO6</f>
         <v>36</v>
       </c>
-      <c r="BP8" s="70"/>
+      <c r="BP8" s="63"/>
       <c r="BQ8" s="24">
         <f>(BQ6+BQ7)/2</f>
         <v>28</v>
@@ -12536,15 +12536,92 @@
     </row>
   </sheetData>
   <mergeCells count="119">
-    <mergeCell ref="BC8:BD8"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="BO7:BP7"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AU7:AV7"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="BE3:BF3"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BC7:BD7"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="AY7:AZ7"/>
+    <mergeCell ref="BK8:BL8"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AQ3:AR3"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AI7:AJ7"/>
+    <mergeCell ref="AU2:AX2"/>
+    <mergeCell ref="AY8:AZ8"/>
+    <mergeCell ref="BG8:BH8"/>
+    <mergeCell ref="BG2:BJ2"/>
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="BI3:BJ3"/>
+    <mergeCell ref="BG5:BH5"/>
+    <mergeCell ref="BG6:BH6"/>
+    <mergeCell ref="BG7:BH7"/>
+    <mergeCell ref="AU8:AV8"/>
+    <mergeCell ref="AI8:AJ8"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="BO8:BP8"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="BO2:BR2"/>
+    <mergeCell ref="BO3:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="AY2:BB2"/>
+    <mergeCell ref="AY3:AZ3"/>
+    <mergeCell ref="BA3:BB3"/>
+    <mergeCell ref="BK2:BN2"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="BM3:BN3"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BK7:BL7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="G5:H5"/>
@@ -12569,92 +12646,15 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="W8:X8"/>
     <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="BO8:BP8"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="BO2:BR2"/>
-    <mergeCell ref="BO3:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BO5:BP5"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="AY2:BB2"/>
-    <mergeCell ref="AY3:AZ3"/>
-    <mergeCell ref="BA3:BB3"/>
-    <mergeCell ref="BK2:BN2"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="BM3:BN3"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BK7:BL7"/>
-    <mergeCell ref="BK8:BL8"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AQ3:AR3"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AI7:AJ7"/>
-    <mergeCell ref="AU2:AX2"/>
-    <mergeCell ref="AY8:AZ8"/>
-    <mergeCell ref="BG8:BH8"/>
-    <mergeCell ref="BG2:BJ2"/>
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="BI3:BJ3"/>
-    <mergeCell ref="BG5:BH5"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="BG7:BH7"/>
-    <mergeCell ref="AU8:AV8"/>
-    <mergeCell ref="AI8:AJ8"/>
-    <mergeCell ref="AS3:AT3"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="BO7:BP7"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AW3:AX3"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AU7:AV7"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="BE3:BF3"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BC7:BD7"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="AY7:AZ7"/>
+    <mergeCell ref="BC8:BD8"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="BC2:BF2"/>
   </mergeCells>
   <conditionalFormatting sqref="BP21">
     <cfRule type="cellIs" dxfId="63" priority="103" operator="lessThan">
@@ -13104,10 +13104,10 @@
   <dimension ref="B1:AN194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="15" topLeftCell="C180" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="15" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="B146" sqref="B146"/>
+      <selection pane="bottomRight" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13375,7 +13375,7 @@
     </row>
     <row r="12" spans="2:40" s="39" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="60" t="s">
         <v>450</v>
       </c>
       <c r="C13" s="35">
@@ -13503,6 +13503,22 @@
       <c r="AJ13" s="39">
         <f>AG13+AH13+AI13</f>
         <v>450</v>
+      </c>
+      <c r="AK13" s="49">
+        <f>AG13-O13</f>
+        <v>82</v>
+      </c>
+      <c r="AL13" s="50">
+        <f>AH13-P13</f>
+        <v>-6</v>
+      </c>
+      <c r="AM13" s="50">
+        <f>AI13-Q13</f>
+        <v>74</v>
+      </c>
+      <c r="AN13" s="51">
+        <f>AJ13-R13</f>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="2:40" s="35" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14349,7 +14365,7 @@
       </c>
     </row>
     <row r="21" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="60" t="s">
         <v>64</v>
       </c>
       <c r="C21" s="35">
@@ -14784,7 +14800,7 @@
       </c>
     </row>
     <row r="24" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="60" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="35">
@@ -16379,7 +16395,7 @@
       </c>
     </row>
     <row r="35" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="60" t="s">
         <v>95</v>
       </c>
       <c r="C35" s="35">
@@ -18119,7 +18135,7 @@
       </c>
     </row>
     <row r="47" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="60" t="s">
         <v>120</v>
       </c>
       <c r="C47" s="35">
@@ -22034,7 +22050,7 @@
       </c>
     </row>
     <row r="74" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B74" s="35" t="s">
+      <c r="B74" s="60" t="s">
         <v>180</v>
       </c>
       <c r="C74" s="35">
@@ -24644,7 +24660,7 @@
       </c>
     </row>
     <row r="92" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B92" s="35" t="s">
+      <c r="B92" s="60" t="s">
         <v>28</v>
       </c>
       <c r="C92" s="35">
@@ -26384,7 +26400,7 @@
       </c>
     </row>
     <row r="104" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B104" s="35" t="s">
+      <c r="B104" s="60" t="s">
         <v>249</v>
       </c>
       <c r="C104" s="35">
@@ -29135,7 +29151,7 @@
       </c>
     </row>
     <row r="123" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B123" s="35" t="s">
+      <c r="B123" s="60" t="s">
         <v>293</v>
       </c>
       <c r="C123" s="35">
@@ -29570,7 +29586,7 @@
       </c>
     </row>
     <row r="126" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B126" s="35" t="s">
+      <c r="B126" s="60" t="s">
         <v>299</v>
       </c>
       <c r="C126" s="35">
@@ -29715,7 +29731,7 @@
       </c>
     </row>
     <row r="127" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B127" s="35" t="s">
+      <c r="B127" s="60" t="s">
         <v>301</v>
       </c>
       <c r="C127" s="35">
@@ -30875,7 +30891,7 @@
       </c>
     </row>
     <row r="135" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B135" s="35" t="s">
+      <c r="B135" s="60" t="s">
         <v>321</v>
       </c>
       <c r="C135" s="35">
@@ -31165,7 +31181,7 @@
       </c>
     </row>
     <row r="137" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B137" s="35" t="s">
+      <c r="B137" s="60" t="s">
         <v>327</v>
       </c>
       <c r="C137" s="35">
@@ -32180,7 +32196,7 @@
       </c>
     </row>
     <row r="144" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B144" s="35" t="s">
+      <c r="B144" s="60" t="s">
         <v>341</v>
       </c>
       <c r="C144" s="35">
@@ -32325,7 +32341,7 @@
       </c>
     </row>
     <row r="145" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B145" s="35" t="s">
+      <c r="B145" s="60" t="s">
         <v>343</v>
       </c>
       <c r="C145" s="35">
@@ -32615,7 +32631,7 @@
       </c>
     </row>
     <row r="147" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B147" s="35" t="s">
+      <c r="B147" s="60" t="s">
         <v>347</v>
       </c>
       <c r="C147" s="35">
@@ -35660,7 +35676,7 @@
       </c>
     </row>
     <row r="168" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B168" s="35" t="s">
+      <c r="B168" s="60" t="s">
         <v>401</v>
       </c>
       <c r="C168" s="35">

</xml_diff>